<commit_message>
Initial schema of database + update of plan
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOTNET_React_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Schedule_state">Лист1!$U$5:$U$8</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t>11.09.18</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>Create .Net Rest Api application with GET method</t>
-  </si>
-  <si>
     <t>TA6</t>
   </si>
   <si>
@@ -228,15 +225,6 @@
     <t>E2E Regression</t>
   </si>
   <si>
-    <t>Add POST method (controllers+services+DAL)</t>
-  </si>
-  <si>
-    <t>Add PUT method (controllers+services+DAL)</t>
-  </si>
-  <si>
-    <t>Add DELETE method (controllers+services+DAL)</t>
-  </si>
-  <si>
     <t>Unit tests</t>
   </si>
   <si>
@@ -256,12 +244,30 @@
   </si>
   <si>
     <t>Frontend React/Redux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add POST method (controllers+services+server side validation+DAL) </t>
+  </si>
+  <si>
+    <t>Add PUT method (controllers+server side validation+services+DAL)</t>
+  </si>
+  <si>
+    <t>Add DELETE method (controllers+server side validation+services+DAL)</t>
+  </si>
+  <si>
+    <t>TA20</t>
+  </si>
+  <si>
+    <t>Investigate OData</t>
+  </si>
+  <si>
+    <t>Create .Net Rest Api application with GET method (controllers+services+DAL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -770,7 +776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -874,6 +880,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,8 +984,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -992,9 +1001,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1032,7 +1041,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1104,7 +1113,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1254,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,27 +1282,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="57" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="58"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1311,14 +1320,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
+      <c r="B3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1329,12 +1338,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="59" t="s">
+      <c r="A4" s="47"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1355,8 +1364,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>24</v>
@@ -1382,8 +1391,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -1409,8 +1418,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>28</v>
@@ -1436,14 +1445,14 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>36</v>
@@ -1463,8 +1472,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>38</v>
@@ -1487,19 +1496,19 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
         <f>SUM(G11,G15,G18)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -1507,12 +1516,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="59" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="60"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1525,19 +1534,19 @@
       </c>
       <c r="H11" s="23">
         <f>SUM(H12:H16)</f>
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="I11" s="23">
         <f>SUM(I12:I16)</f>
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>39</v>
@@ -1557,11 +1566,11 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>25</v>
@@ -1581,11 +1590,11 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
@@ -1605,14 +1614,14 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="62"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="63"/>
       <c r="E15" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>35</v>
@@ -1623,22 +1632,22 @@
       </c>
       <c r="H15" s="11">
         <f>SUM(H16:H17)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I15" s="11">
         <f>SUM(I16:I17)</f>
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>35</v>
@@ -1647,187 +1656,187 @@
         <v>8</v>
       </c>
       <c r="H16" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I16" s="2">
         <f>G16-H16</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2">
         <v>8</v>
       </c>
       <c r="H17" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I17" s="2">
         <f>G17-H17</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="42"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="43"/>
       <c r="E18" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="12">
-        <f>SUM(G19:G20)</f>
-        <v>8</v>
-      </c>
-      <c r="H18" s="12">
-        <f>SUM(H19:H20)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="12">
-        <f>SUM(I19:I20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="49"/>
+        <f>SUM(G19:G21)</f>
+        <v>10</v>
+      </c>
+      <c r="H18" s="35">
+        <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G19" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="2">
         <f>G19-H19</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="8">
-        <v>4</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="8">
+      <c r="G20" s="2">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <f>G20-H20</f>
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="48" t="s">
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="8">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30">
-        <f>SUM(G22)</f>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30">
+        <f>SUM(G23)</f>
         <v>40</v>
       </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="H22" s="29"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="12">
-        <f>SUM(G23:G29)</f>
+      <c r="G23" s="12">
+        <f>SUM(G24:G30)</f>
         <v>40</v>
       </c>
-      <c r="H22" s="12">
-        <f t="shared" ref="H22:I22" si="1">SUM(H23:H29)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
-        <f t="shared" si="1"/>
+      <c r="H23" s="12">
+        <f t="shared" ref="H23:I23" si="2">SUM(H24:H30)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="2">
-        <v>4</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <f>G23-H23</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="49"/>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>34</v>
@@ -1839,19 +1848,19 @@
         <v>0</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" ref="I24:I29" si="2">G24-H24</f>
+        <f>G24-H24</f>
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>34</v>
@@ -1863,19 +1872,19 @@
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="49"/>
+        <f t="shared" ref="I25:I30" si="3">G25-H25</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>34</v>
@@ -1887,208 +1896,232 @@
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="8">
-        <v>12</v>
+      <c r="G27" s="2">
+        <v>4</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" ref="I27:I28" si="3">G27-H27</f>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I28:I29" si="4">G28-H28</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="50"/>
       <c r="C29" s="7"/>
       <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="8">
+        <v>8</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="48"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="8">
+        <v>4</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="30">
+        <f>120</f>
+        <v>120</v>
+      </c>
+      <c r="H31" s="33"/>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="F32" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="36">
+        <f>SUM(G33:G33)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="36">
+        <f>SUM(H33:H33)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="36">
+        <f>SUM(I33:I33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="38"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="30">
+        <f>80</f>
+        <v>80</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" s="31"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="45"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F35" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="8">
-        <v>4</v>
-      </c>
-      <c r="H29" s="8">
-        <v>0</v>
-      </c>
-      <c r="I29" s="8">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="30">
-        <f>SUM(G31)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="31"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="35">
-        <f>SUM(G32:G32)</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="35">
-        <f>SUM(H32:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="35">
-        <f>SUM(I32:I32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="30">
-        <f>SUM(G34)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="40"/>
-      <c r="E34" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="35">
-        <v>0</v>
-      </c>
-      <c r="H34" s="35">
-        <f>SUM(H35:H38)</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="35">
-        <f>SUM(I35:I38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="G35" s="36">
+        <v>0</v>
+      </c>
+      <c r="H35" s="36">
+        <f>SUM(H36:H39)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="36">
+        <f>SUM(I36:I39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B36" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2098,30 +2131,30 @@
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A10:A20"/>
-    <mergeCell ref="B10:B20"/>
+    <mergeCell ref="A10:A21"/>
+    <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:E33"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F31 F33:F34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:F35 F4:F32">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "Initial schema of database + update of plan"
This reverts commit 71ae8b3d28ba3ae89dc973e94b637345d0b89b8e.
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOTNET_React_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Schedule_state">Лист1!$U$5:$U$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>11.09.18</t>
   </si>
@@ -150,6 +150,9 @@
     <t>Planning</t>
   </si>
   <si>
+    <t>Create .Net Rest Api application with GET method</t>
+  </si>
+  <si>
     <t>TA6</t>
   </si>
   <si>
@@ -225,6 +228,15 @@
     <t>E2E Regression</t>
   </si>
   <si>
+    <t>Add POST method (controllers+services+DAL)</t>
+  </si>
+  <si>
+    <t>Add PUT method (controllers+services+DAL)</t>
+  </si>
+  <si>
+    <t>Add DELETE method (controllers+services+DAL)</t>
+  </si>
+  <si>
     <t>Unit tests</t>
   </si>
   <si>
@@ -244,30 +256,12 @@
   </si>
   <si>
     <t>Frontend React/Redux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add POST method (controllers+services+server side validation+DAL) </t>
-  </si>
-  <si>
-    <t>Add PUT method (controllers+server side validation+services+DAL)</t>
-  </si>
-  <si>
-    <t>Add DELETE method (controllers+server side validation+services+DAL)</t>
-  </si>
-  <si>
-    <t>TA20</t>
-  </si>
-  <si>
-    <t>Investigate OData</t>
-  </si>
-  <si>
-    <t>Create .Net Rest Api application with GET method (controllers+services+DAL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -776,7 +770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -880,9 +874,6 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -984,8 +975,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1001,9 +992,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1041,7 +1032,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1113,7 +1104,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1263,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,27 +1273,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="58" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1320,14 +1311,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
+      <c r="B3" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1338,12 +1329,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="60" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1364,8 +1355,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>24</v>
@@ -1391,8 +1382,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -1418,8 +1409,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>28</v>
@@ -1445,14 +1436,14 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>36</v>
@@ -1472,8 +1463,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>38</v>
@@ -1496,19 +1487,19 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
         <f>SUM(G11,G15,G18)</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -1516,12 +1507,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="60" t="s">
+      <c r="A11" s="46"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="61"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1534,19 +1525,19 @@
       </c>
       <c r="H11" s="23">
         <f>SUM(H12:H16)</f>
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I11" s="23">
         <f>SUM(I12:I16)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>39</v>
@@ -1566,11 +1557,11 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>25</v>
@@ -1590,11 +1581,11 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
@@ -1614,14 +1605,14 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="63"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="62"/>
       <c r="E15" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>35</v>
@@ -1632,22 +1623,22 @@
       </c>
       <c r="H15" s="11">
         <f>SUM(H16:H17)</f>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I15" s="11">
         <f>SUM(I16:I17)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>35</v>
@@ -1656,187 +1647,187 @@
         <v>8</v>
       </c>
       <c r="H16" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I16" s="2">
         <f>G16-H16</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="2">
         <v>8</v>
       </c>
       <c r="H17" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2">
         <f>G17-H17</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="43"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="42"/>
       <c r="E18" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="12">
-        <f>SUM(G19:G21)</f>
-        <v>10</v>
-      </c>
-      <c r="H18" s="35">
-        <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="35">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="50"/>
+        <f>SUM(G19:G20)</f>
+        <v>8</v>
+      </c>
+      <c r="H18" s="12">
+        <f>SUM(H19:H20)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <f>SUM(I19:I20)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="46"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G19" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="2">
         <f>G19-H19</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="46"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="2">
-        <v>4</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <f>G20-H20</f>
+      <c r="G20" s="8">
+        <v>4</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="27" t="s">
+      <c r="A21" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30">
+        <f>SUM(G22)</f>
+        <v>40</v>
+      </c>
+      <c r="H21" s="29"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="46"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="8">
-        <v>4</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0</v>
-      </c>
-      <c r="I21" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30">
-        <f>SUM(G23)</f>
+      <c r="G22" s="12">
+        <f>SUM(G23:G29)</f>
         <v>40</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="31"/>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="12" t="s">
+      <c r="H22" s="12">
+        <f t="shared" ref="H22:I22" si="1">SUM(H23:H29)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="46"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="12">
-        <f>SUM(G24:G30)</f>
-        <v>40</v>
-      </c>
-      <c r="H23" s="12">
-        <f t="shared" ref="H23:I23" si="2">SUM(H24:H30)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="12">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="G23" s="2">
+        <v>4</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <f>G23-H23</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="46"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>34</v>
@@ -1848,19 +1839,19 @@
         <v>0</v>
       </c>
       <c r="I24" s="2">
-        <f>G24-H24</f>
+        <f t="shared" ref="I24:I29" si="2">G24-H24</f>
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>34</v>
@@ -1872,19 +1863,19 @@
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" ref="I25:I30" si="3">G25-H25</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="46"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>34</v>
@@ -1896,232 +1887,208 @@
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="2">
-        <v>4</v>
+      <c r="G27" s="8">
+        <v>12</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" ref="I27:I28" si="3">G27-H27</f>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="50"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" ref="I28:I29" si="4">G28-H28</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="47"/>
       <c r="B29" s="50"/>
       <c r="C29" s="7"/>
       <c r="D29" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G29" s="8">
+        <v>4</v>
+      </c>
+      <c r="H29" s="8">
+        <v>0</v>
+      </c>
+      <c r="I29" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="37"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="30">
+        <f>SUM(G31)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="33"/>
+      <c r="I30" s="31"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="2" t="s">
+      <c r="B31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="40"/>
+      <c r="E31" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="8" t="s">
+      <c r="F31" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="8">
-        <v>4</v>
-      </c>
-      <c r="H30" s="8">
-        <v>0</v>
-      </c>
-      <c r="I30" s="8">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="30">
-        <f>120</f>
-        <v>120</v>
-      </c>
-      <c r="H31" s="33"/>
-      <c r="I31" s="31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="35">
+        <f>SUM(G32:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="35">
+        <f>SUM(H32:H32)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="35">
+        <f>SUM(I32:I32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="37"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="30">
+        <f>SUM(G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="33"/>
+      <c r="I33" s="31"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="36">
-        <f>SUM(G33:G33)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="36">
-        <f>SUM(H33:H33)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="36">
-        <f>SUM(I33:I33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="30">
-        <f>80</f>
-        <v>80</v>
-      </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="31"/>
+      <c r="G34" s="35">
+        <v>0</v>
+      </c>
+      <c r="H34" s="35">
+        <f>SUM(H35:H38)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="35">
+        <f>SUM(I35:I38)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="F35" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="36">
-        <v>0</v>
-      </c>
-      <c r="H35" s="36">
-        <f>SUM(H36:H39)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="36">
-        <f>SUM(I36:I39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="A35" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B35" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="B21:B29"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2131,30 +2098,30 @@
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A10:A21"/>
-    <mergeCell ref="B10:B21"/>
+    <mergeCell ref="A10:A20"/>
+    <mergeCell ref="B10:B20"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:F35 F4:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F31 F33:F34">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "Revert "Initial schema of database + update of plan""
This reverts commit 20f262d04a637b44420a4637dc261b5108a229ff.
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOTNET_React_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Schedule_state">Лист1!$U$5:$U$8</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t>11.09.18</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>Create .Net Rest Api application with GET method</t>
-  </si>
-  <si>
     <t>TA6</t>
   </si>
   <si>
@@ -228,15 +225,6 @@
     <t>E2E Regression</t>
   </si>
   <si>
-    <t>Add POST method (controllers+services+DAL)</t>
-  </si>
-  <si>
-    <t>Add PUT method (controllers+services+DAL)</t>
-  </si>
-  <si>
-    <t>Add DELETE method (controllers+services+DAL)</t>
-  </si>
-  <si>
     <t>Unit tests</t>
   </si>
   <si>
@@ -256,12 +244,30 @@
   </si>
   <si>
     <t>Frontend React/Redux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add POST method (controllers+services+server side validation+DAL) </t>
+  </si>
+  <si>
+    <t>Add PUT method (controllers+server side validation+services+DAL)</t>
+  </si>
+  <si>
+    <t>Add DELETE method (controllers+server side validation+services+DAL)</t>
+  </si>
+  <si>
+    <t>TA20</t>
+  </si>
+  <si>
+    <t>Investigate OData</t>
+  </si>
+  <si>
+    <t>Create .Net Rest Api application with GET method (controllers+services+DAL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -770,7 +776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -874,6 +880,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,8 +984,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -992,9 +1001,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1032,7 +1041,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1104,7 +1113,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1254,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,27 +1282,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="57" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="58"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1311,14 +1320,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
+      <c r="B3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1329,12 +1338,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="59" t="s">
+      <c r="A4" s="47"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1355,8 +1364,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>24</v>
@@ -1382,8 +1391,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -1409,8 +1418,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>28</v>
@@ -1436,14 +1445,14 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>36</v>
@@ -1463,8 +1472,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>38</v>
@@ -1487,19 +1496,19 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
         <f>SUM(G11,G15,G18)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -1507,12 +1516,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="59" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="60"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1525,19 +1534,19 @@
       </c>
       <c r="H11" s="23">
         <f>SUM(H12:H16)</f>
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="I11" s="23">
         <f>SUM(I12:I16)</f>
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>39</v>
@@ -1557,11 +1566,11 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>25</v>
@@ -1581,11 +1590,11 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
@@ -1605,14 +1614,14 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="62"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="63"/>
       <c r="E15" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>35</v>
@@ -1623,22 +1632,22 @@
       </c>
       <c r="H15" s="11">
         <f>SUM(H16:H17)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I15" s="11">
         <f>SUM(I16:I17)</f>
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>35</v>
@@ -1647,187 +1656,187 @@
         <v>8</v>
       </c>
       <c r="H16" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I16" s="2">
         <f>G16-H16</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2">
         <v>8</v>
       </c>
       <c r="H17" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I17" s="2">
         <f>G17-H17</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="42"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="43"/>
       <c r="E18" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="12">
-        <f>SUM(G19:G20)</f>
-        <v>8</v>
-      </c>
-      <c r="H18" s="12">
-        <f>SUM(H19:H20)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="12">
-        <f>SUM(I19:I20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="49"/>
+        <f>SUM(G19:G21)</f>
+        <v>10</v>
+      </c>
+      <c r="H18" s="35">
+        <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G19" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="2">
         <f>G19-H19</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="8">
-        <v>4</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="8">
+      <c r="G20" s="2">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <f>G20-H20</f>
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="48" t="s">
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="8">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30">
-        <f>SUM(G22)</f>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30">
+        <f>SUM(G23)</f>
         <v>40</v>
       </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="H22" s="29"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="12">
-        <f>SUM(G23:G29)</f>
+      <c r="G23" s="12">
+        <f>SUM(G24:G30)</f>
         <v>40</v>
       </c>
-      <c r="H22" s="12">
-        <f t="shared" ref="H22:I22" si="1">SUM(H23:H29)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
-        <f t="shared" si="1"/>
+      <c r="H23" s="12">
+        <f t="shared" ref="H23:I23" si="2">SUM(H24:H30)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="2">
-        <v>4</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <f>G23-H23</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="49"/>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>34</v>
@@ -1839,19 +1848,19 @@
         <v>0</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" ref="I24:I29" si="2">G24-H24</f>
+        <f>G24-H24</f>
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>34</v>
@@ -1863,19 +1872,19 @@
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="49"/>
+        <f t="shared" ref="I25:I30" si="3">G25-H25</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>34</v>
@@ -1887,208 +1896,232 @@
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="8">
-        <v>12</v>
+      <c r="G27" s="2">
+        <v>4</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" ref="I27:I28" si="3">G27-H27</f>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I28:I29" si="4">G28-H28</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="50"/>
       <c r="C29" s="7"/>
       <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="8">
+        <v>8</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="48"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="8">
+        <v>4</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="30">
+        <f>120</f>
+        <v>120</v>
+      </c>
+      <c r="H31" s="33"/>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="F32" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="36">
+        <f>SUM(G33:G33)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="36">
+        <f>SUM(H33:H33)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="36">
+        <f>SUM(I33:I33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="38"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="30">
+        <f>80</f>
+        <v>80</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" s="31"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="45"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F35" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="8">
-        <v>4</v>
-      </c>
-      <c r="H29" s="8">
-        <v>0</v>
-      </c>
-      <c r="I29" s="8">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="30">
-        <f>SUM(G31)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="31"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="35">
-        <f>SUM(G32:G32)</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="35">
-        <f>SUM(H32:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="35">
-        <f>SUM(I32:I32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="30">
-        <f>SUM(G34)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="40"/>
-      <c r="E34" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="35">
-        <v>0</v>
-      </c>
-      <c r="H34" s="35">
-        <f>SUM(H35:H38)</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="35">
-        <f>SUM(I35:I38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="G35" s="36">
+        <v>0</v>
+      </c>
+      <c r="H35" s="36">
+        <f>SUM(H36:H39)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="36">
+        <f>SUM(I36:I39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B36" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2098,30 +2131,30 @@
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A10:A20"/>
-    <mergeCell ref="B10:B20"/>
+    <mergeCell ref="A10:A21"/>
+    <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:E33"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F31 F33:F34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:F35 F4:F32">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update database and plan
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOTNET_React_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Schedule_state">Лист1!$U$5:$U$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,109 +883,109 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1001,9 +1001,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1041,7 +1041,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1113,7 +1113,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,27 +1282,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="58" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1320,14 +1320,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
+      <c r="B3" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1338,12 +1338,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="60" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1364,8 +1364,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>24</v>
@@ -1391,8 +1391,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -1418,8 +1418,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>28</v>
@@ -1445,8 +1445,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
@@ -1472,8 +1472,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>38</v>
@@ -1496,14 +1496,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1516,12 +1516,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="60" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="61"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1534,16 +1534,16 @@
       </c>
       <c r="H11" s="23">
         <f>SUM(H12:H16)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I11" s="23">
         <f>SUM(I12:I16)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>40</v>
@@ -1566,8 +1566,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>41</v>
@@ -1590,8 +1590,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>42</v>
@@ -1614,17 +1614,17 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="62" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="11" t="s">
         <v>53</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="11">
         <f>SUM(G16:G17)</f>
@@ -1632,16 +1632,16 @@
       </c>
       <c r="H15" s="11">
         <f>SUM(H16:H17)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I15" s="11">
         <f>SUM(I16:I17)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
         <v>45</v>
@@ -1650,22 +1650,22 @@
         <v>48</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" s="2">
         <v>8</v>
       </c>
       <c r="H16" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I16" s="2">
         <f>G16-H16</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>46</v>
@@ -1688,17 +1688,17 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="68" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="43"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="12" t="s">
         <v>54</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G18" s="12">
         <f>SUM(G19:G21)</f>
@@ -1706,16 +1706,16 @@
       </c>
       <c r="H18" s="35">
         <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I18" s="35">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>50</v>
@@ -1724,22 +1724,22 @@
         <v>76</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2">
         <v>2</v>
       </c>
       <c r="H19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="2">
         <f>G19-H19</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2" t="s">
         <v>70</v>
@@ -1754,16 +1754,16 @@
         <v>4</v>
       </c>
       <c r="H20" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20" s="2">
         <f>G20-H20</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="7"/>
       <c r="D21" s="2" t="s">
         <v>51</v>
@@ -1785,14 +1785,14 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="49" t="s">
+      <c r="A22" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="30">
@@ -1803,12 +1803,12 @@
       <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="43" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="12" t="s">
         <v>59</v>
       </c>
@@ -1829,8 +1829,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
         <v>56</v>
@@ -1853,8 +1853,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>57</v>
@@ -1877,8 +1877,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
         <v>58</v>
@@ -1901,8 +1901,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
         <v>60</v>
@@ -1925,8 +1925,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="50"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2" t="s">
         <v>61</v>
@@ -1949,8 +1949,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="7"/>
       <c r="D29" s="2" t="s">
         <v>67</v>
@@ -1973,8 +1973,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="7"/>
       <c r="D30" s="2" t="s">
         <v>75</v>
@@ -2003,8 +2003,8 @@
       <c r="B31" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="28"/>
       <c r="F31" s="33"/>
       <c r="G31" s="30">
@@ -2021,25 +2021,25 @@
       <c r="B32" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="36" t="s">
+      <c r="D32" s="65"/>
+      <c r="E32" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="36">
+      <c r="G32" s="68">
         <f>SUM(G33:G33)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="36">
+      <c r="H32" s="68">
         <f>SUM(H33:H33)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="36">
+      <c r="I32" s="68">
         <f>SUM(I33:I33)</f>
         <v>0</v>
       </c>
@@ -2051,23 +2051,23 @@
       <c r="B33" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="39"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="28"/>
       <c r="F34" s="33"/>
       <c r="G34" s="30">
@@ -2078,26 +2078,26 @@
       <c r="I34" s="31"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="40" t="s">
+      <c r="A35" s="63"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="36" t="s">
+      <c r="D35" s="65"/>
+      <c r="E35" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="36" t="s">
+      <c r="F35" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="36">
-        <v>0</v>
-      </c>
-      <c r="H35" s="36">
+      <c r="G35" s="68">
+        <v>0</v>
+      </c>
+      <c r="H35" s="68">
         <f>SUM(H36:H39)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I35" s="68">
         <f>SUM(I36:I39)</f>
         <v>0</v>
       </c>
@@ -2109,16 +2109,33 @@
       <c r="B36" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="B22:B30"/>
@@ -2135,23 +2152,6 @@
     <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:E33"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:F35 F4:F32">

</xml_diff>

<commit_message>
Update plan and main structure of database
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
   <si>
     <t>11.09.18</t>
   </si>
@@ -262,6 +262,33 @@
   </si>
   <si>
     <t>Create .Net Rest Api application with GET method (controllers+services+DAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Update structure of database to minimal project</t>
+  </si>
+  <si>
+    <t>Create new database in Microsoft SQL</t>
+  </si>
+  <si>
+    <t>Update database</t>
+  </si>
+  <si>
+    <t>TA21</t>
+  </si>
+  <si>
+    <t>TA22</t>
+  </si>
+  <si>
+    <t>US8</t>
+  </si>
+  <si>
+    <t>TA23</t>
+  </si>
+  <si>
+    <t>TA24</t>
   </si>
 </sst>
 </file>
@@ -776,7 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -883,12 +910,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -956,30 +1010,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1263,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,27 +1312,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="48" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="50" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="51"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1320,14 +1350,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
+      <c r="B3" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="65"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1338,12 +1368,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="52" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1364,8 +1394,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>24</v>
@@ -1391,8 +1421,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -1418,8 +1448,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>28</v>
@@ -1445,8 +1475,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
@@ -1472,8 +1502,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>38</v>
@@ -1496,14 +1526,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1516,12 +1546,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="52" t="s">
+      <c r="A11" s="48"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="53"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1542,8 +1572,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>40</v>
@@ -1566,8 +1596,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>41</v>
@@ -1590,8 +1620,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>42</v>
@@ -1614,12 +1644,12 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="54" t="s">
+      <c r="A15" s="48"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="55"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="11" t="s">
         <v>53</v>
       </c>
@@ -1640,8 +1670,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
         <v>45</v>
@@ -1663,9 +1693,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="42"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="48"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>46</v>
@@ -1687,13 +1717,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="60" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="48"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="61"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="12" t="s">
         <v>54</v>
       </c>
@@ -1713,9 +1743,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="42"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>50</v>
@@ -1724,23 +1754,23 @@
         <v>76</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G19" s="2">
         <v>2</v>
       </c>
       <c r="H19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" s="2">
         <f>G19-H19</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="2" t="s">
         <v>70</v>
       </c>
@@ -1748,23 +1778,26 @@
         <v>77</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" s="2">
         <v>4</v>
       </c>
       <c r="H20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2">
         <f>G20-H20</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="2" t="s">
         <v>51</v>
       </c>
@@ -1784,361 +1817,466 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="41" t="s">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="30">
-        <f>SUM(G23)</f>
-        <v>40</v>
+        <f>SUM(G23,G26)</f>
+        <v>52</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="31"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="61" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="48"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="12">
-        <f>SUM(G24:G30)</f>
-        <v>40</v>
-      </c>
-      <c r="H23" s="12">
-        <f t="shared" ref="H23:I23" si="2">SUM(H24:H30)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="12">
+      <c r="D23" s="38"/>
+      <c r="E23" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="36">
+        <f>SUM(G24:G25)</f>
+        <v>4</v>
+      </c>
+      <c r="H23" s="36">
+        <f t="shared" ref="H23:I23" si="2">SUM(H24:H25)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="36">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="42"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="48"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G24" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="I24" s="2">
         <f>G24-H24</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="42"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="48"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <f>G25-H25</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="48"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="2">
-        <v>4</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" ref="I25:I30" si="3">G25-H25</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="2">
-        <v>4</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
+      <c r="G26" s="12">
+        <f>SUM(G27:G35)</f>
+        <v>48</v>
+      </c>
+      <c r="H26" s="36">
+        <f t="shared" ref="H26:I26" si="3">SUM(H27:H35)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="36">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="42"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="48"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <f>G27-H27</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="E28" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="2">
-        <v>4</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="2" t="s">
+      <c r="G28" s="8">
+        <v>4</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0</v>
+      </c>
+      <c r="I28" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="48"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="8">
-        <v>12</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" ref="I28:I29" si="4">G28-H28</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>66</v>
+      <c r="E29" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="2">
+        <v>4</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <f>G29-H29</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="48"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <f>G30-H30</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="48"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="2">
+        <v>4</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <f>G31-H31</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="48"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="2">
+        <v>4</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <f>G32-H32</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="48"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="8">
+        <v>12</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <f>G33-H33</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="48"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="8">
         <v>8</v>
       </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="4"/>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <f>G34-H34</f>
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="26" t="s">
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="8">
-        <v>4</v>
-      </c>
-      <c r="H30" s="8">
-        <v>0</v>
-      </c>
-      <c r="I30" s="8">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
+      <c r="G35" s="8">
+        <v>4</v>
+      </c>
+      <c r="H35" s="8">
+        <v>0</v>
+      </c>
+      <c r="I35" s="8">
+        <f>G35-H35</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="30">
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="30">
         <f>120</f>
         <v>120</v>
       </c>
-      <c r="H31" s="33"/>
-      <c r="I31" s="31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="H36" s="33"/>
+      <c r="I36" s="31"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B37" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="65"/>
-      <c r="E32" s="68" t="s">
+      <c r="C37" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="42"/>
+      <c r="E37" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="68" t="s">
+      <c r="F37" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="68">
-        <f>SUM(G33:G33)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="68">
-        <f>SUM(H33:H33)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="68">
-        <f>SUM(I33:I33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
+      <c r="G37" s="37">
+        <f>SUM(G38:G38)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="37">
+        <f>SUM(H38:H38)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="37">
+        <f>SUM(I38:I38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B38" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="62" t="s">
+      <c r="C38" s="43"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="62" t="s">
+      <c r="B39" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="30">
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="30">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="31"/>
-    </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="63"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="65"/>
-      <c r="E35" s="68" t="s">
+      <c r="H39" s="33"/>
+      <c r="I39" s="31"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="46"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="42"/>
+      <c r="E40" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="68" t="s">
+      <c r="F40" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="68">
-        <v>0</v>
-      </c>
-      <c r="H35" s="68">
-        <f>SUM(H36:H39)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="68">
-        <f>SUM(I36:I39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="G40" s="37">
+        <v>0</v>
+      </c>
+      <c r="H40" s="37">
+        <f>SUM(H41:H44)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="37">
+        <f>SUM(I41:I44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B41" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="66"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D36"/>
+  <mergeCells count="34">
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="A22:A35"/>
+    <mergeCell ref="B22:B35"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2152,16 +2290,33 @@
     <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D38"/>
+    <mergeCell ref="E37:E38"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:F35 F4:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39:F40 F4:F37">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I15 I18" formula="1"/>
+    <ignoredError sqref="I15 I18 I26" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create a file discribing funcionality Update plan Update RestApiApp
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
   <si>
     <t>11.09.18</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>TA24</t>
+  </si>
+  <si>
+    <t>TA25</t>
+  </si>
+  <si>
+    <t>Create SPA with simple components</t>
   </si>
 </sst>
 </file>
@@ -356,7 +362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -793,6 +799,41 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -803,7 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -904,27 +945,51 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -967,12 +1032,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -994,22 +1053,43 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1293,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,27 +1392,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="51" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="53" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="62"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1350,14 +1430,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1368,12 +1448,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="55" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1394,8 +1474,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>24</v>
@@ -1421,8 +1501,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -1448,8 +1528,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>28</v>
@@ -1475,8 +1555,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="45"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
@@ -1502,8 +1582,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
-      <c r="B9" s="46"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>38</v>
@@ -1526,14 +1606,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1546,12 +1626,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="55" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="56"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1572,8 +1652,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>40</v>
@@ -1596,8 +1676,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="45"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>41</v>
@@ -1620,8 +1700,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>42</v>
@@ -1644,12 +1724,12 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="57" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="58"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="11" t="s">
         <v>53</v>
       </c>
@@ -1670,8 +1750,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="45"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
         <v>45</v>
@@ -1694,8 +1774,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>46</v>
@@ -1718,12 +1798,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="63" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="37"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="12" t="s">
         <v>54</v>
       </c>
@@ -1734,18 +1814,18 @@
         <f>SUM(G19:G21)</f>
         <v>10</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="34">
         <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
         <v>3</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="34">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>50</v>
@@ -1768,8 +1848,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="24"/>
       <c r="D20" s="2" t="s">
         <v>70</v>
@@ -1795,8 +1875,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="25"/>
       <c r="D21" s="2" t="s">
         <v>51</v>
@@ -1818,10 +1898,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="44" t="s">
+      <c r="A22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="39"/>
@@ -1836,34 +1916,34 @@
       <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="37" t="s">
+      <c r="A23" s="50"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="44" t="s">
         <v>55</v>
       </c>
       <c r="D23" s="38"/>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="36" t="s">
+      <c r="F23" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="36">
+      <c r="G23" s="35">
         <f>SUM(G24:G25)</f>
         <v>4</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="35">
         <f t="shared" ref="H23:I23" si="2">SUM(H24:H25)</f>
         <v>2</v>
       </c>
-      <c r="I23" s="36">
+      <c r="I23" s="35">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
         <v>56</v>
@@ -1886,8 +1966,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="45"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>57</v>
@@ -1910,9 +1990,9 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="37" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="44" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="38"/>
@@ -1926,18 +2006,18 @@
         <f>SUM(G27:G35)</f>
         <v>48</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="35">
         <f t="shared" ref="H26:I26" si="3">SUM(H27:H35)</f>
         <v>1</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I26" s="35">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
         <v>58</v>
@@ -1960,8 +2040,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="5"/>
       <c r="D28" s="2" t="s">
         <v>60</v>
@@ -1983,8 +2063,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
         <v>61</v>
@@ -2007,8 +2087,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="45"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="5"/>
       <c r="D30" s="2" t="s">
         <v>67</v>
@@ -2031,8 +2111,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="45"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
         <v>75</v>
@@ -2055,8 +2135,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="45"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
         <v>82</v>
@@ -2078,9 +2158,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="45"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="50"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="7"/>
       <c r="D33" s="2" t="s">
         <v>83</v>
@@ -2102,9 +2182,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="50"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="7"/>
       <c r="D34" s="2" t="s">
         <v>85</v>
@@ -2126,9 +2206,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="43"/>
-      <c r="B35" s="46"/>
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="51"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="7"/>
       <c r="D35" s="2" t="s">
         <v>86</v>
@@ -2150,11 +2230,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="79" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="39"/>
@@ -2162,139 +2242,170 @@
       <c r="E36" s="28"/>
       <c r="F36" s="33"/>
       <c r="G36" s="30">
-        <f>120</f>
-        <v>120</v>
+        <f>SUM(G37)</f>
+        <v>16</v>
       </c>
       <c r="H36" s="33"/>
       <c r="I36" s="31"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="K36" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="78"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="82" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="45"/>
+      <c r="E37" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="36">
+        <f>SUM(G38:G40)</f>
+        <v>16</v>
+      </c>
+      <c r="H37" s="36">
+        <f t="shared" ref="H37:I37" si="5">SUM(H38:H40)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="36">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="78"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="2">
+        <v>16</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" ref="I38" si="6">G38-H38</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="78"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="48"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B41" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="67"/>
-      <c r="E37" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="69">
-        <f>SUM(G38:G38)</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="69">
-        <f>SUM(H38:H38)</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="69">
-        <f>SUM(I38:I38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="32" t="s">
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B42" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="68"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="30">
+      <c r="C42" s="70"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="74">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H39" s="33"/>
-      <c r="I39" s="31"/>
-    </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="65"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="66" t="s">
+      <c r="H42" s="73"/>
+      <c r="I42" s="75"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="67"/>
-      <c r="E40" s="69" t="s">
+      <c r="D43" s="42"/>
+      <c r="E43" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="69" t="s">
+      <c r="F43" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="69">
+      <c r="G43" s="37">
         <v>0</v>
       </c>
-      <c r="H40" s="69">
-        <f>SUM(H41:H44)</f>
+      <c r="H43" s="37">
+        <f>SUM(H44:H47)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="69">
-        <f>SUM(I41:I44)</f>
+      <c r="I43" s="37">
+        <f>SUM(I44:I47)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+    <row r="44" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+    </row>
+    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B45" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A22:A35"/>
-    <mergeCell ref="B22:B35"/>
+  <mergeCells count="31">
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2307,9 +2418,28 @@
     <mergeCell ref="A10:A21"/>
     <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A22:A35"/>
+    <mergeCell ref="B22:B35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39:F40 F4:F37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:F43 F4:F39">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update plan, file with actions on SPA, schema and sql file for minimal database
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOTNET_React_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOTNET_React_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Schedule_state">Лист1!$U$5:$U$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
   <si>
     <t>11.09.18</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>To Do</t>
-  </si>
-  <si>
-    <t>Actuals</t>
   </si>
   <si>
     <t>TA1</t>
@@ -207,9 +204,6 @@
     <t>TA16</t>
   </si>
   <si>
-    <t>Backend Web Api (add POST, PUT, DELETE methods)</t>
-  </si>
-  <si>
     <t>TA17</t>
   </si>
   <si>
@@ -246,15 +240,6 @@
     <t>Frontend React/Redux</t>
   </si>
   <si>
-    <t xml:space="preserve">Add POST method (controllers+services+server side validation+DAL) </t>
-  </si>
-  <si>
-    <t>Add PUT method (controllers+server side validation+services+DAL)</t>
-  </si>
-  <si>
-    <t>Add DELETE method (controllers+server side validation+services+DAL)</t>
-  </si>
-  <si>
     <t>TA20</t>
   </si>
   <si>
@@ -294,13 +279,58 @@
     <t>TA25</t>
   </si>
   <si>
-    <t>Create SPA with simple components</t>
+    <t>Time Spent</t>
+  </si>
+  <si>
+    <t>Update database in SQL Server</t>
+  </si>
+  <si>
+    <t>Create .Net Rest Api application</t>
+  </si>
+  <si>
+    <t>Add GET method for "List of products" (controllers+services+server side validation+DAL)</t>
+  </si>
+  <si>
+    <t>Add Post method for "Create order" (controllers+services+server side validation+DAL)</t>
+  </si>
+  <si>
+    <t>Backend Web Api (add GET, POST methods)</t>
+  </si>
+  <si>
+    <t>TA26</t>
+  </si>
+  <si>
+    <t>TA27</t>
+  </si>
+  <si>
+    <t>TA28</t>
+  </si>
+  <si>
+    <t>Create mock-up for page with List of products</t>
+  </si>
+  <si>
+    <t>Mock-ups for List of products and Orders</t>
+  </si>
+  <si>
+    <t>Create mock-up for page with Order</t>
+  </si>
+  <si>
+    <t>Create SPA with simple components for List of product</t>
+  </si>
+  <si>
+    <t>TA29</t>
+  </si>
+  <si>
+    <t>TA30</t>
+  </si>
+  <si>
+    <t>Connect App with React/Redux infrastructure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -757,21 +787,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -831,7 +846,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -844,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -942,160 +957,175 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1111,9 +1141,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1151,7 +1181,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1223,7 +1253,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1373,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,32 +1422,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="61" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="62"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>21</v>
@@ -1426,18 +1456,18 @@
         <v>22</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1448,17 +1478,17 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="6">
         <f>SUM(G5:G9)</f>
@@ -1474,17 +1504,17 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2">
         <v>8</v>
@@ -1497,21 +1527,21 @@
         <v>4</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2">
         <v>4</v>
@@ -1524,21 +1554,21 @@
         <v>2</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2">
         <v>4</v>
@@ -1551,21 +1581,21 @@
         <v>2</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="53"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="8">
         <v>8</v>
@@ -1578,21 +1608,21 @@
         <v>0</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="14">
         <v>4</v>
@@ -1606,14 +1636,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1626,17 +1656,17 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="46"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="50"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="23">
         <f>SUM(G12:G14)</f>
@@ -1652,17 +1682,17 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="2">
         <v>4</v>
@@ -1676,17 +1706,17 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2">
         <v>4</v>
@@ -1700,17 +1730,17 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2">
         <v>4</v>
@@ -1724,17 +1754,17 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="64"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="52"/>
       <c r="E15" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="11">
         <f>SUM(G16:G17)</f>
@@ -1750,17 +1780,17 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="53"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="2">
         <v>8</v>
@@ -1774,17 +1804,17 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="53"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="2">
         <v>8</v>
@@ -1798,43 +1828,43 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="44"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="64"/>
       <c r="E18" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18" s="12">
         <f>SUM(G19:G21)</f>
         <v>10</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="33">
         <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
         <v>3</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="33">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2">
         <v>2</v>
@@ -1848,17 +1878,17 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="24"/>
       <c r="D20" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" s="2">
         <v>4</v>
@@ -1871,21 +1901,21 @@
         <v>3</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="25"/>
       <c r="D21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="8">
         <v>4</v>
@@ -1898,61 +1928,61 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="52" t="s">
+      <c r="A22" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="30">
-        <f>SUM(G23,G26)</f>
-        <v>52</v>
+        <f>SUM(G23,G28,G37,G40)</f>
+        <v>92</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="35">
-        <f>SUM(G24:G25)</f>
-        <v>4</v>
+      <c r="A23" s="54"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="72"/>
+      <c r="E23" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="34">
+        <f>SUM(G24:G27)</f>
+        <v>6</v>
       </c>
       <c r="H23" s="35">
-        <f t="shared" ref="H23:I23" si="2">SUM(H24:H25)</f>
-        <v>2</v>
+        <f t="shared" ref="H23:I23" si="2">SUM(H24:H27)</f>
+        <v>3.25</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G24" s="2">
         <v>2</v>
@@ -1966,17 +1996,17 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G25" s="2">
         <v>2</v>
@@ -1989,139 +2019,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="12" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="12">
-        <f>SUM(G27:G35)</f>
-        <v>48</v>
-      </c>
-      <c r="H26" s="35">
-        <f t="shared" ref="H26:I26" si="3">SUM(H27:H35)</f>
+      <c r="G26" s="2">
         <v>1</v>
       </c>
-      <c r="I26" s="35">
-        <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="53"/>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <f>G26-H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="54"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G27" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="I27" s="2">
         <f>G27-H27</f>
-        <v>3</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="27" t="s">
+      <c r="A28" s="54"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="72"/>
+      <c r="E28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="8">
-        <v>4</v>
-      </c>
-      <c r="H28" s="8">
-        <v>0</v>
-      </c>
-      <c r="I28" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="53"/>
+      <c r="G28" s="12">
+        <f>SUM(G29:G36)</f>
+        <v>46</v>
+      </c>
+      <c r="H28" s="34">
+        <f ca="1">SUM(H26:H36)</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="34">
+        <f ca="1">SUM(I26:I36)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G29" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" ref="I29:I35" si="4">G29-H29</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="53"/>
+        <f>G29-H29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="5"/>
       <c r="D30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="2">
-        <v>4</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="53"/>
+      <c r="G30" s="8">
+        <v>4</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0</v>
+      </c>
+      <c r="I30" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>34</v>
+        <v>86</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="G31" s="2">
         <v>4</v>
@@ -2130,282 +2160,465 @@
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="53"/>
+        <f t="shared" ref="I31" si="3">G31-H31</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="57"/>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="2">
+        <v>8</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" ref="I32" si="4">G32-H32</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="2">
+        <v>4</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <f>G33-H33</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="8">
+        <v>12</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <f>G34-H34</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="8">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <f>G35-H35</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" s="2">
-        <v>4</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="8">
-        <v>12</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33" s="2">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="8">
+      <c r="E36" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="8">
+        <v>4</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0</v>
+      </c>
+      <c r="I36" s="8">
+        <f t="shared" ref="I36" si="5">G36-H36</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="54"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="80"/>
+      <c r="E37" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="11">
+        <f>SUM(G38:G39)</f>
+        <v>4</v>
+      </c>
+      <c r="H37" s="11">
+        <f t="shared" ref="H37:I37" si="6">SUM(H38:H39)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="11">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="54"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38" s="2">
+        <v>2</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" ref="I38" si="7">G38-H38</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="54"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" s="8">
+        <v>2</v>
+      </c>
+      <c r="H39" s="8">
+        <v>0</v>
+      </c>
+      <c r="I39" s="8">
+        <f t="shared" ref="I39" si="8">G39-H39</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="54"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="80"/>
+      <c r="E40" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" s="11">
+        <f>SUM(G41:G43)</f>
+        <v>36</v>
+      </c>
+      <c r="H40" s="11">
+        <f>SUM(H41:H43)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="11">
+        <f>SUM(I41:I43)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="2">
+        <v>4</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" s="2">
+        <v>16</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" ref="I42" si="9">G42-H42</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="55"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="2">
+        <v>16</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" ref="I43" si="10">G43-H43</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="83"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="87"/>
+      <c r="K44" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="75"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="75"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="75"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="66"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="2">
-        <v>0</v>
-      </c>
-      <c r="I34" s="2">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="8">
-        <v>4</v>
-      </c>
-      <c r="H35" s="8">
-        <v>0</v>
-      </c>
-      <c r="I35" s="8">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="77" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="79" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="30">
-        <f>SUM(G37)</f>
-        <v>16</v>
-      </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="31"/>
-      <c r="K36" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="78"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="82" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="36">
-        <f>SUM(G38:G40)</f>
-        <v>16</v>
-      </c>
-      <c r="H37" s="36">
-        <f t="shared" ref="H37:I37" si="5">SUM(H38:H40)</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="36">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="78"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" s="2">
-        <v>16</v>
-      </c>
-      <c r="H38" s="2">
-        <v>0</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" ref="I38" si="6">G38-H38</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="78"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="32" t="s">
+      <c r="B49" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B50" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="74">
+      <c r="C50" s="67"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="38">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H42" s="73"/>
-      <c r="I42" s="75"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
+      <c r="H50" s="37"/>
+      <c r="I50" s="39"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B51" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" s="37">
-        <v>0</v>
-      </c>
-      <c r="H43" s="37">
-        <f>SUM(H44:H47)</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="37">
-        <f>SUM(I44:I47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-    </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="C51" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="70"/>
+      <c r="E51" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="F51" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="79">
+        <v>0</v>
+      </c>
+      <c r="H51" s="79">
+        <f>SUM(H52:H55)</f>
+        <v>0</v>
+      </c>
+      <c r="I51" s="79">
+        <f>SUM(I52:I55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="66"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="72"/>
+      <c r="G52" s="72"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="72"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B53" s="32" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A22:A43"/>
+    <mergeCell ref="B22:B43"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2419,34 +2632,16 @@
     <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A22:A35"/>
-    <mergeCell ref="B22:B35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:F43 F4:F39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F50:F51 F4:F44">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I15 I18 I26" formula="1"/>
+    <ignoredError sqref="I15 I18 I28 I37" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OnlineStoreRestApiApplication + Update plan + Update database + Add file for add entities in database
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -291,9 +291,6 @@
     <t>Add GET method for "List of products" (controllers+services+server side validation+DAL)</t>
   </si>
   <si>
-    <t>Add Post method for "Create order" (controllers+services+server side validation+DAL)</t>
-  </si>
-  <si>
     <t>Backend Web Api (add GET, POST methods)</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>Connect App with React/Redux infrastructure</t>
+  </si>
+  <si>
+    <t>Add POST method for "Create order" (controllers+services+server side validation+DAL)</t>
   </si>
 </sst>
 </file>
@@ -981,136 +981,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1120,6 +991,135 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,27 +1422,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="47" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1460,14 +1460,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
+      <c r="B3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1478,12 +1478,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1504,8 +1504,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="57"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>23</v>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -1558,8 +1558,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="57"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>27</v>
@@ -1585,8 +1585,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="57"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>31</v>
@@ -1612,8 +1612,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>37</v>
@@ -1636,14 +1636,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1656,12 +1656,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="49" t="s">
+      <c r="A11" s="58"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1682,8 +1682,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="57"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>39</v>
@@ -1706,8 +1706,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="57"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>40</v>
@@ -1730,8 +1730,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="57"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>41</v>
@@ -1754,12 +1754,12 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="51" t="s">
+      <c r="A15" s="58"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="52"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="11" t="s">
         <v>52</v>
       </c>
@@ -1780,8 +1780,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
         <v>44</v>
@@ -1804,8 +1804,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="57"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>45</v>
@@ -1828,12 +1828,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="63" t="s">
+      <c r="A18" s="58"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="64"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="12" t="s">
         <v>53</v>
       </c>
@@ -1854,8 +1854,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="57"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>49</v>
@@ -1878,8 +1878,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
-      <c r="B20" s="57"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="24"/>
       <c r="D20" s="2" t="s">
         <v>68</v>
@@ -1905,8 +1905,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="57"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="25"/>
       <c r="D21" s="2" t="s">
         <v>50</v>
@@ -1928,14 +1928,14 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="56" t="s">
+      <c r="A22" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="73"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="78"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="30">
@@ -1946,12 +1946,12 @@
       <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="64" t="s">
+      <c r="A23" s="58"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="72"/>
+      <c r="D23" s="76"/>
       <c r="E23" s="34" t="s">
         <v>76</v>
       </c>
@@ -1972,8 +1972,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="57"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
         <v>55</v>
@@ -1996,8 +1996,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="57"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>56</v>
@@ -2020,8 +2020,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="57"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
         <v>57</v>
@@ -2044,8 +2044,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="57"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
         <v>58</v>
@@ -2068,14 +2068,14 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="64" t="s">
+      <c r="A28" s="58"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="72"/>
+      <c r="D28" s="76"/>
       <c r="E28" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>34</v>
@@ -2094,8 +2094,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="57"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
         <v>59</v>
@@ -2104,22 +2104,22 @@
         <v>85</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
       </c>
       <c r="H29" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" s="2">
         <f>G29-H29</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="57"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="5"/>
       <c r="D30" s="2" t="s">
         <v>65</v>
@@ -2128,21 +2128,21 @@
         <v>46</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G30" s="8">
         <v>4</v>
       </c>
       <c r="H30" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="57"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
         <v>70</v>
@@ -2151,28 +2151,28 @@
         <v>86</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G31" s="2">
         <v>4</v>
       </c>
       <c r="H31" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ref="I31" si="3">G31-H31</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="57"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>33</v>
@@ -2189,8 +2189,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="57"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="5"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
@@ -2213,8 +2213,8 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="57"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="5"/>
       <c r="D34" s="2" t="s">
         <v>80</v>
@@ -2237,8 +2237,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
-      <c r="B35" s="57"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="5"/>
       <c r="D35" s="2" t="s">
         <v>81</v>
@@ -2261,8 +2261,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
-      <c r="B36" s="57"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8" t="s">
         <v>82</v>
@@ -2285,14 +2285,14 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="52" t="s">
+      <c r="A37" s="58"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="80"/>
+      <c r="D37" s="84"/>
       <c r="E37" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>33</v>
@@ -2311,14 +2311,14 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
-      <c r="B38" s="57"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="61"/>
       <c r="C38" s="5"/>
       <c r="D38" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>33</v>
@@ -2335,14 +2335,14 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
-      <c r="B39" s="57"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="61"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>33</v>
@@ -2359,12 +2359,12 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="52" t="s">
+      <c r="A40" s="58"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="80"/>
+      <c r="D40" s="84"/>
       <c r="E40" s="11" t="s">
         <v>69</v>
       </c>
@@ -2385,14 +2385,14 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
-      <c r="B41" s="57"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="61"/>
       <c r="C41" s="5"/>
       <c r="D41" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>33</v>
@@ -2408,14 +2408,14 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
-      <c r="B42" s="57"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="61"/>
       <c r="C42" s="5"/>
       <c r="D42" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>33</v>
@@ -2432,14 +2432,14 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
-      <c r="B43" s="58"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="62"/>
       <c r="C43" s="5"/>
       <c r="D43" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>33</v>
@@ -2456,26 +2456,26 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="74" t="s">
+      <c r="A44" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="83"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="86"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="43"/>
       <c r="G44" s="19"/>
-      <c r="H44" s="86"/>
-      <c r="I44" s="87"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="44"/>
       <c r="K44" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="75"/>
-      <c r="B45" s="77"/>
+      <c r="A45" s="80"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="40"/>
       <c r="D45" s="40"/>
       <c r="E45" s="40"/>
@@ -2485,8 +2485,8 @@
       <c r="I45" s="40"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="75"/>
-      <c r="B46" s="77"/>
+      <c r="A46" s="80"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
       <c r="E46" s="40"/>
@@ -2496,8 +2496,8 @@
       <c r="I46" s="40"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="75"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="82"/>
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
       <c r="E47" s="40"/>
@@ -2507,8 +2507,8 @@
       <c r="I47" s="40"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="66"/>
-      <c r="B48" s="78"/>
+      <c r="A48" s="70"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="40"/>
       <c r="D48" s="40"/>
       <c r="E48" s="40"/>
@@ -2521,7 +2521,7 @@
       <c r="A49" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="40"/>
@@ -2539,8 +2539,8 @@
       <c r="B50" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="67"/>
-      <c r="D50" s="68"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="72"/>
       <c r="E50" s="36"/>
       <c r="F50" s="37"/>
       <c r="G50" s="38">
@@ -2551,44 +2551,44 @@
       <c r="I50" s="39"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="65" t="s">
+      <c r="B51" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="69" t="s">
+      <c r="C51" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="70"/>
-      <c r="E51" s="79" t="s">
+      <c r="D51" s="74"/>
+      <c r="E51" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="F51" s="79" t="s">
+      <c r="F51" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="79">
-        <v>0</v>
-      </c>
-      <c r="H51" s="79">
+      <c r="G51" s="87">
+        <v>0</v>
+      </c>
+      <c r="H51" s="87">
         <f>SUM(H52:H55)</f>
         <v>0</v>
       </c>
-      <c r="I51" s="79">
+      <c r="I51" s="87">
         <f>SUM(I52:I55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
-      <c r="B52" s="66"/>
-      <c r="C52" s="71"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
+      <c r="A52" s="70"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">

</xml_diff>

<commit_message>
Update plan + Update database (sql code)
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="110">
   <si>
     <t>11.09.18</t>
   </si>
@@ -325,6 +325,40 @@
   </si>
   <si>
     <t>Add POST method for "Create order" (controllers+services+server side validation+DAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Continue] Backend Web Api </t>
+  </si>
+  <si>
+    <t>Method POST: Orders, ItemsOfOrders</t>
+  </si>
+  <si>
+    <t>Add POST method for Users</t>
+  </si>
+  <si>
+    <t>Controllers: Products, Users, Orders, ItemsOfOrders
+Method GET: Products, Users, Orders, ItemsOfOrders</t>
+  </si>
+  <si>
+    <t>Add services+server side validation for all models</t>
+  </si>
+  <si>
+    <t>TA31</t>
+  </si>
+  <si>
+    <t>TA32</t>
+  </si>
+  <si>
+    <t>TA33</t>
+  </si>
+  <si>
+    <t>TA34</t>
+  </si>
+  <si>
+    <t>TA35</t>
+  </si>
+  <si>
+    <t>TA36</t>
   </si>
 </sst>
 </file>
@@ -392,7 +426,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -775,21 +809,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -823,15 +842,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -842,10 +852,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -859,7 +871,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -951,9 +963,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -966,22 +975,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -993,6 +999,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1074,7 +1095,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1083,43 +1110,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1403,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,31 +1424,33 @@
     <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="51" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="55"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1460,14 +1468,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
+      <c r="B3" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1478,12 +1486,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="53" t="s">
+      <c r="A4" s="61"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1504,8 +1512,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="61"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>23</v>
@@ -1531,8 +1539,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="61"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -1558,8 +1566,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="61"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>27</v>
@@ -1585,8 +1593,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="61"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>31</v>
@@ -1612,8 +1620,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="62"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>37</v>
@@ -1636,14 +1644,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1656,12 +1664,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="53" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="57"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1682,8 +1690,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>39</v>
@@ -1706,8 +1714,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>40</v>
@@ -1730,8 +1738,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>41</v>
@@ -1754,12 +1762,12 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="55" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="11" t="s">
         <v>52</v>
       </c>
@@ -1780,8 +1788,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
         <v>44</v>
@@ -1804,8 +1812,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="64"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>45</v>
@@ -1828,12 +1836,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="67" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="68"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="12" t="s">
         <v>53</v>
       </c>
@@ -1844,18 +1852,18 @@
         <f>SUM(G19:G21)</f>
         <v>10</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="32">
         <f t="shared" ref="H18:I18" si="1">SUM(H19:H21)</f>
         <v>3</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="32">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="61"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>49</v>
@@ -1878,8 +1886,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="24"/>
       <c r="D20" s="2" t="s">
         <v>68</v>
@@ -1905,8 +1913,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
-      <c r="B21" s="61"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="25"/>
       <c r="D21" s="2" t="s">
         <v>50</v>
@@ -1928,52 +1936,52 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="60" t="s">
+      <c r="A22" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="81"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="30">
         <f>SUM(G23,G28,G37,G40)</f>
         <v>92</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="31"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="58"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="68" t="s">
+      <c r="A23" s="61"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="71" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="76"/>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="33">
         <f>SUM(G24:G27)</f>
         <v>6</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="34">
         <f t="shared" ref="H23:I23" si="2">SUM(H24:H27)</f>
         <v>3.25</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="34">
         <f t="shared" si="2"/>
         <v>2.75</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
-      <c r="B24" s="61"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="64"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
         <v>55</v>
@@ -1996,8 +2004,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
-      <c r="B25" s="61"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="64"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>56</v>
@@ -2020,8 +2028,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
-      <c r="B26" s="61"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="64"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
         <v>57</v>
@@ -2044,8 +2052,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="58"/>
-      <c r="B27" s="61"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
         <v>58</v>
@@ -2068,9 +2076,9 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="68" t="s">
+      <c r="A28" s="61"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="71" t="s">
         <v>66</v>
       </c>
       <c r="D28" s="76"/>
@@ -2084,18 +2092,18 @@
         <f>SUM(G29:G36)</f>
         <v>46</v>
       </c>
-      <c r="H28" s="34">
+      <c r="H28" s="33">
         <f ca="1">SUM(H26:H36)</f>
         <v>1</v>
       </c>
-      <c r="I28" s="34">
+      <c r="I28" s="33">
         <f ca="1">SUM(I26:I36)</f>
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="58"/>
-      <c r="B29" s="61"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="64"/>
       <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
         <v>59</v>
@@ -2118,8 +2126,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="58"/>
-      <c r="B30" s="61"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="5"/>
       <c r="D30" s="2" t="s">
         <v>65</v>
@@ -2141,8 +2149,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="58"/>
-      <c r="B31" s="61"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
         <v>70</v>
@@ -2151,22 +2159,25 @@
         <v>86</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G31" s="2">
         <v>4</v>
       </c>
       <c r="H31" s="2">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ref="I31" si="3">G31-H31</f>
-        <v>1</v>
+        <v>-12</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="58"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
         <v>77</v>
@@ -2175,22 +2186,25 @@
         <v>98</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G32" s="2">
         <v>8</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ref="I32" si="4">G32-H32</f>
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="58"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="64"/>
       <c r="C33" s="5"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
@@ -2213,8 +2227,8 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="58"/>
-      <c r="B34" s="61"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="64"/>
       <c r="C34" s="5"/>
       <c r="D34" s="2" t="s">
         <v>80</v>
@@ -2237,8 +2251,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="58"/>
-      <c r="B35" s="61"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="64"/>
       <c r="C35" s="5"/>
       <c r="D35" s="2" t="s">
         <v>81</v>
@@ -2261,8 +2275,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="58"/>
-      <c r="B36" s="61"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8" t="s">
         <v>82</v>
@@ -2285,12 +2299,12 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="56" t="s">
+      <c r="A37" s="61"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="84"/>
+      <c r="D37" s="82"/>
       <c r="E37" s="11" t="s">
         <v>92</v>
       </c>
@@ -2311,8 +2325,8 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
-      <c r="B38" s="61"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="5"/>
       <c r="D38" s="2" t="s">
         <v>88</v>
@@ -2335,8 +2349,8 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="58"/>
-      <c r="B39" s="61"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
         <v>89</v>
@@ -2359,12 +2373,12 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="58"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="56" t="s">
+      <c r="A40" s="61"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="84"/>
+      <c r="D40" s="82"/>
       <c r="E40" s="11" t="s">
         <v>69</v>
       </c>
@@ -2385,8 +2399,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
-      <c r="B41" s="61"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="64"/>
       <c r="C41" s="5"/>
       <c r="D41" s="2" t="s">
         <v>90</v>
@@ -2408,8 +2422,8 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="58"/>
-      <c r="B42" s="61"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="64"/>
       <c r="C42" s="5"/>
       <c r="D42" s="2" t="s">
         <v>95</v>
@@ -2432,8 +2446,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="59"/>
-      <c r="B43" s="62"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="65"/>
       <c r="C43" s="5"/>
       <c r="D43" s="2" t="s">
         <v>96</v>
@@ -2456,169 +2470,316 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="79" t="s">
+      <c r="A44" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="81" t="s">
+      <c r="B44" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="85"/>
-      <c r="D44" s="86"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="44"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="83"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="19">
+        <f>SUM(G45)</f>
+        <v>38</v>
+      </c>
+      <c r="H44" s="41"/>
+      <c r="I44" s="42"/>
       <c r="K44" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="80"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="82"/>
+      <c r="E45" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="47">
+        <f>SUM(G46:G53)</f>
+        <v>38</v>
+      </c>
+      <c r="H45" s="47">
+        <f t="shared" ref="H45:I45" si="11">SUM(H46:H53)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="47">
+        <f t="shared" si="11"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="80"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="80"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
+      <c r="A46" s="61"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" s="2">
+        <v>2</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" ref="I46:I47" si="12">G46-H46</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="61"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G47" s="2">
+        <v>8</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="70"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
+      <c r="A48" s="61"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" s="2">
+        <v>4</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <f>G48-H48</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="61"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" s="8">
+        <v>12</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <f>G49-H49</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="61"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="8">
         <v>8</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <f>G50-H50</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="61"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="8">
+        <v>4</v>
+      </c>
+      <c r="H51" s="8">
+        <v>0</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" ref="I51" si="13">G51-H51</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="61"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="62"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="32" t="s">
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="32" t="s">
+      <c r="B55" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="71"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="38">
+    </row>
+    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="74"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="37">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H50" s="37"/>
-      <c r="I50" s="39"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="73" t="s">
+      <c r="H56" s="36"/>
+      <c r="I56" s="38"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="73"/>
+      <c r="B57" s="73"/>
+      <c r="C57" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="74"/>
-      <c r="E51" s="87" t="s">
+      <c r="D57" s="78"/>
+      <c r="E57" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="F51" s="87" t="s">
+      <c r="F57" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="87">
-        <v>0</v>
-      </c>
-      <c r="H51" s="87">
-        <f>SUM(H52:H55)</f>
-        <v>0</v>
-      </c>
-      <c r="I51" s="87">
-        <f>SUM(I52:I55)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="70"/>
-      <c r="B52" s="70"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="76"/>
-      <c r="I52" s="76"/>
-    </row>
-    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
+      <c r="G57" s="44">
+        <v>0</v>
+      </c>
+      <c r="H57" s="44">
+        <f>SUM(H58:H60)</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="44">
+        <f>SUM(I58:I60)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="32" t="s">
+      <c r="B58" s="31" t="s">
         <v>15</v>
       </c>
+      <c r="C58" s="79"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="I51:I52"/>
+  <mergeCells count="28">
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A22:A43"/>
     <mergeCell ref="B22:B43"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="B44:B53"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:D56"/>
     <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C57:D58"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2634,7 +2795,7 @@
     <mergeCell ref="C11:D11"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F50:F51 F4:F44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56:F57 F4:F52">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update plan + Add US8 and US9
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="115">
   <si>
     <t>11.09.18</t>
   </si>
@@ -330,12 +330,6 @@
     <t xml:space="preserve">[Continue] Backend Web Api </t>
   </si>
   <si>
-    <t>Method POST: Orders, ItemsOfOrders</t>
-  </si>
-  <si>
-    <t>Add POST method for Users</t>
-  </si>
-  <si>
     <t>Controllers: Products, Users, Orders, ItemsOfOrders
 Method GET: Products, Users, Orders, ItemsOfOrders</t>
   </si>
@@ -343,9 +337,6 @@
     <t>Add services+server side validation for all models</t>
   </si>
   <si>
-    <t>TA31</t>
-  </si>
-  <si>
     <t>TA32</t>
   </si>
   <si>
@@ -359,6 +350,30 @@
   </si>
   <si>
     <t>TA36</t>
+  </si>
+  <si>
+    <t>US9</t>
+  </si>
+  <si>
+    <t>[Continue] Frontend React/Redux</t>
+  </si>
+  <si>
+    <t>Create SPA with simple components for Cart</t>
+  </si>
+  <si>
+    <t>Method POST: Products, Users, Orders, ItemsOfOrders</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>TA37</t>
+  </si>
+  <si>
+    <t>TA38</t>
+  </si>
+  <si>
+    <t>TA39</t>
   </si>
 </sst>
 </file>
@@ -871,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1014,39 +1029,111 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1057,75 +1144,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1409,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U58"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,27 +1448,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="76" t="s">
+      <c r="A2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="77"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1468,14 +1486,14 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="82"/>
+      <c r="B3" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19">
@@ -1486,12 +1504,12 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="78" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1512,8 +1530,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>23</v>
@@ -1539,8 +1557,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -1566,8 +1584,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="56"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>27</v>
@@ -1593,8 +1611,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
         <v>31</v>
@@ -1620,8 +1638,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="57"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14" t="s">
         <v>37</v>
@@ -1644,14 +1662,14 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="83"/>
-      <c r="D10" s="84"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -1664,12 +1682,12 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="78" t="s">
+      <c r="A11" s="62"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="79"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1690,8 +1708,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>39</v>
@@ -1714,8 +1732,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="56"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>40</v>
@@ -1738,8 +1756,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>41</v>
@@ -1762,12 +1780,12 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="80" t="s">
+      <c r="A15" s="62"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="58"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="11" t="s">
         <v>52</v>
       </c>
@@ -1788,8 +1806,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2" t="s">
         <v>44</v>
@@ -1812,8 +1830,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="56"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>45</v>
@@ -1836,12 +1854,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="85" t="s">
+      <c r="A18" s="62"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="12" t="s">
         <v>53</v>
       </c>
@@ -1862,8 +1880,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="56"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>49</v>
@@ -1886,8 +1904,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="24"/>
       <c r="D20" s="2" t="s">
         <v>68</v>
@@ -1913,8 +1931,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
-      <c r="B21" s="56"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="25"/>
       <c r="D21" s="2" t="s">
         <v>50</v>
@@ -1936,30 +1954,30 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="55" t="s">
+      <c r="A22" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
       <c r="G22" s="30">
         <f>SUM(G23,G28,G37,G40)</f>
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="48" t="s">
+      <c r="A23" s="62"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="D23" s="77"/>
       <c r="E23" s="33" t="s">
         <v>76</v>
       </c>
@@ -1980,8 +1998,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="56"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
         <v>55</v>
@@ -2004,8 +2022,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="56"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>56</v>
@@ -2028,8 +2046,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="56"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
         <v>57</v>
@@ -2052,8 +2070,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="56"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
         <v>58</v>
@@ -2076,12 +2094,12 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="48" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="77"/>
       <c r="E28" s="12" t="s">
         <v>87</v>
       </c>
@@ -2102,8 +2120,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
         <v>59</v>
@@ -2126,8 +2144,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="5"/>
       <c r="D30" s="2" t="s">
         <v>65</v>
@@ -2149,8 +2167,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="56"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="65"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
         <v>70</v>
@@ -2172,12 +2190,12 @@
         <v>-12</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
         <v>77</v>
@@ -2199,13 +2217,13 @@
         <v>6</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
@@ -2227,9 +2245,9 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="5"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="2" t="s">
         <v>80</v>
       </c>
@@ -2251,9 +2269,9 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="5"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="2" t="s">
         <v>81</v>
       </c>
@@ -2275,9 +2293,9 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="62"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="8" t="s">
         <v>82</v>
       </c>
@@ -2299,12 +2317,12 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="58" t="s">
+      <c r="A37" s="62"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="59"/>
+      <c r="D37" s="83"/>
       <c r="E37" s="11" t="s">
         <v>92</v>
       </c>
@@ -2325,8 +2343,8 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
-      <c r="B38" s="56"/>
+      <c r="A38" s="62"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="5"/>
       <c r="D38" s="2" t="s">
         <v>88</v>
@@ -2349,8 +2367,8 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
-      <c r="B39" s="56"/>
+      <c r="A39" s="62"/>
+      <c r="B39" s="65"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
         <v>89</v>
@@ -2373,12 +2391,12 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="53"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="58" t="s">
+      <c r="A40" s="62"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="59"/>
+      <c r="D40" s="83"/>
       <c r="E40" s="11" t="s">
         <v>69</v>
       </c>
@@ -2387,116 +2405,118 @@
       </c>
       <c r="G40" s="11">
         <f>SUM(G41:G43)</f>
-        <v>36</v>
-      </c>
-      <c r="H40" s="11">
-        <f>SUM(H41:H43)</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
-        <f>SUM(I41:I43)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="H40" s="48">
+        <f t="shared" ref="H40:I40" si="9">SUM(H41:H43)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="48">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="62"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G41" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
       </c>
       <c r="I41" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="53"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="5"/>
+        <f t="shared" ref="I41" si="10">G41-H41</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="62"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G42" s="2">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" ref="I42" si="9">G42-H42</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="54"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="5"/>
+        <f t="shared" ref="I42" si="11">G42-H42</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="63"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G43" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" ref="I43" si="10">G43-H43</f>
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="52" t="s">
+      <c r="A44" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="60"/>
-      <c r="D44" s="61"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="85"/>
       <c r="E44" s="40"/>
       <c r="F44" s="41"/>
       <c r="G44" s="19">
-        <f>SUM(G45)</f>
-        <v>38</v>
-      </c>
-      <c r="H44" s="41"/>
+        <f>SUM(G45,G52)</f>
+        <v>56</v>
+      </c>
+      <c r="H44" s="41" t="s">
+        <v>111</v>
+      </c>
       <c r="I44" s="42"/>
       <c r="K44" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="62" t="s">
+      <c r="A45" s="62"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="59"/>
+      <c r="D45" s="83"/>
       <c r="E45" s="47" t="s">
         <v>99</v>
       </c>
@@ -2504,24 +2524,24 @@
         <v>33</v>
       </c>
       <c r="G45" s="47">
-        <f>SUM(G46:G53)</f>
-        <v>38</v>
-      </c>
-      <c r="H45" s="47">
-        <f t="shared" ref="H45:I45" si="11">SUM(H46:H53)</f>
-        <v>0</v>
-      </c>
-      <c r="I45" s="47">
-        <f t="shared" si="11"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="53"/>
-      <c r="B46" s="56"/>
+        <f>SUM(G46:G51)</f>
+        <v>36</v>
+      </c>
+      <c r="H45" s="48">
+        <f>SUM(H46:H51)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="48">
+        <f>SUM(I46:I51)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="62"/>
+      <c r="B46" s="65"/>
       <c r="C46" s="5"/>
       <c r="D46" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>101</v>
@@ -2530,241 +2550,381 @@
         <v>33</v>
       </c>
       <c r="G46" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" ref="I46:I47" si="12">G46-H46</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
-      <c r="B47" s="56"/>
+        <f t="shared" ref="I46" si="12">G46-H46</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="62"/>
+      <c r="B47" s="65"/>
       <c r="C47" s="5"/>
       <c r="D47" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F47" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G47" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H47" s="2">
         <v>0</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="12"/>
-        <v>8</v>
+        <f>G47-H47</f>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="53"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="62"/>
+      <c r="B48" s="65"/>
       <c r="C48" s="5"/>
       <c r="D48" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>60</v>
+        <v>104</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G48" s="2">
-        <v>4</v>
+      <c r="G48" s="8">
+        <v>12</v>
       </c>
       <c r="H48" s="2">
         <v>0</v>
       </c>
       <c r="I48" s="2">
         <f>G48-H48</f>
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="53"/>
-      <c r="B49" s="56"/>
+      <c r="A49" s="62"/>
+      <c r="B49" s="65"/>
       <c r="C49" s="5"/>
       <c r="D49" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G49" s="8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H49" s="2">
         <v>0</v>
       </c>
       <c r="I49" s="2">
         <f>G49-H49</f>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
-      <c r="B50" s="56"/>
+      <c r="A50" s="62"/>
+      <c r="B50" s="65"/>
       <c r="C50" s="5"/>
       <c r="D50" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="8">
+        <v>4</v>
+      </c>
+      <c r="H50" s="8">
+        <v>0</v>
+      </c>
+      <c r="I50" s="8">
+        <f t="shared" ref="I50" si="13">G50-H50</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="62"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="62"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="83"/>
+      <c r="E52" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F50" s="2" t="s">
+      <c r="F52" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" s="48">
+        <f>SUM(G53:G55)</f>
+        <v>20</v>
+      </c>
+      <c r="H52" s="48">
+        <f>SUM(H53:H55)</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="48">
+        <f>SUM(I53:I55)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="62"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G53" s="2">
         <v>8</v>
       </c>
-      <c r="H50" s="2">
-        <v>0</v>
-      </c>
-      <c r="I50" s="2">
-        <f>G50-H50</f>
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" ref="I53:I54" si="14">G53-H53</f>
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="53"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="2" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="62"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F51" s="8" t="s">
+      <c r="F54" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="8">
-        <v>4</v>
-      </c>
-      <c r="H51" s="8">
-        <v>0</v>
-      </c>
-      <c r="I51" s="8">
-        <f t="shared" ref="I51" si="13">G51-H51</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="53"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="54"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="45" t="s">
+      <c r="G54" s="2">
         <v>8</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="62"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G55" s="2">
+        <v>4</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="62"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="62"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="62"/>
+      <c r="B58" s="65"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="62"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="63"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="31" t="s">
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="39"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B62" s="31" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="63" t="s">
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="39"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="63" t="s">
+      <c r="B63" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="65"/>
-      <c r="D56" s="66"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="37">
+      <c r="C63" s="75"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="37">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H56" s="36"/>
-      <c r="I56" s="38"/>
-    </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="64"/>
-      <c r="B57" s="64"/>
-      <c r="C57" s="67" t="s">
+      <c r="H63" s="36"/>
+      <c r="I63" s="38"/>
+    </row>
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="74"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="D57" s="68"/>
-      <c r="E57" s="44" t="s">
+      <c r="D64" s="79"/>
+      <c r="E64" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="F57" s="44" t="s">
+      <c r="F64" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G57" s="44">
-        <v>0</v>
-      </c>
-      <c r="H57" s="44">
-        <f>SUM(H58:H60)</f>
-        <v>0</v>
-      </c>
-      <c r="I57" s="44">
-        <f>SUM(I58:I60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="31" t="s">
+      <c r="G64" s="44">
+        <v>0</v>
+      </c>
+      <c r="H64" s="44">
+        <f>SUM(H65:H67)</f>
+        <v>0</v>
+      </c>
+      <c r="I64" s="44">
+        <f>SUM(I65:I67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B65" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="69"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A22:A43"/>
+    <mergeCell ref="B22:B43"/>
+    <mergeCell ref="A44:A60"/>
+    <mergeCell ref="B44:B60"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C64:D65"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
@@ -2778,24 +2938,9 @@
     <mergeCell ref="B10:B21"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C57:D58"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A22:A43"/>
-    <mergeCell ref="B22:B43"/>
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="B44:B53"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56:F57 F4:F52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F63:F64 F4:F59">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update plan (add US11-US13 and Defects)
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6870"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
   <si>
     <t>11.09.18</t>
   </si>
@@ -385,9 +385,6 @@
     <t>Merge DB context files into one file</t>
   </si>
   <si>
-    <t>Fix path for IIS to js/main.*.js</t>
-  </si>
-  <si>
     <t>Functionality "add to cart/remove from cart"</t>
   </si>
   <si>
@@ -410,6 +407,57 @@
   </si>
   <si>
     <t>TA43</t>
+  </si>
+  <si>
+    <t>Fix path to js/main.*.js in ReactReduxApp and connect with IIS</t>
+  </si>
+  <si>
+    <t>US12</t>
+  </si>
+  <si>
+    <t>TA44</t>
+  </si>
+  <si>
+    <t>TA45</t>
+  </si>
+  <si>
+    <t>TA46</t>
+  </si>
+  <si>
+    <t>Fix re render of tab "Cart"</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>Security Issue</t>
+  </si>
+  <si>
+    <t>TA47</t>
+  </si>
+  <si>
+    <t>US13</t>
+  </si>
+  <si>
+    <t>Frontend html/css</t>
+  </si>
+  <si>
+    <t>Create UI for App component</t>
+  </si>
+  <si>
+    <t>TA48</t>
+  </si>
+  <si>
+    <t>Create UI for Products component</t>
+  </si>
+  <si>
+    <t>TA49</t>
+  </si>
+  <si>
+    <t>Create UI for Cart component</t>
+  </si>
+  <si>
+    <t>US14</t>
   </si>
 </sst>
 </file>
@@ -477,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -767,15 +815,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -788,17 +827,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -827,26 +855,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1045,6 +1053,41 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -1059,7 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1106,22 +1149,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1130,220 +1161,235 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1627,11 +1673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U69"/>
+  <dimension ref="A1:U84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,38 +1694,38 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="81" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82"/>
-      <c r="B1" s="83"/>
-      <c r="C1" s="82" t="s">
+    <row r="1" spans="1:21" s="44" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="84"/>
-      <c r="E1" s="85" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="85" t="s">
+      <c r="H1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="46" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
+      <c r="B2" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11">
@@ -1687,38 +1733,38 @@
         <v>28</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="72"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="73" t="s">
+      <c r="A3" s="55"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="26" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="20">
         <f>SUM(G4:G8)</f>
         <v>28</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="20">
         <f>SUM(H4:H8)</f>
         <v>20</v>
       </c>
-      <c r="I3" s="74">
+      <c r="I3" s="40">
         <f>SUM(I4:I8)</f>
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="68"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1734,7 +1780,7 @@
       <c r="H4" s="2">
         <v>4</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="26">
         <f>G4-H4</f>
         <v>4</v>
       </c>
@@ -1743,9 +1789,9 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="68"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1761,7 +1807,7 @@
       <c r="H5" s="2">
         <v>2</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="26">
         <f>G5-H5</f>
         <v>2</v>
       </c>
@@ -1770,9 +1816,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="69"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1788,7 +1834,7 @@
       <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="26">
         <f t="shared" ref="I6:I8" si="0">G6-H6</f>
         <v>2</v>
       </c>
@@ -1797,9 +1843,9 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="75"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1815,7 +1861,7 @@
       <c r="H7" s="4">
         <v>8</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1824,9 +1870,9 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="35"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
@@ -1842,19 +1888,19 @@
       <c r="H8" s="7">
         <v>4</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="76"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="63"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
@@ -1863,40 +1909,40 @@
         <v>38</v>
       </c>
       <c r="H9" s="13"/>
-      <c r="I9" s="77"/>
+      <c r="I9" s="42"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="73" t="s">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="26" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="20">
         <f>SUM(G11:G13)</f>
         <v>12</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="20">
         <f>SUM(H11:H15)</f>
         <v>36</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="40">
         <f>SUM(I11:I15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
@@ -1912,15 +1958,15 @@
       <c r="H11" s="2">
         <v>4</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="26">
         <f>G11-H11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="32"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1936,15 +1982,15 @@
       <c r="H12" s="2">
         <v>4</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="26">
         <f>G12-H12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="70"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
@@ -1960,41 +2006,41 @@
       <c r="H13" s="2">
         <v>4</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="26">
         <f>G13-H13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="78" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="29" t="s">
+      <c r="D14" s="53"/>
+      <c r="E14" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="23">
         <f>SUM(G15:G16)</f>
         <v>16</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="23">
         <f>SUM(H15:H16)</f>
         <v>16</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="24">
         <f>SUM(I15:I16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="32"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
@@ -2010,15 +2056,15 @@
       <c r="H15" s="2">
         <v>8</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="26">
         <f>G15-H15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="32"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
@@ -2034,41 +2080,41 @@
       <c r="H16" s="2">
         <v>8</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="26">
         <f>G16-H16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="79" t="s">
+      <c r="A17" s="55"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="27" t="s">
+      <c r="D17" s="65"/>
+      <c r="E17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="21">
         <f>SUM(G18:G20)</f>
         <v>10</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="21">
         <f t="shared" ref="H17:I17" si="1">SUM(H18:H20)</f>
         <v>3</v>
       </c>
-      <c r="I17" s="67">
+      <c r="I17" s="34">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="2" t="s">
         <v>47</v>
       </c>
@@ -2084,15 +2130,15 @@
       <c r="H18" s="2">
         <v>2</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="26">
         <f>G18-H18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="68"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="2" t="s">
         <v>66</v>
       </c>
@@ -2108,7 +2154,7 @@
       <c r="H19" s="2">
         <v>1</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="26">
         <f>G19-H19</f>
         <v>3</v>
       </c>
@@ -2117,16 +2163,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="71"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="80" t="s">
+      <c r="F20" s="43" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="7">
@@ -2135,58 +2181,58 @@
       <c r="H20" s="7">
         <v>0</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="29">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="45" t="s">
+      <c r="A21" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="41"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="28"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="17">
         <f>SUM(G22,G27,G36,G39)</f>
         <v>76</v>
       </c>
       <c r="H21" s="17"/>
-      <c r="I21" s="65"/>
+      <c r="I21" s="33"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="46"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="27" t="s">
+      <c r="D22" s="67"/>
+      <c r="E22" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="21">
         <f>SUM(G23:G26)</f>
         <v>6</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="21">
         <f t="shared" ref="H22:I22" si="2">SUM(H23:H26)</f>
         <v>3.25</v>
       </c>
-      <c r="I22" s="67">
+      <c r="I22" s="34">
         <f t="shared" si="2"/>
         <v>2.75</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="32"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
@@ -2202,15 +2248,15 @@
       <c r="H23" s="2">
         <v>1</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I23" s="26">
         <f>G23-H23</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="32"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="2" t="s">
         <v>54</v>
       </c>
@@ -2226,15 +2272,15 @@
       <c r="H24" s="2">
         <v>1</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I24" s="26">
         <f>G24-H24</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="32"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2250,15 +2296,15 @@
       <c r="H25" s="2">
         <v>1</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="26">
         <f>G25-H25</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="32"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="2" t="s">
         <v>56</v>
       </c>
@@ -2274,41 +2320,41 @@
       <c r="H26" s="2">
         <v>0.25</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="26">
         <f>G26-H26</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="46"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="40"/>
-      <c r="E27" s="27" t="s">
+      <c r="D27" s="67"/>
+      <c r="E27" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="21">
         <f>SUM(G28:G35)</f>
         <v>46</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="21">
         <f ca="1">SUM(H25:H35)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="67">
+      <c r="I27" s="34">
         <f ca="1">SUM(I25:I35)</f>
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="32"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="2" t="s">
         <v>57</v>
       </c>
@@ -2324,15 +2370,15 @@
       <c r="H28" s="2">
         <v>2</v>
       </c>
-      <c r="I28" s="33">
+      <c r="I28" s="26">
         <f>G28-H28</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="32"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="2" t="s">
         <v>63</v>
       </c>
@@ -2348,14 +2394,14 @@
       <c r="H29" s="4">
         <v>4</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="32"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="2" t="s">
         <v>68</v>
       </c>
@@ -2371,7 +2417,7 @@
       <c r="H30" s="2">
         <v>16</v>
       </c>
-      <c r="I30" s="33">
+      <c r="I30" s="26">
         <f t="shared" ref="I30" si="3">G30-H30</f>
         <v>-12</v>
       </c>
@@ -2380,9 +2426,9 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="32"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="2" t="s">
         <v>75</v>
       </c>
@@ -2398,7 +2444,7 @@
       <c r="H31" s="2">
         <v>2</v>
       </c>
-      <c r="I31" s="33">
+      <c r="I31" s="26">
         <f t="shared" ref="I31" si="4">G31-H31</f>
         <v>6</v>
       </c>
@@ -2407,9 +2453,9 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="68"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="2" t="s">
         <v>76</v>
       </c>
@@ -2425,15 +2471,15 @@
       <c r="H32" s="2">
         <v>0</v>
       </c>
-      <c r="I32" s="33">
+      <c r="I32" s="26">
         <f>G32-H32</f>
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="68"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="55"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
@@ -2449,15 +2495,15 @@
       <c r="H33" s="2">
         <v>0</v>
       </c>
-      <c r="I33" s="33">
+      <c r="I33" s="26">
         <f>G33-H33</f>
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="68"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="55"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="35"/>
       <c r="D34" s="2" t="s">
         <v>79</v>
       </c>
@@ -2473,15 +2519,15 @@
       <c r="H34" s="2">
         <v>0</v>
       </c>
-      <c r="I34" s="33">
+      <c r="I34" s="26">
         <f>G34-H34</f>
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="69"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="4" t="s">
         <v>80</v>
       </c>
@@ -2497,41 +2543,41 @@
       <c r="H35" s="4">
         <v>0</v>
       </c>
-      <c r="I35" s="34">
+      <c r="I35" s="27">
         <f t="shared" ref="I35" si="5">G35-H35</f>
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="46"/>
-      <c r="C36" s="52" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="55"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="49"/>
-      <c r="E36" s="29" t="s">
+      <c r="D36" s="76"/>
+      <c r="E36" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F36" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="23">
         <f>SUM(G37:G38)</f>
         <v>4</v>
       </c>
-      <c r="H36" s="29">
+      <c r="H36" s="23">
         <f t="shared" ref="H36:I36" si="6">SUM(H37:H38)</f>
         <v>1</v>
       </c>
-      <c r="I36" s="31">
+      <c r="I36" s="24">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="32"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="55"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="2" t="s">
         <v>86</v>
       </c>
@@ -2547,15 +2593,15 @@
       <c r="H37" s="2">
         <v>0.5</v>
       </c>
-      <c r="I37" s="33">
+      <c r="I37" s="26">
         <f t="shared" ref="I37" si="7">G37-H37</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="70"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="55"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="4" t="s">
         <v>87</v>
       </c>
@@ -2571,41 +2617,41 @@
       <c r="H38" s="4">
         <v>0.5</v>
       </c>
-      <c r="I38" s="34">
+      <c r="I38" s="27">
         <f t="shared" ref="I38" si="8">G38-H38</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="52" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="29" t="s">
+      <c r="D39" s="76"/>
+      <c r="E39" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="29" t="s">
+      <c r="F39" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="29">
+      <c r="G39" s="23">
         <f>SUM(G40:G42)</f>
         <v>20</v>
       </c>
-      <c r="H39" s="29">
+      <c r="H39" s="23">
         <f t="shared" ref="H39:I39" si="9">SUM(H40:H42)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="31">
+      <c r="I39" s="24">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="68"/>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="55"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="2" t="s">
         <v>93</v>
       </c>
@@ -2621,15 +2667,15 @@
       <c r="H40" s="2">
         <v>0</v>
       </c>
-      <c r="I40" s="33">
+      <c r="I40" s="26">
         <f t="shared" ref="I40" si="10">G40-H40</f>
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="68"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="55"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="2" t="s">
         <v>94</v>
       </c>
@@ -2645,15 +2691,15 @@
       <c r="H41" s="2">
         <v>0</v>
       </c>
-      <c r="I41" s="33">
+      <c r="I41" s="26">
         <f t="shared" ref="I41" si="11">G41-H41</f>
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
-      <c r="B42" s="47"/>
-      <c r="C42" s="71"/>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="56"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="7" t="s">
         <v>88</v>
       </c>
@@ -2669,69 +2715,66 @@
       <c r="H42" s="7">
         <v>0</v>
       </c>
-      <c r="I42" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="42" t="s">
+      <c r="I42" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="50"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="30"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="32"/>
       <c r="G43" s="11">
         <f>SUM(G44,G46)</f>
         <v>48.5</v>
       </c>
       <c r="H43" s="11">
         <f>SUM(H44,H46,H53)</f>
-        <v>24</v>
-      </c>
-      <c r="I43" s="23"/>
-      <c r="K43" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="55"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="29" t="s">
+      <c r="D44" s="76"/>
+      <c r="E44" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F44" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="29">
+      <c r="G44" s="31">
         <f>SUM(G45:G45)</f>
         <v>8</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H44" s="31">
         <f t="shared" ref="H44:I44" si="12">SUM(H45:H45)</f>
         <v>0</v>
       </c>
-      <c r="I44" s="29">
+      <c r="I44" s="24">
         <f t="shared" si="12"/>
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
-      <c r="B45" s="54"/>
-      <c r="C45" s="32"/>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="55"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>31</v>
@@ -2742,41 +2785,41 @@
       <c r="H45" s="2">
         <v>0</v>
       </c>
-      <c r="I45" s="33">
+      <c r="I45" s="26">
         <f>G45-H45</f>
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="52" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="55"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="29" t="s">
+      <c r="D46" s="76"/>
+      <c r="E46" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="29" t="s">
+      <c r="F46" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="31">
         <f>SUM(G47:G54)</f>
         <v>40.5</v>
       </c>
-      <c r="H46" s="29">
+      <c r="H46" s="31">
         <f>SUM(H47:H54)</f>
-        <v>21.5</v>
-      </c>
-      <c r="I46" s="31">
+        <v>37.5</v>
+      </c>
+      <c r="I46" s="24">
         <f>SUM(I47:I54)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="32"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="55"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="25"/>
       <c r="D47" s="2" t="s">
         <v>101</v>
       </c>
@@ -2792,15 +2835,15 @@
       <c r="H47" s="2">
         <v>8</v>
       </c>
-      <c r="I47" s="33">
-        <f t="shared" ref="I47:I50" si="13">G47-H47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="32"/>
+      <c r="I47" s="26">
+        <f t="shared" ref="I47:I52" si="13">G47-H47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="55"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="25"/>
       <c r="D48" s="2" t="s">
         <v>102</v>
       </c>
@@ -2808,23 +2851,23 @@
         <v>107</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G48" s="2">
         <v>8</v>
       </c>
       <c r="H48" s="2">
-        <v>5</v>
-      </c>
-      <c r="I48" s="33">
+        <v>8</v>
+      </c>
+      <c r="I48" s="26">
         <f t="shared" si="13"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="70"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="55"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="2" t="s">
         <v>103</v>
       </c>
@@ -2840,66 +2883,69 @@
       <c r="H49" s="2">
         <v>4</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="54"/>
-      <c r="C50" s="75"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="55"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="41"/>
       <c r="D50" s="2" t="s">
         <v>104</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G50" s="2">
         <v>4</v>
       </c>
       <c r="H50" s="2">
-        <v>0</v>
-      </c>
-      <c r="I50" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="43"/>
-      <c r="B51" s="54"/>
-      <c r="C51" s="75"/>
+        <v>5</v>
+      </c>
+      <c r="I50" s="26">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
+      <c r="J50" s="80"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="55"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="81"/>
       <c r="D51" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G51" s="2">
         <v>4</v>
       </c>
       <c r="H51" s="2">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
-      <c r="B52" s="54"/>
-      <c r="C52" s="75"/>
+        <v>2</v>
+      </c>
+      <c r="I51" s="26">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="55"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="81"/>
       <c r="D52" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>31</v>
@@ -2910,133 +2956,134 @@
       <c r="H52" s="2">
         <v>0</v>
       </c>
-      <c r="I52" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="43"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="29" t="s">
+      <c r="I52" s="26">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="55"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="29">
+      <c r="F53" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G53" s="31">
         <f>SUM(G54:G55)</f>
         <v>4.5</v>
       </c>
-      <c r="H53" s="29">
+      <c r="H53" s="31">
         <f>SUM(H54:H55)</f>
-        <v>2.5</v>
-      </c>
-      <c r="I53" s="29">
+        <v>5.5</v>
+      </c>
+      <c r="I53" s="24">
         <f>SUM(I54:I55)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="43"/>
-      <c r="B54" s="87"/>
-      <c r="C54" s="93"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="55"/>
+      <c r="B54" s="77"/>
+      <c r="C54" s="25"/>
       <c r="D54" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G54" s="2">
         <v>4</v>
       </c>
       <c r="H54" s="2">
-        <v>2</v>
-      </c>
-      <c r="I54" s="2">
+        <v>5</v>
+      </c>
+      <c r="I54" s="26">
         <f>G54-H54</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="43"/>
-      <c r="B55" s="87"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="2" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="55"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="7">
         <v>0.5</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="7">
         <v>0.5</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="29">
         <f>G55-H55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="89" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="50"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="30"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="32"/>
       <c r="G56" s="11">
-        <f>SUM(G57,G64)</f>
-        <v>36</v>
+        <f>SUM(G57,G64,G67)</f>
+        <v>61</v>
       </c>
       <c r="H56" s="11">
-        <f>SUM(H57,H67)</f>
-        <v>0</v>
-      </c>
-      <c r="I56" s="23"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
-      <c r="B57" s="90"/>
-      <c r="C57" s="52" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="49"/>
-      <c r="E57" s="29" t="s">
+        <f>SUM(H57,H64,J59)</f>
+        <v>34</v>
+      </c>
+      <c r="I56" s="19"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="69"/>
+      <c r="C57" s="75" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="76"/>
+      <c r="E57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="F57" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G57" s="29">
-        <f>SUM(G58:G66)</f>
-        <v>36</v>
-      </c>
-      <c r="H57" s="29">
-        <f t="shared" ref="H57:I57" si="14">SUM(H58:H66)</f>
-        <v>0</v>
-      </c>
-      <c r="I57" s="29">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="43"/>
-      <c r="B58" s="90"/>
-      <c r="C58" s="32"/>
+      <c r="G57" s="31">
+        <f>SUM(G58:G63)</f>
+        <v>44</v>
+      </c>
+      <c r="H57" s="31">
+        <f>SUM(H58:H81)</f>
+        <v>28</v>
+      </c>
+      <c r="I57" s="24">
+        <f>SUM(I58:I81)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="55"/>
+      <c r="B58" s="69"/>
+      <c r="C58" s="25"/>
       <c r="D58" s="2" t="s">
         <v>111</v>
       </c>
@@ -3052,15 +3099,15 @@
       <c r="H58" s="2">
         <v>0</v>
       </c>
-      <c r="I58" s="33">
+      <c r="I58" s="26">
         <f>G58-H58</f>
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="43"/>
-      <c r="B59" s="90"/>
-      <c r="C59" s="32"/>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="55"/>
+      <c r="B59" s="69"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="2" t="s">
         <v>113</v>
       </c>
@@ -3076,17 +3123,17 @@
       <c r="H59" s="2">
         <v>0</v>
       </c>
-      <c r="I59" s="33">
+      <c r="I59" s="26">
         <f>G59-H59</f>
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
-      <c r="B60" s="90"/>
-      <c r="C60" s="32"/>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="55"/>
+      <c r="B60" s="69"/>
+      <c r="C60" s="25"/>
       <c r="D60" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E60" s="15" t="s">
         <v>61</v>
@@ -3100,17 +3147,17 @@
       <c r="H60" s="2">
         <v>0</v>
       </c>
-      <c r="I60" s="33">
+      <c r="I60" s="26">
         <f>G60-H60</f>
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="43"/>
-      <c r="B61" s="90"/>
-      <c r="C61" s="32"/>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="55"/>
+      <c r="B61" s="69"/>
+      <c r="C61" s="25"/>
       <c r="D61" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E61" s="15" t="s">
         <v>62</v>
@@ -3124,17 +3171,17 @@
       <c r="H61" s="2">
         <v>0</v>
       </c>
-      <c r="I61" s="33">
+      <c r="I61" s="26">
         <f>G61-H61</f>
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="43"/>
-      <c r="B62" s="90"/>
-      <c r="C62" s="93"/>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="55"/>
+      <c r="B62" s="69"/>
+      <c r="C62" s="25"/>
       <c r="D62" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>59</v>
@@ -3148,119 +3195,543 @@
       <c r="H62" s="4">
         <v>0</v>
       </c>
-      <c r="I62" s="34">
-        <f t="shared" ref="I62" si="15">G62-H62</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
-      <c r="B63" s="90"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="93"/>
-      <c r="F63" s="93"/>
-      <c r="G63" s="93"/>
-      <c r="H63" s="93"/>
-      <c r="I63" s="93"/>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="44"/>
-      <c r="B64" s="91"/>
-      <c r="C64" s="93"/>
-      <c r="D64" s="93"/>
-      <c r="E64" s="93"/>
-      <c r="F64" s="93"/>
-      <c r="G64" s="93"/>
-      <c r="H64" s="93"/>
-      <c r="I64" s="93"/>
+      <c r="I62" s="27">
+        <f t="shared" ref="I62" si="14">G62-H62</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="55"/>
+      <c r="B63" s="69"/>
+      <c r="C63" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" s="2">
+        <v>8</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63" s="26">
+        <f>G63-H63</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="55"/>
+      <c r="B64" s="69"/>
+      <c r="C64" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="76"/>
+      <c r="E64" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G64" s="31">
+        <f>SUM(G65:G66)</f>
+        <v>8</v>
+      </c>
+      <c r="H64" s="31">
+        <f t="shared" ref="H64:I64" si="15">SUM(H65:H66)</f>
+        <v>6</v>
+      </c>
+      <c r="I64" s="24">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="42" t="s">
+      <c r="A65" s="55"/>
+      <c r="B65" s="69"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G65" s="2">
+        <v>4</v>
+      </c>
+      <c r="H65" s="2">
+        <v>4</v>
+      </c>
+      <c r="I65" s="26">
+        <f t="shared" ref="I65:I66" si="16">G65-H65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="55"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G66" s="2">
+        <v>4</v>
+      </c>
+      <c r="H66" s="2">
+        <v>2</v>
+      </c>
+      <c r="I66" s="26">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="55"/>
+      <c r="B67" s="69"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" s="31">
+        <f>SUM(G68:G69)</f>
+        <v>9</v>
+      </c>
+      <c r="H67" s="31">
+        <f t="shared" ref="H67:I67" si="17">SUM(H68:H69)</f>
+        <v>8</v>
+      </c>
+      <c r="I67" s="24">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="55"/>
+      <c r="B68" s="69"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G68" s="2">
+        <v>4</v>
+      </c>
+      <c r="H68" s="2">
+        <v>8</v>
+      </c>
+      <c r="I68" s="26">
+        <f>G68-H68</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="55"/>
+      <c r="B69" s="69"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69" s="2">
+        <v>5</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0</v>
+      </c>
+      <c r="I69" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="55"/>
+      <c r="B70" s="69"/>
+      <c r="C70" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="53"/>
+      <c r="E70" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G70" s="31">
+        <f>SUM(G71:G73)</f>
+        <v>24</v>
+      </c>
+      <c r="H70" s="31">
+        <f t="shared" ref="H70" si="18">SUM(H71:H74)</f>
+        <v>0</v>
+      </c>
+      <c r="I70" s="24">
+        <f t="shared" ref="I70" si="19">SUM(I71:I74)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="55"/>
+      <c r="B71" s="69"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" s="2">
+        <v>8</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0</v>
+      </c>
+      <c r="I71" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="55"/>
+      <c r="B72" s="69"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E72" s="82" t="s">
+        <v>139</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" s="2">
+        <v>8</v>
+      </c>
+      <c r="H72" s="2">
+        <v>0</v>
+      </c>
+      <c r="I72" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="56"/>
+      <c r="B73" s="70"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E73" s="83" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G73" s="7">
+        <v>8</v>
+      </c>
+      <c r="H73" s="7">
+        <v>0</v>
+      </c>
+      <c r="I73" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="92" t="s">
+      <c r="B74" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="93"/>
-      <c r="D65" s="93"/>
-      <c r="E65" s="93"/>
-      <c r="F65" s="93"/>
-      <c r="G65" s="93"/>
-      <c r="H65" s="93"/>
-      <c r="I65" s="93"/>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="44"/>
-      <c r="B66" s="88"/>
-      <c r="C66" s="93"/>
-      <c r="D66" s="93"/>
-      <c r="E66" s="93"/>
-      <c r="F66" s="93"/>
-      <c r="G66" s="93"/>
-      <c r="H66" s="93"/>
-      <c r="I66" s="93"/>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="42" t="s">
+      <c r="C74" s="73"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="11">
+        <f>SUM(G75)</f>
+        <v>36</v>
+      </c>
+      <c r="H74" s="11">
+        <f>SUM(H75,H82,J77)</f>
+        <v>0</v>
+      </c>
+      <c r="I74" s="19"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="55"/>
+      <c r="B75" s="77"/>
+      <c r="C75" s="75" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" s="76"/>
+      <c r="E75" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G75" s="31">
+        <f>SUM(G76:G81)</f>
+        <v>36</v>
+      </c>
+      <c r="H75" s="31">
+        <f>SUM(H76:H99)</f>
+        <v>0</v>
+      </c>
+      <c r="I75" s="24">
+        <f>SUM(I76:I99)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="55"/>
+      <c r="B76" s="77"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G76" s="2">
+        <v>8</v>
+      </c>
+      <c r="H76" s="2">
+        <v>0</v>
+      </c>
+      <c r="I76" s="26">
+        <f>G76-H76</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="55"/>
+      <c r="B77" s="77"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" s="2">
+        <v>4</v>
+      </c>
+      <c r="H77" s="2">
+        <v>0</v>
+      </c>
+      <c r="I77" s="26">
+        <f>G77-H77</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="55"/>
+      <c r="B78" s="77"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G78" s="4">
         <v>12</v>
       </c>
-      <c r="B67" s="45" t="s">
+      <c r="H78" s="2">
+        <v>0</v>
+      </c>
+      <c r="I78" s="26">
+        <f>G78-H78</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="55"/>
+      <c r="B79" s="77"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G79" s="4">
+        <v>8</v>
+      </c>
+      <c r="H79" s="2">
+        <v>0</v>
+      </c>
+      <c r="I79" s="26">
+        <f>G79-H79</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="55"/>
+      <c r="B80" s="77"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E80" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G80" s="4">
+        <v>4</v>
+      </c>
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+      <c r="I80" s="27">
+        <f t="shared" ref="I80" si="20">G80-H80</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="56"/>
+      <c r="B81" s="72"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="93"/>
+      <c r="E81" s="93"/>
+      <c r="F81" s="93"/>
+      <c r="G81" s="93"/>
+      <c r="H81" s="93"/>
+      <c r="I81" s="94"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="55"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="20">
+      <c r="C82" s="73"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="32"/>
+      <c r="G82" s="11">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H67" s="19"/>
-      <c r="I67" s="21"/>
-    </row>
-    <row r="68" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="44"/>
-      <c r="B68" s="47"/>
-      <c r="C68" s="57" t="s">
+      <c r="H82" s="32"/>
+      <c r="I82" s="19"/>
+    </row>
+    <row r="83" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="56"/>
+      <c r="B83" s="70"/>
+      <c r="C83" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="D68" s="58"/>
-      <c r="E68" s="25" t="s">
+      <c r="D83" s="90"/>
+      <c r="E83" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F83" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="G68" s="25">
-        <v>0</v>
-      </c>
-      <c r="H68" s="25">
-        <f>SUM(H59:H63)</f>
-        <v>0</v>
-      </c>
-      <c r="I68" s="25">
-        <f>SUM(I59:I63)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="37" t="s">
+      <c r="G83" s="91">
+        <v>0</v>
+      </c>
+      <c r="H83" s="91">
+        <f>SUM(0)</f>
+        <v>0</v>
+      </c>
+      <c r="I83" s="92">
+        <f>SUM(0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B69" s="38" t="s">
+      <c r="B84" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="59"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
+      <c r="C84" s="85"/>
+      <c r="D84" s="86"/>
+      <c r="E84" s="87"/>
+      <c r="F84" s="87"/>
+      <c r="G84" s="87"/>
+      <c r="H84" s="87"/>
+      <c r="I84" s="88"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="40">
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A56:A73"/>
+    <mergeCell ref="B56:B73"/>
+    <mergeCell ref="A43:A55"/>
+    <mergeCell ref="B43:B55"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A21:A42"/>
+    <mergeCell ref="B21:B42"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C83:D84"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C3:D3"/>
@@ -3273,32 +3744,9 @@
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="B56:B64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A43:A55"/>
-    <mergeCell ref="B43:B55"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A21:A42"/>
-    <mergeCell ref="B21:B42"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F67:F68 F3:F62">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F82:F83 F3:F80">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update plan (add US14, update defect`s and tasks status)
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="151">
   <si>
     <t>11.09.18</t>
   </si>
@@ -458,6 +458,30 @@
   </si>
   <si>
     <t>US14</t>
+  </si>
+  <si>
+    <t>TA50</t>
+  </si>
+  <si>
+    <t>TA51</t>
+  </si>
+  <si>
+    <t>TA52</t>
+  </si>
+  <si>
+    <t>TA53</t>
+  </si>
+  <si>
+    <t>TA54</t>
+  </si>
+  <si>
+    <t>1 action</t>
+  </si>
+  <si>
+    <t>TA55</t>
+  </si>
+  <si>
+    <t>[Continue] Frontend html/css</t>
   </si>
 </sst>
 </file>
@@ -488,7 +512,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,8 +548,14 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="45">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1023,15 +1053,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1091,6 +1112,37 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1102,7 +1154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1245,108 +1297,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1359,37 +1309,151 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1673,11 +1737,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U84"/>
+  <dimension ref="A1:U87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J69" sqref="J69"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,12 +1759,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="44" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="47" t="s">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="49"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="45" t="s">
         <v>17</v>
       </c>
@@ -1718,14 +1782,14 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="61"/>
+      <c r="B2" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="72"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11">
@@ -1736,12 +1800,12 @@
       <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="66"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="20" t="s">
         <v>19</v>
       </c>
@@ -1762,8 +1826,8 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="35"/>
       <c r="D4" s="2" t="s">
         <v>22</v>
@@ -1789,8 +1853,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="35"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
@@ -1816,8 +1880,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="36"/>
       <c r="D6" s="4" t="s">
         <v>26</v>
@@ -1843,8 +1907,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="41"/>
       <c r="D7" s="4" t="s">
         <v>29</v>
@@ -1870,8 +1934,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
-      <c r="B8" s="59"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="28"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
@@ -1894,14 +1958,14 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14">
@@ -1914,12 +1978,12 @@
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="50" t="s">
+      <c r="A10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="20" t="s">
         <v>19</v>
       </c>
@@ -1940,8 +2004,8 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="58"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="25"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -1964,8 +2028,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
-      <c r="B12" s="58"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="25"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
@@ -1988,8 +2052,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
-      <c r="B13" s="58"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="37"/>
       <c r="D13" s="4" t="s">
         <v>39</v>
@@ -2012,12 +2076,12 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="52" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="53"/>
+      <c r="D14" s="64"/>
       <c r="E14" s="23" t="s">
         <v>50</v>
       </c>
@@ -2038,8 +2102,8 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="58"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="25"/>
       <c r="D15" s="2" t="s">
         <v>42</v>
@@ -2062,8 +2126,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="58"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="25"/>
       <c r="D16" s="2" t="s">
         <v>43</v>
@@ -2086,12 +2150,12 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="64" t="s">
+      <c r="A17" s="66"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="65"/>
+      <c r="D17" s="76"/>
       <c r="E17" s="21" t="s">
         <v>51</v>
       </c>
@@ -2112,8 +2176,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="58"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="69"/>
       <c r="C18" s="25"/>
       <c r="D18" s="2" t="s">
         <v>47</v>
@@ -2136,8 +2200,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="58"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="69"/>
       <c r="C19" s="35"/>
       <c r="D19" s="2" t="s">
         <v>66</v>
@@ -2163,8 +2227,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="55"/>
-      <c r="B20" s="58"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="69"/>
       <c r="C20" s="38"/>
       <c r="D20" s="7" t="s">
         <v>48</v>
@@ -2186,14 +2250,14 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="57" t="s">
+      <c r="A21" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="78"/>
-      <c r="D21" s="79"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="78"/>
       <c r="E21" s="16"/>
       <c r="F21" s="22"/>
       <c r="G21" s="17">
@@ -2204,12 +2268,12 @@
       <c r="I21" s="33"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="66" t="s">
+      <c r="A22" s="66"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="67"/>
+      <c r="D22" s="86"/>
       <c r="E22" s="21" t="s">
         <v>74</v>
       </c>
@@ -2230,8 +2294,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="58"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="69"/>
       <c r="C23" s="25"/>
       <c r="D23" s="2" t="s">
         <v>53</v>
@@ -2254,8 +2318,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
-      <c r="B24" s="58"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="69"/>
       <c r="C24" s="25"/>
       <c r="D24" s="2" t="s">
         <v>54</v>
@@ -2278,8 +2342,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="69"/>
       <c r="C25" s="25"/>
       <c r="D25" s="2" t="s">
         <v>55</v>
@@ -2302,8 +2366,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
-      <c r="B26" s="58"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="69"/>
       <c r="C26" s="25"/>
       <c r="D26" s="2" t="s">
         <v>56</v>
@@ -2326,12 +2390,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="66" t="s">
+      <c r="A27" s="66"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="67"/>
+      <c r="D27" s="86"/>
       <c r="E27" s="21" t="s">
         <v>85</v>
       </c>
@@ -2352,8 +2416,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="58"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="69"/>
       <c r="C28" s="25"/>
       <c r="D28" s="2" t="s">
         <v>57</v>
@@ -2376,8 +2440,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="58"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="25"/>
       <c r="D29" s="2" t="s">
         <v>63</v>
@@ -2399,8 +2463,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="58"/>
+      <c r="A30" s="66"/>
+      <c r="B30" s="69"/>
       <c r="C30" s="25"/>
       <c r="D30" s="2" t="s">
         <v>68</v>
@@ -2426,8 +2490,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="58"/>
+      <c r="A31" s="66"/>
+      <c r="B31" s="69"/>
       <c r="C31" s="25"/>
       <c r="D31" s="2" t="s">
         <v>75</v>
@@ -2453,8 +2517,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
-      <c r="B32" s="58"/>
+      <c r="A32" s="66"/>
+      <c r="B32" s="69"/>
       <c r="C32" s="35"/>
       <c r="D32" s="2" t="s">
         <v>76</v>
@@ -2477,8 +2541,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
-      <c r="B33" s="58"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="69"/>
       <c r="C33" s="35"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
@@ -2501,8 +2565,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
-      <c r="B34" s="58"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="69"/>
       <c r="C34" s="35"/>
       <c r="D34" s="2" t="s">
         <v>79</v>
@@ -2525,8 +2589,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
-      <c r="B35" s="58"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="69"/>
       <c r="C35" s="36"/>
       <c r="D35" s="4" t="s">
         <v>80</v>
@@ -2549,12 +2613,12 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="75" t="s">
+      <c r="A36" s="66"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="76"/>
+      <c r="D36" s="80"/>
       <c r="E36" s="23" t="s">
         <v>90</v>
       </c>
@@ -2575,8 +2639,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
-      <c r="B37" s="58"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="69"/>
       <c r="C37" s="25"/>
       <c r="D37" s="2" t="s">
         <v>86</v>
@@ -2599,8 +2663,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="55"/>
-      <c r="B38" s="58"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="69"/>
       <c r="C38" s="37"/>
       <c r="D38" s="4" t="s">
         <v>87</v>
@@ -2623,12 +2687,12 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="75" t="s">
+      <c r="A39" s="66"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="76"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="23" t="s">
         <v>67</v>
       </c>
@@ -2649,8 +2713,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="55"/>
-      <c r="B40" s="58"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="69"/>
       <c r="C40" s="35"/>
       <c r="D40" s="2" t="s">
         <v>93</v>
@@ -2673,8 +2737,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
-      <c r="B41" s="58"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="69"/>
       <c r="C41" s="35"/>
       <c r="D41" s="2" t="s">
         <v>94</v>
@@ -2697,8 +2761,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="56"/>
-      <c r="B42" s="59"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="70"/>
       <c r="C42" s="38"/>
       <c r="D42" s="7" t="s">
         <v>88</v>
@@ -2720,14 +2784,14 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="54" t="s">
+      <c r="A43" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="71" t="s">
+      <c r="B43" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="73"/>
-      <c r="D43" s="74"/>
+      <c r="C43" s="83"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="18"/>
       <c r="F43" s="32"/>
       <c r="G43" s="11">
@@ -2741,12 +2805,12 @@
       <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
-      <c r="B44" s="77"/>
-      <c r="C44" s="75" t="s">
+      <c r="A44" s="66"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="76"/>
+      <c r="D44" s="80"/>
       <c r="E44" s="31" t="s">
         <v>97</v>
       </c>
@@ -2767,8 +2831,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
-      <c r="B45" s="77"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="92"/>
       <c r="C45" s="35"/>
       <c r="D45" s="2" t="s">
         <v>100</v>
@@ -2791,12 +2855,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
-      <c r="B46" s="77"/>
-      <c r="C46" s="75" t="s">
+      <c r="A46" s="66"/>
+      <c r="B46" s="92"/>
+      <c r="C46" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="76"/>
+      <c r="D46" s="80"/>
       <c r="E46" s="31" t="s">
         <v>106</v>
       </c>
@@ -2817,8 +2881,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="55"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="66"/>
+      <c r="B47" s="92"/>
       <c r="C47" s="25"/>
       <c r="D47" s="2" t="s">
         <v>101</v>
@@ -2841,8 +2905,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="55"/>
-      <c r="B48" s="77"/>
+      <c r="A48" s="66"/>
+      <c r="B48" s="92"/>
       <c r="C48" s="25"/>
       <c r="D48" s="2" t="s">
         <v>102</v>
@@ -2865,8 +2929,8 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="92"/>
       <c r="C49" s="37"/>
       <c r="D49" s="2" t="s">
         <v>103</v>
@@ -2889,8 +2953,8 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="55"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="92"/>
       <c r="C50" s="41"/>
       <c r="D50" s="2" t="s">
         <v>104</v>
@@ -2911,12 +2975,12 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="J50" s="80"/>
+      <c r="J50" s="47"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="55"/>
-      <c r="B51" s="77"/>
-      <c r="C51" s="81"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="92"/>
+      <c r="C51" s="48"/>
       <c r="D51" s="2" t="s">
         <v>109</v>
       </c>
@@ -2938,9 +3002,9 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="55"/>
-      <c r="B52" s="77"/>
-      <c r="C52" s="81"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="92"/>
+      <c r="C52" s="48"/>
       <c r="D52" s="2" t="s">
         <v>110</v>
       </c>
@@ -2962,10 +3026,10 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="55"/>
-      <c r="B53" s="77"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="53"/>
+      <c r="A53" s="66"/>
+      <c r="B53" s="92"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="64"/>
       <c r="E53" s="31" t="s">
         <v>114</v>
       </c>
@@ -2986,8 +3050,8 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="55"/>
-      <c r="B54" s="77"/>
+      <c r="A54" s="66"/>
+      <c r="B54" s="92"/>
       <c r="C54" s="25"/>
       <c r="D54" s="2" t="s">
         <v>115</v>
@@ -3010,8 +3074,8 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="55"/>
-      <c r="B55" s="77"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="92"/>
       <c r="C55" s="28"/>
       <c r="D55" s="7" t="s">
         <v>116</v>
@@ -3034,14 +3098,14 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="68" t="s">
+      <c r="A56" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="73"/>
-      <c r="D56" s="74"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="84"/>
       <c r="E56" s="18"/>
       <c r="F56" s="32"/>
       <c r="G56" s="11">
@@ -3050,17 +3114,17 @@
       </c>
       <c r="H56" s="11">
         <f>SUM(H57,H64,J59)</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I56" s="19"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="55"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="75" t="s">
+      <c r="A57" s="66"/>
+      <c r="B57" s="93"/>
+      <c r="C57" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="D57" s="76"/>
+      <c r="D57" s="80"/>
       <c r="E57" s="31" t="s">
         <v>97</v>
       </c>
@@ -3072,18 +3136,18 @@
         <v>44</v>
       </c>
       <c r="H57" s="31">
-        <f>SUM(H58:H81)</f>
-        <v>28</v>
+        <f>SUM(H58:H84)</f>
+        <v>54</v>
       </c>
       <c r="I57" s="24">
-        <f>SUM(I58:I81)</f>
-        <v>170</v>
+        <f>SUM(I58:I84)</f>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="55"/>
-      <c r="B58" s="69"/>
-      <c r="C58" s="25"/>
+      <c r="A58" s="66"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="2" t="s">
         <v>111</v>
       </c>
@@ -3105,9 +3169,9 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="55"/>
-      <c r="B59" s="69"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="66"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="2" t="s">
         <v>113</v>
       </c>
@@ -3129,9 +3193,9 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="55"/>
-      <c r="B60" s="69"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="66"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="2" t="s">
         <v>119</v>
       </c>
@@ -3153,9 +3217,9 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="55"/>
-      <c r="B61" s="69"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="66"/>
+      <c r="B61" s="93"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="2" t="s">
         <v>120</v>
       </c>
@@ -3177,9 +3241,9 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="55"/>
-      <c r="B62" s="69"/>
-      <c r="C62" s="25"/>
+      <c r="A62" s="66"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="35"/>
       <c r="D62" s="2" t="s">
         <v>125</v>
       </c>
@@ -3201,8 +3265,8 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="55"/>
-      <c r="B63" s="69"/>
+      <c r="A63" s="66"/>
+      <c r="B63" s="93"/>
       <c r="C63" s="25" t="s">
         <v>132</v>
       </c>
@@ -3227,12 +3291,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="55"/>
-      <c r="B64" s="69"/>
-      <c r="C64" s="75" t="s">
+      <c r="A64" s="66"/>
+      <c r="B64" s="93"/>
+      <c r="C64" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="76"/>
+      <c r="D64" s="80"/>
       <c r="E64" s="31" t="s">
         <v>106</v>
       </c>
@@ -3253,8 +3317,8 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="55"/>
-      <c r="B65" s="69"/>
+      <c r="A65" s="66"/>
+      <c r="B65" s="93"/>
       <c r="C65" s="25"/>
       <c r="D65" s="2" t="s">
         <v>129</v>
@@ -3277,8 +3341,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="55"/>
-      <c r="B66" s="69"/>
+      <c r="A66" s="66"/>
+      <c r="B66" s="93"/>
       <c r="C66" s="25"/>
       <c r="D66" s="2" t="s">
         <v>130</v>
@@ -3301,10 +3365,10 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="55"/>
-      <c r="B67" s="69"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="53"/>
+      <c r="A67" s="66"/>
+      <c r="B67" s="93"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="64"/>
       <c r="E67" s="31" t="s">
         <v>114</v>
       </c>
@@ -3325,8 +3389,8 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="55"/>
-      <c r="B68" s="69"/>
+      <c r="A68" s="66"/>
+      <c r="B68" s="93"/>
       <c r="C68" s="25"/>
       <c r="D68" s="2" t="s">
         <v>115</v>
@@ -3349,9 +3413,9 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
-      <c r="B69" s="69"/>
-      <c r="C69" s="25"/>
+      <c r="A69" s="66"/>
+      <c r="B69" s="93"/>
+      <c r="C69" s="35"/>
       <c r="D69" s="2" t="s">
         <v>116</v>
       </c>
@@ -3372,17 +3436,17 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="55"/>
-      <c r="B70" s="69"/>
-      <c r="C70" s="52" t="s">
+      <c r="A70" s="66"/>
+      <c r="B70" s="93"/>
+      <c r="C70" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="53"/>
+      <c r="D70" s="64"/>
       <c r="E70" s="31" t="s">
         <v>136</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G70" s="31">
         <f>SUM(G71:G73)</f>
@@ -3390,7 +3454,7 @@
       </c>
       <c r="H70" s="31">
         <f t="shared" ref="H70" si="18">SUM(H71:H74)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I70" s="24">
         <f t="shared" ref="I70" si="19">SUM(I71:I74)</f>
@@ -3398,8 +3462,8 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="55"/>
-      <c r="B71" s="69"/>
+      <c r="A71" s="66"/>
+      <c r="B71" s="93"/>
       <c r="C71" s="25"/>
       <c r="D71" s="2" t="s">
         <v>134</v>
@@ -3408,49 +3472,49 @@
         <v>137</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G71" s="2">
         <v>8</v>
       </c>
       <c r="H71" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I71" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="55"/>
-      <c r="B72" s="69"/>
+      <c r="A72" s="66"/>
+      <c r="B72" s="93"/>
       <c r="C72" s="25"/>
       <c r="D72" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E72" s="82" t="s">
+      <c r="E72" s="49" t="s">
         <v>139</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G72" s="2">
         <v>8</v>
       </c>
       <c r="H72" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I72" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="56"/>
-      <c r="B73" s="70"/>
+      <c r="A73" s="67"/>
+      <c r="B73" s="82"/>
       <c r="C73" s="28"/>
       <c r="D73" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="E73" s="83" t="s">
+      <c r="E73" s="50" t="s">
         <v>141</v>
       </c>
       <c r="F73" s="7" t="s">
@@ -3467,58 +3531,58 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="54" t="s">
+      <c r="A74" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="71" t="s">
+      <c r="B74" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C74" s="73"/>
-      <c r="D74" s="74"/>
+      <c r="C74" s="83"/>
+      <c r="D74" s="84"/>
       <c r="E74" s="18"/>
-      <c r="F74" s="32"/>
+      <c r="F74" s="56"/>
       <c r="G74" s="11">
         <f>SUM(G75)</f>
         <v>36</v>
       </c>
       <c r="H74" s="11">
-        <f>SUM(H75,H82,J77)</f>
+        <f>SUM(H75,H85,J77)</f>
         <v>0</v>
       </c>
       <c r="I74" s="19"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="55"/>
-      <c r="B75" s="77"/>
-      <c r="C75" s="75" t="s">
+      <c r="A75" s="66"/>
+      <c r="B75" s="95"/>
+      <c r="C75" s="79" t="s">
         <v>142</v>
       </c>
-      <c r="D75" s="76"/>
-      <c r="E75" s="31" t="s">
+      <c r="D75" s="80"/>
+      <c r="E75" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="F75" s="31" t="s">
+      <c r="F75" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="G75" s="31">
-        <f>SUM(G76:G81)</f>
+      <c r="G75" s="57">
+        <f>SUM(G76:G80)</f>
         <v>36</v>
       </c>
-      <c r="H75" s="31">
-        <f>SUM(H76:H99)</f>
+      <c r="H75" s="57">
+        <f t="shared" ref="H75:I75" si="20">SUM(H76:H80)</f>
         <v>0</v>
       </c>
       <c r="I75" s="24">
-        <f>SUM(I76:I99)</f>
+        <f t="shared" si="20"/>
         <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="55"/>
-      <c r="B76" s="77"/>
+      <c r="A76" s="66"/>
+      <c r="B76" s="95"/>
       <c r="C76" s="25"/>
       <c r="D76" s="2" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>99</v>
@@ -3538,11 +3602,11 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="55"/>
-      <c r="B77" s="77"/>
+      <c r="A77" s="66"/>
+      <c r="B77" s="95"/>
       <c r="C77" s="25"/>
       <c r="D77" s="2" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>58</v>
@@ -3562,11 +3626,11 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="55"/>
-      <c r="B78" s="77"/>
+      <c r="A78" s="66"/>
+      <c r="B78" s="95"/>
       <c r="C78" s="25"/>
-      <c r="D78" s="2" t="s">
-        <v>119</v>
+      <c r="D78" s="98" t="s">
+        <v>145</v>
       </c>
       <c r="E78" s="15" t="s">
         <v>61</v>
@@ -3586,11 +3650,11 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="55"/>
-      <c r="B79" s="77"/>
+      <c r="A79" s="66"/>
+      <c r="B79" s="95"/>
       <c r="C79" s="25"/>
       <c r="D79" s="2" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>62</v>
@@ -3610,11 +3674,11 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="55"/>
-      <c r="B80" s="77"/>
+      <c r="A80" s="66"/>
+      <c r="B80" s="95"/>
       <c r="C80" s="25"/>
       <c r="D80" s="2" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="E80" s="15" t="s">
         <v>59</v>
@@ -3629,81 +3693,171 @@
         <v>0</v>
       </c>
       <c r="I80" s="27">
-        <f t="shared" ref="I80" si="20">G80-H80</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="56"/>
-      <c r="B81" s="72"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="93"/>
-      <c r="E81" s="93"/>
-      <c r="F81" s="93"/>
-      <c r="G81" s="93"/>
-      <c r="H81" s="93"/>
-      <c r="I81" s="94"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="54" t="s">
+        <f t="shared" ref="I80" si="21">G80-H80</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="66"/>
+      <c r="B81" s="95"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F81" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="G81" s="57">
+        <f>SUM(G82:G82)</f>
+        <v>5</v>
+      </c>
+      <c r="H81" s="57">
+        <f>SUM(H82:H82)</f>
+        <v>0</v>
+      </c>
+      <c r="I81" s="24">
+        <f>SUM(I82:I82)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="66"/>
+      <c r="B82" s="95"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82" s="4">
+        <v>5</v>
+      </c>
+      <c r="H82" s="4">
+        <v>0</v>
+      </c>
+      <c r="I82" s="27">
+        <v>5</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="66"/>
+      <c r="B83" s="95"/>
+      <c r="C83" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D83" s="64"/>
+      <c r="E83" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="F83" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="G83" s="57">
+        <f>SUM(G84)</f>
+        <v>0</v>
+      </c>
+      <c r="H83" s="57">
+        <f t="shared" ref="H83:I83" si="22">SUM(H84)</f>
+        <v>0</v>
+      </c>
+      <c r="I83" s="57">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="67"/>
+      <c r="B84" s="96"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="98" t="s">
+        <v>149</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G84" s="2">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B82" s="68" t="s">
+      <c r="B85" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="73"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="11">
+      <c r="C85" s="83"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="32"/>
+      <c r="G85" s="11">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="H82" s="32"/>
-      <c r="I82" s="19"/>
-    </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="56"/>
-      <c r="B83" s="70"/>
-      <c r="C83" s="89" t="s">
+      <c r="H85" s="32"/>
+      <c r="I85" s="19"/>
+    </row>
+    <row r="86" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="67"/>
+      <c r="B86" s="82"/>
+      <c r="C86" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D83" s="90"/>
-      <c r="E83" s="91" t="s">
+      <c r="D86" s="88"/>
+      <c r="E86" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="F83" s="91" t="s">
+      <c r="F86" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="G83" s="91">
-        <v>0</v>
-      </c>
-      <c r="H83" s="91">
+      <c r="G86" s="54">
+        <v>0</v>
+      </c>
+      <c r="H86" s="54">
         <f>SUM(0)</f>
         <v>0</v>
       </c>
-      <c r="I83" s="92">
+      <c r="I86" s="55">
         <f>SUM(0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="30" t="s">
+    <row r="87" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B84" s="84" t="s">
+      <c r="B87" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C84" s="85"/>
-      <c r="D84" s="86"/>
-      <c r="E84" s="87"/>
-      <c r="F84" s="87"/>
-      <c r="G84" s="87"/>
-      <c r="H84" s="87"/>
-      <c r="I84" s="88"/>
+      <c r="C87" s="89"/>
+      <c r="D87" s="90"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+      <c r="H87" s="52"/>
+      <c r="I87" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="42">
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C83:D83"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C64:D64"/>
@@ -3714,24 +3868,24 @@
     <mergeCell ref="A43:A55"/>
     <mergeCell ref="B43:B55"/>
     <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A21:A42"/>
     <mergeCell ref="B21:B42"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:D85"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C83:D84"/>
-    <mergeCell ref="A74:A81"/>
-    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C86:D87"/>
+    <mergeCell ref="A74:A84"/>
+    <mergeCell ref="B74:B84"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C3:D3"/>
@@ -3746,7 +3900,7 @@
     <mergeCell ref="C10:D10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F82:F83 F3:F80">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F86">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update plan (close Sprint 6 and add tasts for Sprint 7)
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="172">
   <si>
     <t>11.09.18</t>
   </si>
@@ -482,6 +482,69 @@
   </si>
   <si>
     <t>[Continue] Frontend html/css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error then click "remove from cart" then amount of product equal 0 </t>
+  </si>
+  <si>
+    <t>Create UI for App components</t>
+  </si>
+  <si>
+    <t>TA56</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Continue] Security Issue</t>
+  </si>
+  <si>
+    <t>Create popup dialog "Order is sucsessful"</t>
+  </si>
+  <si>
+    <t>TA57</t>
+  </si>
+  <si>
+    <t>Add different pictures to products</t>
+  </si>
+  <si>
+    <t>TA58</t>
+  </si>
+  <si>
+    <t>TA59</t>
+  </si>
+  <si>
+    <t>TA60</t>
+  </si>
+  <si>
+    <t>TA61</t>
+  </si>
+  <si>
+    <t>TA62</t>
+  </si>
+  <si>
+    <t>Add new model to backend</t>
+  </si>
+  <si>
+    <t>US15</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>Sprint 7</t>
   </si>
 </sst>
 </file>
@@ -512,7 +575,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,12 +611,6 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="47">
     <border>
@@ -916,17 +973,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1108,17 +1154,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1145,6 +1180,26 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1190,9 +1245,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1201,106 +1253,100 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1309,25 +1355,112 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1348,112 +1481,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1737,11 +1792,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U87"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,77 +1813,79 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="44" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58"/>
-      <c r="B1" s="59"/>
-      <c r="C1" s="58" t="s">
+    <row r="1" spans="1:21" s="41" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="84"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="45" t="s">
+      <c r="D1" s="86"/>
+      <c r="E1" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="43" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="11" t="s">
+        <v>165</v>
+      </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11">
         <f>SUM(G3)</f>
         <v>28</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="39"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="61" t="s">
+      <c r="A3" s="69"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="88"/>
+      <c r="E3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="17">
         <f>SUM(G4:G8)</f>
         <v>28</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="17">
         <f>SUM(H4:H8)</f>
         <v>20</v>
       </c>
-      <c r="I3" s="40">
+      <c r="I3" s="37">
         <f>SUM(I4:I8)</f>
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1844,7 +1901,7 @@
       <c r="H4" s="2">
         <v>4</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="23">
         <f>G4-H4</f>
         <v>4</v>
       </c>
@@ -1853,9 +1910,9 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1871,7 +1928,7 @@
       <c r="H5" s="2">
         <v>2</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="23">
         <f>G5-H5</f>
         <v>2</v>
       </c>
@@ -1880,9 +1937,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="36"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1898,7 +1955,7 @@
       <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="23">
         <f t="shared" ref="I6:I8" si="0">G6-H6</f>
         <v>2</v>
       </c>
@@ -1907,9 +1964,9 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1925,7 +1982,7 @@
       <c r="H7" s="4">
         <v>8</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1934,9 +1991,9 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
@@ -1952,61 +2009,63 @@
       <c r="H8" s="7">
         <v>4</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14">
+      <c r="C9" s="91"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13">
         <f>SUM(G10,G14,G17)</f>
         <v>38</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="42"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="39"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="61" t="s">
+      <c r="A10" s="69"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="20" t="s">
+      <c r="D10" s="88"/>
+      <c r="E10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="17">
         <f>SUM(G11:G13)</f>
         <v>12</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <f>SUM(H11:H15)</f>
         <v>36</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="37">
         <f>SUM(I11:I15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="25"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
@@ -2022,15 +2081,15 @@
       <c r="H11" s="2">
         <v>4</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="23">
         <f>G11-H11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -2046,15 +2105,15 @@
       <c r="H12" s="2">
         <v>4</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="23">
         <f>G12-H12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="37"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
@@ -2070,41 +2129,41 @@
       <c r="H13" s="2">
         <v>4</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="23">
         <f>G13-H13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="66"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="63" t="s">
+      <c r="A14" s="69"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="23" t="s">
+      <c r="D14" s="61"/>
+      <c r="E14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <f>SUM(G15:G16)</f>
         <v>16</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="20">
         <f>SUM(H15:H16)</f>
         <v>16</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="21">
         <f>SUM(I15:I16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="25"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
@@ -2120,15 +2179,15 @@
       <c r="H15" s="2">
         <v>8</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="23">
         <f>G15-H15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
@@ -2144,41 +2203,41 @@
       <c r="H16" s="2">
         <v>8</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="23">
         <f>G16-H16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="75" t="s">
+      <c r="A17" s="69"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="21" t="s">
+      <c r="D17" s="94"/>
+      <c r="E17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="18">
         <f>SUM(G18:G20)</f>
         <v>10</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="18">
         <f t="shared" ref="H17:I17" si="1">SUM(H18:H20)</f>
         <v>3</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="31">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="2" t="s">
         <v>47</v>
       </c>
@@ -2194,15 +2253,15 @@
       <c r="H18" s="2">
         <v>2</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="23">
         <f>G18-H18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="35"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="2" t="s">
         <v>66</v>
       </c>
@@ -2218,7 +2277,7 @@
       <c r="H19" s="2">
         <v>1</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="23">
         <f>G19-H19</f>
         <v>3</v>
       </c>
@@ -2227,16 +2286,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="66"/>
-      <c r="B20" s="69"/>
-      <c r="C20" s="38"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="43" t="s">
+      <c r="F20" s="40" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="7">
@@ -2245,58 +2304,60 @@
       <c r="H20" s="7">
         <v>0</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="26">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="68" t="s">
+      <c r="A21" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="17">
+      <c r="C21" s="95"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="15">
         <f>SUM(G22,G27,G36,G39)</f>
         <v>76</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="33"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="85" t="s">
+      <c r="A22" s="69"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="63"/>
+      <c r="E22" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="18">
         <f>SUM(G23:G26)</f>
         <v>6</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="18">
         <f t="shared" ref="H22:I22" si="2">SUM(H23:H26)</f>
         <v>3.25</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="31">
         <f t="shared" si="2"/>
         <v>2.75</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
@@ -2312,15 +2373,15 @@
       <c r="H23" s="2">
         <v>1</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="23">
         <f>G23-H23</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="2" t="s">
         <v>54</v>
       </c>
@@ -2336,15 +2397,15 @@
       <c r="H24" s="2">
         <v>1</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="23">
         <f>G24-H24</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2360,15 +2421,15 @@
       <c r="H25" s="2">
         <v>1</v>
       </c>
-      <c r="I25" s="26">
+      <c r="I25" s="23">
         <f>G25-H25</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="66"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="2" t="s">
         <v>56</v>
       </c>
@@ -2384,41 +2445,41 @@
       <c r="H26" s="2">
         <v>0.25</v>
       </c>
-      <c r="I26" s="26">
+      <c r="I26" s="23">
         <f>G26-H26</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="85" t="s">
+      <c r="A27" s="69"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="86"/>
-      <c r="E27" s="21" t="s">
+      <c r="D27" s="63"/>
+      <c r="E27" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="18">
         <f>SUM(G28:G35)</f>
         <v>46</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="18">
         <f ca="1">SUM(H25:H35)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="31">
         <f ca="1">SUM(I25:I35)</f>
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="2" t="s">
         <v>57</v>
       </c>
@@ -2434,19 +2495,19 @@
       <c r="H28" s="2">
         <v>2</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="23">
         <f>G28-H28</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>44</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -2458,14 +2519,14 @@
       <c r="H29" s="4">
         <v>4</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="24">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="2" t="s">
         <v>68</v>
       </c>
@@ -2481,7 +2542,7 @@
       <c r="H30" s="2">
         <v>16</v>
       </c>
-      <c r="I30" s="26">
+      <c r="I30" s="23">
         <f t="shared" ref="I30" si="3">G30-H30</f>
         <v>-12</v>
       </c>
@@ -2490,9 +2551,9 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="2" t="s">
         <v>75</v>
       </c>
@@ -2508,7 +2569,7 @@
       <c r="H31" s="2">
         <v>2</v>
       </c>
-      <c r="I31" s="26">
+      <c r="I31" s="23">
         <f t="shared" ref="I31" si="4">G31-H31</f>
         <v>6</v>
       </c>
@@ -2517,9 +2578,9 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="35"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="2" t="s">
         <v>76</v>
       </c>
@@ -2535,19 +2596,19 @@
       <c r="H32" s="2">
         <v>0</v>
       </c>
-      <c r="I32" s="26">
+      <c r="I32" s="23">
         <f>G32-H32</f>
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="66"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="35"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>61</v>
       </c>
       <c r="F33" s="2" t="s">
@@ -2559,19 +2620,19 @@
       <c r="H33" s="2">
         <v>0</v>
       </c>
-      <c r="I33" s="26">
+      <c r="I33" s="23">
         <f>G33-H33</f>
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="66"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="35"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F34" s="2" t="s">
@@ -2583,19 +2644,19 @@
       <c r="H34" s="2">
         <v>0</v>
       </c>
-      <c r="I34" s="26">
+      <c r="I34" s="23">
         <f>G34-H34</f>
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="66"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="36"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="14" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -2607,41 +2668,41 @@
       <c r="H35" s="4">
         <v>0</v>
       </c>
-      <c r="I35" s="27">
+      <c r="I35" s="24">
         <f t="shared" ref="I35" si="5">G35-H35</f>
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="66"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="79" t="s">
+      <c r="A36" s="69"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="80"/>
-      <c r="E36" s="23" t="s">
+      <c r="D36" s="65"/>
+      <c r="E36" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="20">
         <f>SUM(G37:G38)</f>
         <v>4</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="20">
         <f t="shared" ref="H36:I36" si="6">SUM(H37:H38)</f>
         <v>1</v>
       </c>
-      <c r="I36" s="24">
+      <c r="I36" s="21">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
-      <c r="B37" s="69"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="2" t="s">
         <v>86</v>
       </c>
@@ -2657,19 +2718,19 @@
       <c r="H37" s="2">
         <v>0.5</v>
       </c>
-      <c r="I37" s="26">
+      <c r="I37" s="23">
         <f t="shared" ref="I37" si="7">G37-H37</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="66"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="37"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -2681,41 +2742,41 @@
       <c r="H38" s="4">
         <v>0.5</v>
       </c>
-      <c r="I38" s="27">
+      <c r="I38" s="24">
         <f t="shared" ref="I38" si="8">G38-H38</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="79" t="s">
+      <c r="A39" s="69"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="80"/>
-      <c r="E39" s="23" t="s">
+      <c r="D39" s="65"/>
+      <c r="E39" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="20">
         <f>SUM(G40:G42)</f>
         <v>20</v>
       </c>
-      <c r="H39" s="23">
+      <c r="H39" s="20">
         <f t="shared" ref="H39:I39" si="9">SUM(H40:H42)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="21">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="66"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="35"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="2" t="s">
         <v>93</v>
       </c>
@@ -2731,15 +2792,15 @@
       <c r="H40" s="2">
         <v>0</v>
       </c>
-      <c r="I40" s="26">
+      <c r="I40" s="23">
         <f t="shared" ref="I40" si="10">G40-H40</f>
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="66"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="35"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="2" t="s">
         <v>94</v>
       </c>
@@ -2755,15 +2816,15 @@
       <c r="H41" s="2">
         <v>0</v>
       </c>
-      <c r="I41" s="26">
+      <c r="I41" s="23">
         <f t="shared" ref="I41" si="11">G41-H41</f>
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="67"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="38"/>
+      <c r="A42" s="70"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="7" t="s">
         <v>88</v>
       </c>
@@ -2779,21 +2840,23 @@
       <c r="H42" s="7">
         <v>0</v>
       </c>
-      <c r="I42" s="29">
+      <c r="I42" s="26">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="65" t="s">
+      <c r="A43" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="83"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="32"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="29"/>
       <c r="G43" s="11">
         <f>SUM(G44,G46)</f>
         <v>48.5</v>
@@ -2802,38 +2865,38 @@
         <f>SUM(H44,H46,H53)</f>
         <v>43</v>
       </c>
-      <c r="I43" s="19"/>
+      <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="66"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="79" t="s">
+      <c r="A44" s="69"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="80"/>
-      <c r="E44" s="31" t="s">
+      <c r="D44" s="65"/>
+      <c r="E44" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="31">
+      <c r="G44" s="28">
         <f>SUM(G45:G45)</f>
         <v>8</v>
       </c>
-      <c r="H44" s="31">
+      <c r="H44" s="28">
         <f t="shared" ref="H44:I44" si="12">SUM(H45:H45)</f>
         <v>0</v>
       </c>
-      <c r="I44" s="24">
+      <c r="I44" s="21">
         <f t="shared" si="12"/>
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="66"/>
-      <c r="B45" s="92"/>
-      <c r="C45" s="35"/>
+      <c r="A45" s="69"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="2" t="s">
         <v>100</v>
       </c>
@@ -2849,41 +2912,41 @@
       <c r="H45" s="2">
         <v>0</v>
       </c>
-      <c r="I45" s="26">
+      <c r="I45" s="23">
         <f>G45-H45</f>
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="66"/>
-      <c r="B46" s="92"/>
-      <c r="C46" s="79" t="s">
+      <c r="A46" s="69"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="80"/>
-      <c r="E46" s="31" t="s">
+      <c r="D46" s="65"/>
+      <c r="E46" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G46" s="31">
+      <c r="G46" s="28">
         <f>SUM(G47:G54)</f>
         <v>40.5</v>
       </c>
-      <c r="H46" s="31">
+      <c r="H46" s="28">
         <f>SUM(H47:H54)</f>
         <v>37.5</v>
       </c>
-      <c r="I46" s="24">
+      <c r="I46" s="21">
         <f>SUM(I47:I54)</f>
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="66"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="25"/>
+      <c r="A47" s="69"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="2" t="s">
         <v>101</v>
       </c>
@@ -2899,15 +2962,15 @@
       <c r="H47" s="2">
         <v>8</v>
       </c>
-      <c r="I47" s="26">
+      <c r="I47" s="23">
         <f t="shared" ref="I47:I52" si="13">G47-H47</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="66"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="25"/>
+      <c r="A48" s="69"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="2" t="s">
         <v>102</v>
       </c>
@@ -2923,15 +2986,15 @@
       <c r="H48" s="2">
         <v>8</v>
       </c>
-      <c r="I48" s="26">
+      <c r="I48" s="23">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="66"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="34"/>
       <c r="D49" s="2" t="s">
         <v>103</v>
       </c>
@@ -2947,15 +3010,15 @@
       <c r="H49" s="2">
         <v>4</v>
       </c>
-      <c r="I49" s="26">
+      <c r="I49" s="23">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="66"/>
-      <c r="B50" s="92"/>
-      <c r="C50" s="41"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="2" t="s">
         <v>104</v>
       </c>
@@ -2971,16 +3034,16 @@
       <c r="H50" s="2">
         <v>5</v>
       </c>
-      <c r="I50" s="26">
+      <c r="I50" s="23">
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="J50" s="47"/>
+      <c r="J50" s="44"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="66"/>
-      <c r="B51" s="92"/>
-      <c r="C51" s="48"/>
+      <c r="A51" s="69"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="45"/>
       <c r="D51" s="2" t="s">
         <v>109</v>
       </c>
@@ -2996,15 +3059,15 @@
       <c r="H51" s="2">
         <v>2</v>
       </c>
-      <c r="I51" s="26">
+      <c r="I51" s="23">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
-      <c r="B52" s="92"/>
-      <c r="C52" s="48"/>
+      <c r="A52" s="69"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="45"/>
       <c r="D52" s="2" t="s">
         <v>110</v>
       </c>
@@ -3020,39 +3083,39 @@
       <c r="H52" s="2">
         <v>0</v>
       </c>
-      <c r="I52" s="26">
+      <c r="I52" s="23">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="66"/>
-      <c r="B53" s="92"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="31" t="s">
+      <c r="A53" s="69"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F53" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G53" s="31">
+      <c r="G53" s="28">
         <f>SUM(G54:G55)</f>
         <v>4.5</v>
       </c>
-      <c r="H53" s="31">
+      <c r="H53" s="28">
         <f>SUM(H54:H55)</f>
         <v>5.5</v>
       </c>
-      <c r="I53" s="24">
+      <c r="I53" s="21">
         <f>SUM(I54:I55)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="66"/>
-      <c r="B54" s="92"/>
-      <c r="C54" s="25"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="22"/>
       <c r="D54" s="2" t="s">
         <v>115</v>
       </c>
@@ -3068,15 +3131,15 @@
       <c r="H54" s="2">
         <v>5</v>
       </c>
-      <c r="I54" s="26">
+      <c r="I54" s="23">
         <f>G54-H54</f>
         <v>-1</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="66"/>
-      <c r="B55" s="92"/>
-      <c r="C55" s="28"/>
+      <c r="A55" s="69"/>
+      <c r="B55" s="81"/>
+      <c r="C55" s="25"/>
       <c r="D55" s="7" t="s">
         <v>116</v>
       </c>
@@ -3092,62 +3155,64 @@
       <c r="H55" s="7">
         <v>0.5</v>
       </c>
-      <c r="I55" s="29">
+      <c r="I55" s="26">
         <f>G55-H55</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="81" t="s">
+      <c r="A56" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="83"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="32"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F56" s="29"/>
       <c r="G56" s="11">
         <f>SUM(G57,G64,G67)</f>
         <v>61</v>
       </c>
       <c r="H56" s="11">
         <f>SUM(H57,H64,J59)</f>
-        <v>60</v>
-      </c>
-      <c r="I56" s="19"/>
+        <v>120.5</v>
+      </c>
+      <c r="I56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="66"/>
-      <c r="B57" s="93"/>
-      <c r="C57" s="79" t="s">
+      <c r="A57" s="69"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="D57" s="80"/>
-      <c r="E57" s="31" t="s">
+      <c r="D57" s="65"/>
+      <c r="E57" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="G57" s="31">
+      <c r="G57" s="28">
         <f>SUM(G58:G63)</f>
         <v>44</v>
       </c>
-      <c r="H57" s="31">
-        <f>SUM(H58:H84)</f>
-        <v>54</v>
-      </c>
-      <c r="I57" s="24">
-        <f>SUM(I58:I84)</f>
-        <v>180</v>
+      <c r="H57" s="28">
+        <f>SUM(H58:H85)</f>
+        <v>114.5</v>
+      </c>
+      <c r="I57" s="21">
+        <f>SUM(I58:I85)</f>
+        <v>162.5</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="66"/>
-      <c r="B58" s="93"/>
-      <c r="C58" s="35"/>
+      <c r="A58" s="69"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="32"/>
       <c r="D58" s="2" t="s">
         <v>111</v>
       </c>
@@ -3163,15 +3228,15 @@
       <c r="H58" s="2">
         <v>0</v>
       </c>
-      <c r="I58" s="26">
+      <c r="I58" s="23">
         <f>G58-H58</f>
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="66"/>
-      <c r="B59" s="93"/>
-      <c r="C59" s="35"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="78"/>
+      <c r="C59" s="32"/>
       <c r="D59" s="2" t="s">
         <v>113</v>
       </c>
@@ -3187,19 +3252,19 @@
       <c r="H59" s="2">
         <v>0</v>
       </c>
-      <c r="I59" s="26">
+      <c r="I59" s="23">
         <f>G59-H59</f>
         <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="66"/>
-      <c r="B60" s="93"/>
-      <c r="C60" s="35"/>
+      <c r="A60" s="69"/>
+      <c r="B60" s="78"/>
+      <c r="C60" s="32"/>
       <c r="D60" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="15" t="s">
+      <c r="E60" s="14" t="s">
         <v>61</v>
       </c>
       <c r="F60" s="2" t="s">
@@ -3211,19 +3276,19 @@
       <c r="H60" s="2">
         <v>0</v>
       </c>
-      <c r="I60" s="26">
+      <c r="I60" s="23">
         <f>G60-H60</f>
         <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="66"/>
-      <c r="B61" s="93"/>
-      <c r="C61" s="35"/>
+      <c r="A61" s="69"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="32"/>
       <c r="D61" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F61" s="2" t="s">
@@ -3235,19 +3300,19 @@
       <c r="H61" s="2">
         <v>0</v>
       </c>
-      <c r="I61" s="26">
+      <c r="I61" s="23">
         <f>G61-H61</f>
         <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="66"/>
-      <c r="B62" s="93"/>
-      <c r="C62" s="35"/>
+      <c r="A62" s="69"/>
+      <c r="B62" s="78"/>
+      <c r="C62" s="32"/>
       <c r="D62" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="14" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -3259,15 +3324,15 @@
       <c r="H62" s="4">
         <v>0</v>
       </c>
-      <c r="I62" s="27">
+      <c r="I62" s="24">
         <f t="shared" ref="I62" si="14">G62-H62</f>
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="66"/>
-      <c r="B63" s="93"/>
-      <c r="C63" s="25" t="s">
+      <c r="A63" s="69"/>
+      <c r="B63" s="78"/>
+      <c r="C63" s="22" t="s">
         <v>132</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -3285,41 +3350,41 @@
       <c r="H63" s="2">
         <v>0</v>
       </c>
-      <c r="I63" s="26">
+      <c r="I63" s="23">
         <f>G63-H63</f>
         <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="66"/>
-      <c r="B64" s="93"/>
-      <c r="C64" s="79" t="s">
+      <c r="A64" s="69"/>
+      <c r="B64" s="78"/>
+      <c r="C64" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="80"/>
-      <c r="E64" s="31" t="s">
+      <c r="D64" s="65"/>
+      <c r="E64" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F64" s="31" t="s">
+      <c r="F64" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G64" s="31">
+      <c r="G64" s="28">
         <f>SUM(G65:G66)</f>
         <v>8</v>
       </c>
-      <c r="H64" s="31">
+      <c r="H64" s="28">
         <f t="shared" ref="H64:I64" si="15">SUM(H65:H66)</f>
         <v>6</v>
       </c>
-      <c r="I64" s="24">
+      <c r="I64" s="21">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="66"/>
-      <c r="B65" s="93"/>
-      <c r="C65" s="25"/>
+      <c r="A65" s="69"/>
+      <c r="B65" s="78"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="2" t="s">
         <v>129</v>
       </c>
@@ -3335,15 +3400,15 @@
       <c r="H65" s="2">
         <v>4</v>
       </c>
-      <c r="I65" s="26">
+      <c r="I65" s="23">
         <f t="shared" ref="I65:I66" si="16">G65-H65</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="66"/>
-      <c r="B66" s="93"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="69"/>
+      <c r="B66" s="78"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="2" t="s">
         <v>130</v>
       </c>
@@ -3359,39 +3424,39 @@
       <c r="H66" s="2">
         <v>2</v>
       </c>
-      <c r="I66" s="26">
+      <c r="I66" s="23">
         <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="66"/>
-      <c r="B67" s="93"/>
-      <c r="C67" s="63"/>
-      <c r="D67" s="64"/>
-      <c r="E67" s="31" t="s">
+      <c r="A67" s="69"/>
+      <c r="B67" s="78"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="F67" s="31" t="s">
+      <c r="F67" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G67" s="31">
+      <c r="G67" s="28">
         <f>SUM(G68:G69)</f>
         <v>9</v>
       </c>
-      <c r="H67" s="31">
+      <c r="H67" s="28">
         <f t="shared" ref="H67:I67" si="17">SUM(H68:H69)</f>
         <v>8</v>
       </c>
-      <c r="I67" s="24">
+      <c r="I67" s="21">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="66"/>
-      <c r="B68" s="93"/>
-      <c r="C68" s="25"/>
+      <c r="A68" s="69"/>
+      <c r="B68" s="78"/>
+      <c r="C68" s="22"/>
       <c r="D68" s="2" t="s">
         <v>115</v>
       </c>
@@ -3407,15 +3472,15 @@
       <c r="H68" s="2">
         <v>8</v>
       </c>
-      <c r="I68" s="26">
+      <c r="I68" s="23">
         <f>G68-H68</f>
         <v>-4</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="66"/>
-      <c r="B69" s="93"/>
-      <c r="C69" s="35"/>
+      <c r="A69" s="69"/>
+      <c r="B69" s="78"/>
+      <c r="C69" s="32"/>
       <c r="D69" s="2" t="s">
         <v>116</v>
       </c>
@@ -3431,40 +3496,40 @@
       <c r="H69" s="2">
         <v>0</v>
       </c>
-      <c r="I69" s="26">
+      <c r="I69" s="23">
         <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="66"/>
-      <c r="B70" s="93"/>
-      <c r="C70" s="63" t="s">
+      <c r="A70" s="69"/>
+      <c r="B70" s="78"/>
+      <c r="C70" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="64"/>
-      <c r="E70" s="31" t="s">
+      <c r="D70" s="61"/>
+      <c r="E70" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F70" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G70" s="31">
+      <c r="G70" s="28">
         <f>SUM(G71:G73)</f>
         <v>24</v>
       </c>
-      <c r="H70" s="31">
+      <c r="H70" s="28">
         <f t="shared" ref="H70" si="18">SUM(H71:H74)</f>
-        <v>13</v>
-      </c>
-      <c r="I70" s="24">
+        <v>28</v>
+      </c>
+      <c r="I70" s="21">
         <f t="shared" ref="I70" si="19">SUM(I71:I74)</f>
         <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="66"/>
-      <c r="B71" s="93"/>
-      <c r="C71" s="25"/>
+      <c r="A71" s="69"/>
+      <c r="B71" s="78"/>
+      <c r="C71" s="22"/>
       <c r="D71" s="2" t="s">
         <v>134</v>
       </c>
@@ -3480,18 +3545,18 @@
       <c r="H71" s="2">
         <v>8</v>
       </c>
-      <c r="I71" s="26">
+      <c r="I71" s="23">
         <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="66"/>
-      <c r="B72" s="93"/>
-      <c r="C72" s="25"/>
+      <c r="A72" s="69"/>
+      <c r="B72" s="78"/>
+      <c r="C72" s="22"/>
       <c r="D72" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E72" s="49" t="s">
+      <c r="E72" s="46" t="s">
         <v>139</v>
       </c>
       <c r="F72" s="2" t="s">
@@ -3503,18 +3568,18 @@
       <c r="H72" s="2">
         <v>5</v>
       </c>
-      <c r="I72" s="26">
+      <c r="I72" s="23">
         <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="67"/>
-      <c r="B73" s="82"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="43" t="s">
+      <c r="A73" s="70"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="E73" s="50" t="s">
+      <c r="E73" s="47" t="s">
         <v>141</v>
       </c>
       <c r="F73" s="7" t="s">
@@ -3526,61 +3591,63 @@
       <c r="H73" s="7">
         <v>0</v>
       </c>
-      <c r="I73" s="29">
+      <c r="I73" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="65" t="s">
+      <c r="A74" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="94" t="s">
+      <c r="B74" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C74" s="83"/>
-      <c r="D74" s="84"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="56"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F74" s="52"/>
       <c r="G74" s="11">
         <f>SUM(G75)</f>
         <v>36</v>
       </c>
       <c r="H74" s="11">
-        <f>SUM(H75,H85,J77)</f>
-        <v>0</v>
-      </c>
-      <c r="I74" s="19"/>
+        <f>SUM(H75,H81,H84)</f>
+        <v>15</v>
+      </c>
+      <c r="I74" s="16"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="66"/>
-      <c r="B75" s="95"/>
-      <c r="C75" s="79" t="s">
+      <c r="A75" s="69"/>
+      <c r="B75" s="75"/>
+      <c r="C75" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="D75" s="80"/>
-      <c r="E75" s="57" t="s">
+      <c r="D75" s="65"/>
+      <c r="E75" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="F75" s="57" t="s">
+      <c r="F75" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G75" s="57">
+      <c r="G75" s="51">
         <f>SUM(G76:G80)</f>
         <v>36</v>
       </c>
-      <c r="H75" s="57">
+      <c r="H75" s="51">
         <f t="shared" ref="H75:I75" si="20">SUM(H76:H80)</f>
         <v>0</v>
       </c>
-      <c r="I75" s="24">
+      <c r="I75" s="21">
         <f t="shared" si="20"/>
         <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="66"/>
-      <c r="B76" s="95"/>
-      <c r="C76" s="25"/>
+      <c r="A76" s="69"/>
+      <c r="B76" s="75"/>
+      <c r="C76" s="22"/>
       <c r="D76" s="2" t="s">
         <v>143</v>
       </c>
@@ -3596,15 +3663,15 @@
       <c r="H76" s="2">
         <v>0</v>
       </c>
-      <c r="I76" s="26">
+      <c r="I76" s="23">
         <f>G76-H76</f>
         <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="66"/>
-      <c r="B77" s="95"/>
-      <c r="C77" s="25"/>
+      <c r="A77" s="69"/>
+      <c r="B77" s="75"/>
+      <c r="C77" s="22"/>
       <c r="D77" s="2" t="s">
         <v>144</v>
       </c>
@@ -3620,19 +3687,19 @@
       <c r="H77" s="2">
         <v>0</v>
       </c>
-      <c r="I77" s="26">
+      <c r="I77" s="23">
         <f>G77-H77</f>
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="66"/>
-      <c r="B78" s="95"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="98" t="s">
+      <c r="A78" s="69"/>
+      <c r="B78" s="75"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E78" s="15" t="s">
+      <c r="E78" s="14" t="s">
         <v>61</v>
       </c>
       <c r="F78" s="2" t="s">
@@ -3644,19 +3711,19 @@
       <c r="H78" s="2">
         <v>0</v>
       </c>
-      <c r="I78" s="26">
+      <c r="I78" s="23">
         <f>G78-H78</f>
         <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
-      <c r="B79" s="95"/>
-      <c r="C79" s="25"/>
+      <c r="A79" s="69"/>
+      <c r="B79" s="75"/>
+      <c r="C79" s="22"/>
       <c r="D79" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E79" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F79" s="2" t="s">
@@ -3668,19 +3735,19 @@
       <c r="H79" s="2">
         <v>0</v>
       </c>
-      <c r="I79" s="26">
+      <c r="I79" s="23">
         <f>G79-H79</f>
         <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="66"/>
-      <c r="B80" s="95"/>
-      <c r="C80" s="25"/>
+      <c r="A80" s="69"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="22"/>
       <c r="D80" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E80" s="15" t="s">
+      <c r="E80" s="14" t="s">
         <v>59</v>
       </c>
       <c r="F80" s="4" t="s">
@@ -3692,200 +3759,468 @@
       <c r="H80" s="4">
         <v>0</v>
       </c>
-      <c r="I80" s="27">
-        <f t="shared" ref="I80" si="21">G80-H80</f>
+      <c r="I80" s="23">
+        <f t="shared" ref="I80:I85" si="21">G80-H80</f>
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="66"/>
-      <c r="B81" s="95"/>
-      <c r="C81" s="63"/>
-      <c r="D81" s="64"/>
-      <c r="E81" s="57" t="s">
+      <c r="A81" s="69"/>
+      <c r="B81" s="75"/>
+      <c r="C81" s="60"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="F81" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="G81" s="57">
+      <c r="F81" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="51">
         <f>SUM(G82:G82)</f>
         <v>5</v>
       </c>
-      <c r="H81" s="57">
+      <c r="H81" s="51">
         <f>SUM(H82:H82)</f>
-        <v>0</v>
-      </c>
-      <c r="I81" s="24">
-        <f>SUM(I82:I82)</f>
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="I81" s="21">
+        <f t="shared" si="21"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="66"/>
-      <c r="B82" s="95"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="97" t="s">
+      <c r="A82" s="69"/>
+      <c r="B82" s="75"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E82" s="15" t="s">
+      <c r="E82" s="14" t="s">
         <v>133</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G82" s="4">
         <v>5</v>
       </c>
       <c r="H82" s="4">
-        <v>0</v>
-      </c>
-      <c r="I82" s="27">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="I82" s="23">
+        <f t="shared" si="21"/>
+        <v>-1</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="66"/>
-      <c r="B83" s="95"/>
-      <c r="C83" s="63" t="s">
+    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="69"/>
+      <c r="B83" s="75"/>
+      <c r="C83" s="53"/>
+      <c r="D83" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G83" s="4">
+        <v>3</v>
+      </c>
+      <c r="H83" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I83" s="23">
+        <f t="shared" si="21"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="69"/>
+      <c r="B84" s="75"/>
+      <c r="C84" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="D83" s="64"/>
-      <c r="E83" s="57" t="s">
+      <c r="D84" s="61"/>
+      <c r="E84" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F83" s="57" t="s">
+      <c r="F84" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="G84" s="51">
+        <f>SUM(G85)</f>
+        <v>5</v>
+      </c>
+      <c r="H84" s="51">
+        <f t="shared" ref="H84" si="22">SUM(H85)</f>
+        <v>9</v>
+      </c>
+      <c r="I84" s="21">
+        <f t="shared" si="21"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="70"/>
+      <c r="B85" s="76"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G85" s="7">
+        <v>5</v>
+      </c>
+      <c r="H85" s="7">
+        <v>9</v>
+      </c>
+      <c r="I85" s="23">
+        <f t="shared" si="21"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="66"/>
+      <c r="D86" s="67"/>
+      <c r="E86" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="F86" s="57"/>
+      <c r="G86" s="11">
+        <f>SUM(G87,G89,G93)</f>
+        <v>7</v>
+      </c>
+      <c r="H86" s="57"/>
+      <c r="I86" s="16"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="69"/>
+      <c r="B87" s="72"/>
+      <c r="C87" s="60"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="F87" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="G87" s="56">
+        <f>SUM(G88:G88)</f>
+        <v>2</v>
+      </c>
+      <c r="H87" s="56">
+        <f>SUM(H88:H88)</f>
+        <v>0</v>
+      </c>
+      <c r="I87" s="21">
+        <f t="shared" ref="I87:I90" si="23">G87-H87</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="69"/>
+      <c r="B88" s="72"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G88" s="4">
+        <v>2</v>
+      </c>
+      <c r="H88" s="4">
+        <v>0</v>
+      </c>
+      <c r="I88" s="23">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="69"/>
+      <c r="B89" s="72"/>
+      <c r="C89" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="D89" s="61"/>
+      <c r="E89" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F89" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="G83" s="57">
-        <f>SUM(G84)</f>
-        <v>0</v>
-      </c>
-      <c r="H83" s="57">
-        <f t="shared" ref="H83:I83" si="22">SUM(H84)</f>
-        <v>0</v>
-      </c>
-      <c r="I83" s="57">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="67"/>
-      <c r="B84" s="96"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="98" t="s">
-        <v>149</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="G89" s="56">
+        <f>SUM(G90)</f>
+        <v>5</v>
+      </c>
+      <c r="H89" s="56">
+        <f t="shared" ref="H89" si="24">SUM(H90)</f>
+        <v>0</v>
+      </c>
+      <c r="I89" s="21">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="69"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G84" s="2">
-        <v>0</v>
-      </c>
-      <c r="H84" s="2">
-        <v>0</v>
-      </c>
-      <c r="I84" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="65" t="s">
+      <c r="G90" s="2">
+        <v>5</v>
+      </c>
+      <c r="H90" s="2">
+        <v>0</v>
+      </c>
+      <c r="I90" s="23">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="69"/>
+      <c r="B91" s="72"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G91" s="2">
+        <v>3</v>
+      </c>
+      <c r="H91" s="2">
+        <v>0</v>
+      </c>
+      <c r="I91" s="23">
+        <f t="shared" ref="I91" si="25">G91-H91</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="69"/>
+      <c r="B92" s="72"/>
+      <c r="C92" s="58"/>
+      <c r="D92" s="59"/>
+      <c r="E92" s="59"/>
+      <c r="F92" s="59"/>
+      <c r="G92" s="59"/>
+      <c r="H92" s="59"/>
+      <c r="I92" s="98"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="69"/>
+      <c r="B93" s="72"/>
+      <c r="C93" s="82" t="s">
+        <v>164</v>
+      </c>
+      <c r="D93" s="83"/>
+      <c r="E93" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F93" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="G93" s="49">
+        <v>0</v>
+      </c>
+      <c r="H93" s="49">
+        <f>SUM(0)</f>
+        <v>0</v>
+      </c>
+      <c r="I93" s="50">
+        <f>SUM(0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="69"/>
+      <c r="B94" s="72"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G94" s="2">
+        <v>8</v>
+      </c>
+      <c r="H94" s="2">
+        <v>0</v>
+      </c>
+      <c r="I94" s="23">
+        <f>G94-H94</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="69"/>
+      <c r="B95" s="72"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" s="2">
+        <v>4</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0</v>
+      </c>
+      <c r="I95" s="23">
+        <f>G95-H95</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="69"/>
+      <c r="B96" s="72"/>
+      <c r="C96" s="34"/>
+      <c r="D96" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G96" s="4">
         <v>12</v>
       </c>
-      <c r="B85" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" s="83"/>
-      <c r="D85" s="84"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="11">
-        <f>80</f>
-        <v>80</v>
-      </c>
-      <c r="H85" s="32"/>
-      <c r="I85" s="19"/>
-    </row>
-    <row r="86" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="67"/>
-      <c r="B86" s="82"/>
-      <c r="C86" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="D86" s="88"/>
-      <c r="E86" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="F86" s="54" t="s">
+      <c r="H96" s="2">
+        <v>0</v>
+      </c>
+      <c r="I96" s="23">
+        <f>G96-H96</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="69"/>
+      <c r="B97" s="72"/>
+      <c r="C97" s="34"/>
+      <c r="D97" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G86" s="54">
-        <v>0</v>
-      </c>
-      <c r="H86" s="54">
-        <f>SUM(0)</f>
-        <v>0</v>
-      </c>
-      <c r="I86" s="55">
-        <f>SUM(0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="30" t="s">
+      <c r="G97" s="4">
+        <v>8</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0</v>
+      </c>
+      <c r="I97" s="23">
+        <f>G97-H97</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="69"/>
+      <c r="B98" s="72"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G98" s="4">
+        <v>4</v>
+      </c>
+      <c r="H98" s="4">
+        <v>0</v>
+      </c>
+      <c r="I98" s="23">
+        <f t="shared" ref="I98" si="26">G98-H98</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="70"/>
+      <c r="B99" s="73"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="54"/>
+      <c r="E99" s="54"/>
+      <c r="F99" s="54"/>
+      <c r="G99" s="54"/>
+      <c r="H99" s="54"/>
+      <c r="I99" s="55"/>
+    </row>
+    <row r="100" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B87" s="51" t="s">
+      <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="89"/>
-      <c r="D87" s="90"/>
-      <c r="E87" s="52"/>
-      <c r="F87" s="52"/>
-      <c r="G87" s="52"/>
-      <c r="H87" s="52"/>
-      <c r="I87" s="53"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="54"/>
+      <c r="E100" s="54"/>
+      <c r="F100" s="54"/>
+      <c r="G100" s="54"/>
+      <c r="H100" s="54"/>
+      <c r="I100" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A56:A73"/>
-    <mergeCell ref="B56:B73"/>
-    <mergeCell ref="A43:A55"/>
-    <mergeCell ref="B43:B55"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C46:D46"/>
+  <mergeCells count="44">
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A21:A42"/>
     <mergeCell ref="B21:B42"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C86:D87"/>
-    <mergeCell ref="A74:A84"/>
-    <mergeCell ref="B74:B84"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C36:D36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C3:D3"/>
@@ -3898,9 +4233,38 @@
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A86:A99"/>
+    <mergeCell ref="B86:B99"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A74:A85"/>
+    <mergeCell ref="B74:B85"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A56:A73"/>
+    <mergeCell ref="B56:B73"/>
+    <mergeCell ref="A43:A55"/>
+    <mergeCell ref="B43:B55"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F86">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F91 F93:F98">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Sprint 7 and add tasks to Sprint 8
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12480" windowHeight="6870"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
   <si>
     <t>11.09.18</t>
   </si>
@@ -496,9 +496,6 @@
     <t xml:space="preserve"> [Continue] Security Issue</t>
   </si>
   <si>
-    <t>Create popup dialog "Order is sucsessful"</t>
-  </si>
-  <si>
     <t>TA57</t>
   </si>
   <si>
@@ -520,9 +517,6 @@
     <t>TA62</t>
   </si>
   <si>
-    <t>Add new model to backend</t>
-  </si>
-  <si>
     <t>US15</t>
   </si>
   <si>
@@ -545,6 +539,69 @@
   </si>
   <si>
     <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>Create 1 function in action (post 1 object with order and items). Add new model for NewOrder in api. Delete POST method in ItemsOfOrdersController</t>
+  </si>
+  <si>
+    <t>Create UI "Order is sucsessful"</t>
+  </si>
+  <si>
+    <t>TA63</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Update product`s amount after create order</t>
+  </si>
+  <si>
+    <t>TA64</t>
+  </si>
+  <si>
+    <t>New function for UI for successful order. Clear state`s parameters after create order.</t>
+  </si>
+  <si>
+    <t>Add new column in db.Poducts. Update DB</t>
+  </si>
+  <si>
+    <t>If product.amount=0 then "add to cart" is disabled</t>
+  </si>
+  <si>
+    <t>Amend to frontend and backend functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amend UI "Order is sucsessful" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amend validation "items is sucsessful" </t>
+  </si>
+  <si>
+    <t>Amend functionality of browse pictures to products</t>
+  </si>
+  <si>
+    <t>Sprint 8</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
+  <si>
+    <t>TA65</t>
+  </si>
+  <si>
+    <t>TA66</t>
+  </si>
+  <si>
+    <t>TA67</t>
+  </si>
+  <si>
+    <t>TA68</t>
+  </si>
+  <si>
+    <t>TA69</t>
+  </si>
+  <si>
+    <t>[NN] Add enter field for product`s amount</t>
   </si>
 </sst>
 </file>
@@ -612,7 +669,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1131,30 +1188,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1185,21 +1218,23 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1209,7 +1244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1289,9 +1324,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1355,93 +1387,132 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1457,58 +1528,11 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1792,11 +1816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:U107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,40 +1837,40 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="41" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="84" t="s">
+    <row r="1" spans="1:21" s="40" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="42" t="s">
+      <c r="D1" s="68"/>
+      <c r="E1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
+      <c r="B2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
       <c r="E2" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11">
@@ -1854,15 +1878,15 @@
         <v>28</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="36"/>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="87" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="88"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="17" t="s">
         <v>19</v>
       </c>
@@ -1877,15 +1901,15 @@
         <f>SUM(H4:H8)</f>
         <v>20</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="36">
         <f>SUM(I4:I8)</f>
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1910,9 +1934,9 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="32"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1937,9 +1961,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="33"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1964,9 +1988,9 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1991,8 +2015,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="70"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="25"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
@@ -2015,16 +2039,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="92"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
       <c r="E9" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13">
@@ -2032,17 +2056,17 @@
         <v>38</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="39"/>
+      <c r="I9" s="38"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="87" t="s">
+      <c r="A10" s="61"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="88"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="17" t="s">
         <v>19</v>
       </c>
@@ -2057,14 +2081,14 @@
         <f>SUM(H11:H15)</f>
         <v>36</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="36">
         <f>SUM(I11:I15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="22"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -2087,8 +2111,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="22"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
@@ -2111,9 +2135,9 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
@@ -2135,12 +2159,12 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="60" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="61"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="20" t="s">
         <v>50</v>
       </c>
@@ -2161,8 +2185,8 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="69"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="22"/>
       <c r="D15" s="2" t="s">
         <v>42</v>
@@ -2185,8 +2209,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
-      <c r="B16" s="72"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="22"/>
       <c r="D16" s="2" t="s">
         <v>43</v>
@@ -2209,12 +2233,12 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="93" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="94"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="18" t="s">
         <v>51</v>
       </c>
@@ -2229,14 +2253,14 @@
         <f t="shared" ref="H17:I17" si="1">SUM(H18:H20)</f>
         <v>3</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="30">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="69"/>
-      <c r="B18" s="72"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="22"/>
       <c r="D18" s="2" t="s">
         <v>47</v>
@@ -2259,9 +2283,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="69"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="32"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="2" t="s">
         <v>66</v>
       </c>
@@ -2286,16 +2310,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="69"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="35"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="39" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="7">
@@ -2309,16 +2333,16 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="68" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="71" t="s">
+      <c r="A21" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="96"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="15">
@@ -2326,15 +2350,15 @@
         <v>76</v>
       </c>
       <c r="H21" s="15"/>
-      <c r="I21" s="30"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="69"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="62" t="s">
+      <c r="A22" s="61"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="63"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="18" t="s">
         <v>74</v>
       </c>
@@ -2349,14 +2373,14 @@
         <f t="shared" ref="H22:I22" si="2">SUM(H23:H26)</f>
         <v>3.25</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="30">
         <f t="shared" si="2"/>
         <v>2.75</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="69"/>
-      <c r="B23" s="72"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="64"/>
       <c r="C23" s="22"/>
       <c r="D23" s="2" t="s">
         <v>53</v>
@@ -2379,8 +2403,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="69"/>
-      <c r="B24" s="72"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="64"/>
       <c r="C24" s="22"/>
       <c r="D24" s="2" t="s">
         <v>54</v>
@@ -2403,8 +2427,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
-      <c r="B25" s="72"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="64"/>
       <c r="C25" s="22"/>
       <c r="D25" s="2" t="s">
         <v>55</v>
@@ -2427,8 +2451,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
-      <c r="B26" s="72"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="64"/>
       <c r="C26" s="22"/>
       <c r="D26" s="2" t="s">
         <v>56</v>
@@ -2451,12 +2475,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="62" t="s">
+      <c r="A27" s="61"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="63"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="18" t="s">
         <v>85</v>
       </c>
@@ -2471,14 +2495,14 @@
         <f ca="1">SUM(H25:H35)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="31">
+      <c r="I27" s="30">
         <f ca="1">SUM(I25:I35)</f>
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
-      <c r="B28" s="72"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="64"/>
       <c r="C28" s="22"/>
       <c r="D28" s="2" t="s">
         <v>57</v>
@@ -2501,8 +2525,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
-      <c r="B29" s="72"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="64"/>
       <c r="C29" s="22"/>
       <c r="D29" s="2" t="s">
         <v>63</v>
@@ -2524,8 +2548,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
-      <c r="B30" s="72"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="22"/>
       <c r="D30" s="2" t="s">
         <v>68</v>
@@ -2551,8 +2575,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="69"/>
-      <c r="B31" s="72"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="22"/>
       <c r="D31" s="2" t="s">
         <v>75</v>
@@ -2578,9 +2602,9 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="32"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="2" t="s">
         <v>76</v>
       </c>
@@ -2602,9 +2626,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="69"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="32"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
@@ -2626,9 +2650,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="32"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="2" t="s">
         <v>79</v>
       </c>
@@ -2650,9 +2674,9 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="33"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="4" t="s">
         <v>80</v>
       </c>
@@ -2674,12 +2698,12 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="64" t="s">
+      <c r="A36" s="61"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="65"/>
+      <c r="D36" s="87"/>
       <c r="E36" s="20" t="s">
         <v>90</v>
       </c>
@@ -2700,8 +2724,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
-      <c r="B37" s="72"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="64"/>
       <c r="C37" s="22"/>
       <c r="D37" s="2" t="s">
         <v>86</v>
@@ -2724,9 +2748,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="69"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="34"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="33"/>
       <c r="D38" s="4" t="s">
         <v>87</v>
       </c>
@@ -2748,12 +2772,12 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="69"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="64" t="s">
+      <c r="A39" s="61"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="65"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="20" t="s">
         <v>67</v>
       </c>
@@ -2774,9 +2798,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="69"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="32"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="31"/>
       <c r="D40" s="2" t="s">
         <v>93</v>
       </c>
@@ -2798,9 +2822,9 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="69"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="32"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="31"/>
       <c r="D41" s="2" t="s">
         <v>94</v>
       </c>
@@ -2822,9 +2846,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="70"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="35"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="34"/>
       <c r="D42" s="7" t="s">
         <v>88</v>
       </c>
@@ -2845,18 +2869,18 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="80" t="s">
+      <c r="B43" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="66"/>
-      <c r="D43" s="67"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="80"/>
       <c r="E43" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" s="29"/>
+        <v>166</v>
+      </c>
+      <c r="F43" s="28"/>
       <c r="G43" s="11">
         <f>SUM(G44,G46)</f>
         <v>48.5</v>
@@ -2868,23 +2892,23 @@
       <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="69"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="64" t="s">
+      <c r="A44" s="61"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="65"/>
-      <c r="E44" s="28" t="s">
+      <c r="D44" s="87"/>
+      <c r="E44" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="28">
+      <c r="G44" s="27">
         <f>SUM(G45:G45)</f>
         <v>8</v>
       </c>
-      <c r="H44" s="28">
+      <c r="H44" s="27">
         <f t="shared" ref="H44:I44" si="12">SUM(H45:H45)</f>
         <v>0</v>
       </c>
@@ -2894,9 +2918,9 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="69"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="32"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="31"/>
       <c r="D45" s="2" t="s">
         <v>100</v>
       </c>
@@ -2918,23 +2942,23 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="69"/>
-      <c r="B46" s="81"/>
-      <c r="C46" s="64" t="s">
+      <c r="A46" s="61"/>
+      <c r="B46" s="92"/>
+      <c r="C46" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="28" t="s">
+      <c r="D46" s="87"/>
+      <c r="E46" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="28" t="s">
+      <c r="F46" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G46" s="28">
+      <c r="G46" s="27">
         <f>SUM(G47:G54)</f>
         <v>40.5</v>
       </c>
-      <c r="H46" s="28">
+      <c r="H46" s="27">
         <f>SUM(H47:H54)</f>
         <v>37.5</v>
       </c>
@@ -2944,8 +2968,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="69"/>
-      <c r="B47" s="81"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="92"/>
       <c r="C47" s="22"/>
       <c r="D47" s="2" t="s">
         <v>101</v>
@@ -2968,8 +2992,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="69"/>
-      <c r="B48" s="81"/>
+      <c r="A48" s="61"/>
+      <c r="B48" s="92"/>
       <c r="C48" s="22"/>
       <c r="D48" s="2" t="s">
         <v>102</v>
@@ -2992,9 +3016,9 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="69"/>
-      <c r="B49" s="81"/>
-      <c r="C49" s="34"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="92"/>
+      <c r="C49" s="33"/>
       <c r="D49" s="2" t="s">
         <v>103</v>
       </c>
@@ -3016,9 +3040,9 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="69"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="38"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="92"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="2" t="s">
         <v>104</v>
       </c>
@@ -3038,12 +3062,12 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="J50" s="44"/>
+      <c r="J50" s="43"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="69"/>
-      <c r="B51" s="81"/>
-      <c r="C51" s="45"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="92"/>
+      <c r="C51" s="44"/>
       <c r="D51" s="2" t="s">
         <v>109</v>
       </c>
@@ -3065,9 +3089,9 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="69"/>
-      <c r="B52" s="81"/>
-      <c r="C52" s="45"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="92"/>
+      <c r="C52" s="44"/>
       <c r="D52" s="2" t="s">
         <v>110</v>
       </c>
@@ -3089,21 +3113,21 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="69"/>
-      <c r="B53" s="81"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="28" t="s">
+      <c r="A53" s="61"/>
+      <c r="B53" s="92"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="28" t="s">
+      <c r="F53" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G53" s="28">
+      <c r="G53" s="27">
         <f>SUM(G54:G55)</f>
         <v>4.5</v>
       </c>
-      <c r="H53" s="28">
+      <c r="H53" s="27">
         <f>SUM(H54:H55)</f>
         <v>5.5</v>
       </c>
@@ -3113,8 +3137,8 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="69"/>
-      <c r="B54" s="81"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="92"/>
       <c r="C54" s="22"/>
       <c r="D54" s="2" t="s">
         <v>115</v>
@@ -3137,8 +3161,8 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="69"/>
-      <c r="B55" s="81"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="92"/>
       <c r="C55" s="25"/>
       <c r="D55" s="7" t="s">
         <v>116</v>
@@ -3161,18 +3185,18 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="77" t="s">
+      <c r="A56" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="66"/>
-      <c r="D56" s="67"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="80"/>
       <c r="E56" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="F56" s="29"/>
+        <v>167</v>
+      </c>
+      <c r="F56" s="28"/>
       <c r="G56" s="11">
         <f>SUM(G57,G64,G67)</f>
         <v>61</v>
@@ -3184,23 +3208,23 @@
       <c r="I56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="69"/>
-      <c r="B57" s="78"/>
-      <c r="C57" s="64" t="s">
+      <c r="A57" s="61"/>
+      <c r="B57" s="89"/>
+      <c r="C57" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="D57" s="65"/>
-      <c r="E57" s="28" t="s">
+      <c r="D57" s="87"/>
+      <c r="E57" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="28" t="s">
+      <c r="F57" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G57" s="28">
+      <c r="G57" s="27">
         <f>SUM(G58:G63)</f>
         <v>44</v>
       </c>
-      <c r="H57" s="28">
+      <c r="H57" s="27">
         <f>SUM(H58:H85)</f>
         <v>114.5</v>
       </c>
@@ -3210,9 +3234,9 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="69"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="32"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="89"/>
+      <c r="C58" s="31"/>
       <c r="D58" s="2" t="s">
         <v>111</v>
       </c>
@@ -3234,9 +3258,9 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="69"/>
-      <c r="B59" s="78"/>
-      <c r="C59" s="32"/>
+      <c r="A59" s="61"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="31"/>
       <c r="D59" s="2" t="s">
         <v>113</v>
       </c>
@@ -3258,9 +3282,9 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="69"/>
-      <c r="B60" s="78"/>
-      <c r="C60" s="32"/>
+      <c r="A60" s="61"/>
+      <c r="B60" s="89"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="2" t="s">
         <v>119</v>
       </c>
@@ -3282,9 +3306,9 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="69"/>
-      <c r="B61" s="78"/>
-      <c r="C61" s="32"/>
+      <c r="A61" s="61"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="31"/>
       <c r="D61" s="2" t="s">
         <v>120</v>
       </c>
@@ -3306,9 +3330,9 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="69"/>
-      <c r="B62" s="78"/>
-      <c r="C62" s="32"/>
+      <c r="A62" s="61"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="2" t="s">
         <v>125</v>
       </c>
@@ -3330,8 +3354,8 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="69"/>
-      <c r="B63" s="78"/>
+      <c r="A63" s="61"/>
+      <c r="B63" s="89"/>
       <c r="C63" s="22" t="s">
         <v>132</v>
       </c>
@@ -3356,23 +3380,23 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="69"/>
-      <c r="B64" s="78"/>
-      <c r="C64" s="64" t="s">
+      <c r="A64" s="61"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="65"/>
-      <c r="E64" s="28" t="s">
+      <c r="D64" s="87"/>
+      <c r="E64" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="F64" s="28" t="s">
+      <c r="F64" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G64" s="28">
+      <c r="G64" s="27">
         <f>SUM(G65:G66)</f>
         <v>8</v>
       </c>
-      <c r="H64" s="28">
+      <c r="H64" s="27">
         <f t="shared" ref="H64:I64" si="15">SUM(H65:H66)</f>
         <v>6</v>
       </c>
@@ -3382,8 +3406,8 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="69"/>
-      <c r="B65" s="78"/>
+      <c r="A65" s="61"/>
+      <c r="B65" s="89"/>
       <c r="C65" s="22"/>
       <c r="D65" s="2" t="s">
         <v>129</v>
@@ -3406,8 +3430,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="69"/>
-      <c r="B66" s="78"/>
+      <c r="A66" s="61"/>
+      <c r="B66" s="89"/>
       <c r="C66" s="22"/>
       <c r="D66" s="2" t="s">
         <v>130</v>
@@ -3430,21 +3454,21 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="69"/>
-      <c r="B67" s="78"/>
-      <c r="C67" s="60"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="28" t="s">
+      <c r="A67" s="61"/>
+      <c r="B67" s="89"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="72"/>
+      <c r="E67" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F67" s="28" t="s">
+      <c r="F67" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G67" s="28">
+      <c r="G67" s="27">
         <f>SUM(G68:G69)</f>
         <v>9</v>
       </c>
-      <c r="H67" s="28">
+      <c r="H67" s="27">
         <f t="shared" ref="H67:I67" si="17">SUM(H68:H69)</f>
         <v>8</v>
       </c>
@@ -3454,8 +3478,8 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="69"/>
-      <c r="B68" s="78"/>
+      <c r="A68" s="61"/>
+      <c r="B68" s="89"/>
       <c r="C68" s="22"/>
       <c r="D68" s="2" t="s">
         <v>115</v>
@@ -3478,9 +3502,9 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="69"/>
-      <c r="B69" s="78"/>
-      <c r="C69" s="32"/>
+      <c r="A69" s="61"/>
+      <c r="B69" s="89"/>
+      <c r="C69" s="31"/>
       <c r="D69" s="2" t="s">
         <v>116</v>
       </c>
@@ -3501,23 +3525,23 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="69"/>
-      <c r="B70" s="78"/>
-      <c r="C70" s="60" t="s">
+      <c r="A70" s="61"/>
+      <c r="B70" s="89"/>
+      <c r="C70" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="61"/>
-      <c r="E70" s="28" t="s">
+      <c r="D70" s="72"/>
+      <c r="E70" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="F70" s="28" t="s">
+      <c r="F70" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G70" s="28">
+      <c r="G70" s="27">
         <f>SUM(G71:G73)</f>
         <v>24</v>
       </c>
-      <c r="H70" s="28">
+      <c r="H70" s="27">
         <f t="shared" ref="H70" si="18">SUM(H71:H74)</f>
         <v>28</v>
       </c>
@@ -3527,8 +3551,8 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="69"/>
-      <c r="B71" s="78"/>
+      <c r="A71" s="61"/>
+      <c r="B71" s="89"/>
       <c r="C71" s="22"/>
       <c r="D71" s="2" t="s">
         <v>134</v>
@@ -3550,13 +3574,13 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="69"/>
-      <c r="B72" s="78"/>
+      <c r="A72" s="61"/>
+      <c r="B72" s="89"/>
       <c r="C72" s="22"/>
       <c r="D72" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E72" s="46" t="s">
+      <c r="E72" s="45" t="s">
         <v>139</v>
       </c>
       <c r="F72" s="2" t="s">
@@ -3573,13 +3597,13 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="70"/>
-      <c r="B73" s="79"/>
+      <c r="A73" s="62"/>
+      <c r="B73" s="90"/>
       <c r="C73" s="25"/>
-      <c r="D73" s="40" t="s">
+      <c r="D73" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="E73" s="47" t="s">
+      <c r="E73" s="46" t="s">
         <v>141</v>
       </c>
       <c r="F73" s="7" t="s">
@@ -3596,18 +3620,18 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="68" t="s">
+      <c r="A74" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="74" t="s">
+      <c r="B74" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="C74" s="66"/>
-      <c r="D74" s="67"/>
+      <c r="C74" s="79"/>
+      <c r="D74" s="80"/>
       <c r="E74" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F74" s="52"/>
+        <v>168</v>
+      </c>
+      <c r="F74" s="48"/>
       <c r="G74" s="11">
         <f>SUM(G75)</f>
         <v>36</v>
@@ -3619,23 +3643,23 @@
       <c r="I74" s="16"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="69"/>
-      <c r="B75" s="75"/>
-      <c r="C75" s="64" t="s">
+      <c r="A75" s="61"/>
+      <c r="B75" s="84"/>
+      <c r="C75" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="D75" s="65"/>
-      <c r="E75" s="51" t="s">
+      <c r="D75" s="87"/>
+      <c r="E75" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="F75" s="51" t="s">
+      <c r="F75" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="G75" s="51">
+      <c r="G75" s="47">
         <f>SUM(G76:G80)</f>
         <v>36</v>
       </c>
-      <c r="H75" s="51">
+      <c r="H75" s="47">
         <f t="shared" ref="H75:I75" si="20">SUM(H76:H80)</f>
         <v>0</v>
       </c>
@@ -3645,8 +3669,8 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="69"/>
-      <c r="B76" s="75"/>
+      <c r="A76" s="61"/>
+      <c r="B76" s="84"/>
       <c r="C76" s="22"/>
       <c r="D76" s="2" t="s">
         <v>143</v>
@@ -3669,8 +3693,8 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="69"/>
-      <c r="B77" s="75"/>
+      <c r="A77" s="61"/>
+      <c r="B77" s="84"/>
       <c r="C77" s="22"/>
       <c r="D77" s="2" t="s">
         <v>144</v>
@@ -3693,9 +3717,9 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="69"/>
-      <c r="B78" s="75"/>
-      <c r="C78" s="32"/>
+      <c r="A78" s="61"/>
+      <c r="B78" s="84"/>
+      <c r="C78" s="31"/>
       <c r="D78" s="2" t="s">
         <v>145</v>
       </c>
@@ -3717,8 +3741,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="69"/>
-      <c r="B79" s="75"/>
+      <c r="A79" s="61"/>
+      <c r="B79" s="84"/>
       <c r="C79" s="22"/>
       <c r="D79" s="2" t="s">
         <v>146</v>
@@ -3741,8 +3765,8 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="69"/>
-      <c r="B80" s="75"/>
+      <c r="A80" s="61"/>
+      <c r="B80" s="84"/>
       <c r="C80" s="22"/>
       <c r="D80" s="2" t="s">
         <v>147</v>
@@ -3765,21 +3789,21 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="69"/>
-      <c r="B81" s="75"/>
-      <c r="C81" s="60"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="51" t="s">
+      <c r="A81" s="61"/>
+      <c r="B81" s="84"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="72"/>
+      <c r="E81" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="F81" s="51" t="s">
+      <c r="F81" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="51">
+      <c r="G81" s="47">
         <f>SUM(G82:G82)</f>
         <v>5</v>
       </c>
-      <c r="H81" s="51">
+      <c r="H81" s="47">
         <f>SUM(H82:H82)</f>
         <v>6</v>
       </c>
@@ -3789,9 +3813,9 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="69"/>
-      <c r="B82" s="75"/>
-      <c r="C82" s="32"/>
+      <c r="A82" s="61"/>
+      <c r="B82" s="84"/>
+      <c r="C82" s="31"/>
       <c r="D82" s="4" t="s">
         <v>115</v>
       </c>
@@ -3816,9 +3840,9 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="69"/>
-      <c r="B83" s="75"/>
-      <c r="C83" s="53"/>
+      <c r="A83" s="61"/>
+      <c r="B83" s="84"/>
+      <c r="C83" s="49"/>
       <c r="D83" s="2" t="s">
         <v>116</v>
       </c>
@@ -3840,23 +3864,23 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="69"/>
-      <c r="B84" s="75"/>
-      <c r="C84" s="60" t="s">
+      <c r="A84" s="61"/>
+      <c r="B84" s="84"/>
+      <c r="C84" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="D84" s="61"/>
-      <c r="E84" s="51" t="s">
+      <c r="D84" s="72"/>
+      <c r="E84" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="F84" s="51" t="s">
+      <c r="F84" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G84" s="51">
+      <c r="G84" s="47">
         <f>SUM(G85)</f>
         <v>5</v>
       </c>
-      <c r="H84" s="51">
+      <c r="H84" s="47">
         <f t="shared" ref="H84" si="22">SUM(H85)</f>
         <v>9</v>
       </c>
@@ -3866,8 +3890,8 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="70"/>
-      <c r="B85" s="76"/>
+      <c r="A85" s="62"/>
+      <c r="B85" s="85"/>
       <c r="C85" s="25"/>
       <c r="D85" s="7" t="s">
         <v>149</v>
@@ -3890,52 +3914,55 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="68" t="s">
+      <c r="A86" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="71" t="s">
+      <c r="B86" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="66"/>
-      <c r="D86" s="67"/>
-      <c r="E86" s="97" t="s">
-        <v>171</v>
-      </c>
-      <c r="F86" s="57"/>
+      <c r="C86" s="79"/>
+      <c r="D86" s="80"/>
+      <c r="E86" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="F86" s="51"/>
       <c r="G86" s="11">
-        <f>SUM(G87,G89,G93)</f>
-        <v>7</v>
-      </c>
-      <c r="H86" s="57"/>
+        <f>SUM(G87,G89,G102)</f>
+        <v>56</v>
+      </c>
+      <c r="H86" s="11">
+        <f>SUM(H87,H89,H102)</f>
+        <v>27.5</v>
+      </c>
       <c r="I86" s="16"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="69"/>
-      <c r="B87" s="72"/>
-      <c r="C87" s="60"/>
-      <c r="D87" s="61"/>
-      <c r="E87" s="56" t="s">
+      <c r="A87" s="61"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="72"/>
+      <c r="E87" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="F87" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="G87" s="56">
+      <c r="F87" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="G87" s="50">
         <f>SUM(G88:G88)</f>
         <v>2</v>
       </c>
-      <c r="H87" s="56">
+      <c r="H87" s="50">
         <f>SUM(H88:H88)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I87" s="21">
         <f t="shared" ref="I87:I90" si="23">G87-H87</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="69"/>
-      <c r="B88" s="72"/>
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="61"/>
+      <c r="B88" s="64"/>
       <c r="C88" s="22"/>
       <c r="D88" s="4" t="s">
         <v>115</v>
@@ -3944,280 +3971,515 @@
         <v>154</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G88" s="4">
         <v>2</v>
       </c>
       <c r="H88" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I88" s="23">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>-13</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="69"/>
-      <c r="B89" s="72"/>
-      <c r="C89" s="60" t="s">
+      <c r="A89" s="61"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="D89" s="61"/>
-      <c r="E89" s="56" t="s">
+      <c r="D89" s="72"/>
+      <c r="E89" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="F89" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="G89" s="56">
-        <f>SUM(G90)</f>
-        <v>5</v>
-      </c>
-      <c r="H89" s="56">
-        <f t="shared" ref="H89" si="24">SUM(H90)</f>
-        <v>0</v>
-      </c>
-      <c r="I89" s="21">
-        <f t="shared" si="23"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="69"/>
-      <c r="B90" s="72"/>
+      <c r="F89" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="G89" s="50">
+        <f>SUM(G90:G94)</f>
+        <v>18</v>
+      </c>
+      <c r="H89" s="53">
+        <f t="shared" ref="H89:I89" si="24">SUM(H90:H94)</f>
+        <v>12.5</v>
+      </c>
+      <c r="I89" s="53">
+        <f t="shared" si="24"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="61"/>
+      <c r="B90" s="64"/>
       <c r="C90" s="22"/>
       <c r="D90" s="2" t="s">
         <v>153</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G90" s="2">
         <v>5</v>
       </c>
       <c r="H90" s="2">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I90" s="23">
         <f t="shared" si="23"/>
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="69"/>
-      <c r="B91" s="72"/>
-      <c r="C91" s="58"/>
+      <c r="A91" s="61"/>
+      <c r="B91" s="64"/>
+      <c r="C91" s="95"/>
       <c r="D91" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E91" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="F91" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G91" s="2">
         <v>3</v>
       </c>
       <c r="H91" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I91" s="23">
-        <f t="shared" ref="I91" si="25">G91-H91</f>
+        <f t="shared" ref="I91:I92" si="25">G91-H91</f>
+        <v>-3</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="61"/>
+      <c r="B92" s="64"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G92" s="2">
+        <v>4</v>
+      </c>
+      <c r="H92" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="69"/>
-      <c r="B92" s="72"/>
-      <c r="C92" s="58"/>
-      <c r="D92" s="59"/>
-      <c r="E92" s="59"/>
-      <c r="F92" s="59"/>
-      <c r="G92" s="59"/>
-      <c r="H92" s="59"/>
-      <c r="I92" s="98"/>
+      <c r="I92" s="23">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="69"/>
-      <c r="B93" s="72"/>
-      <c r="C93" s="82" t="s">
-        <v>164</v>
-      </c>
-      <c r="D93" s="83"/>
-      <c r="E93" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="F93" s="56" t="s">
+      <c r="A93" s="61"/>
+      <c r="B93" s="64"/>
+      <c r="C93" s="93" t="s">
+        <v>173</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F93" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G93" s="49">
-        <v>0</v>
-      </c>
-      <c r="H93" s="49">
-        <f>SUM(0)</f>
-        <v>0</v>
-      </c>
-      <c r="I93" s="50">
-        <f>SUM(0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="69"/>
-      <c r="B94" s="72"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F94" s="9" t="s">
+      <c r="G93" s="4">
+        <v>5</v>
+      </c>
+      <c r="H93" s="4">
+        <v>0</v>
+      </c>
+      <c r="I93" s="24">
+        <f t="shared" ref="I93" si="26">G93-H93</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="55"/>
+      <c r="B94" s="56"/>
+      <c r="C94" s="94"/>
+      <c r="D94" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G94" s="7">
+        <v>1</v>
+      </c>
+      <c r="H94" s="7">
+        <v>0</v>
+      </c>
+      <c r="I94" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="79"/>
+      <c r="D95" s="80"/>
+      <c r="E95" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F95" s="54"/>
+      <c r="G95" s="11">
+        <f>SUM(G96,G98,G110)</f>
+        <v>26</v>
+      </c>
+      <c r="H95" s="11">
+        <f>SUM(H96,H98,H110)</f>
+        <v>0</v>
+      </c>
+      <c r="I95" s="16"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="61"/>
+      <c r="B96" s="84"/>
+      <c r="C96" s="86" t="s">
+        <v>142</v>
+      </c>
+      <c r="D96" s="87"/>
+      <c r="E96" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="F96" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G94" s="2">
-        <v>8</v>
-      </c>
-      <c r="H94" s="2">
-        <v>0</v>
-      </c>
-      <c r="I94" s="23">
-        <f>G94-H94</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="69"/>
-      <c r="B95" s="72"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G95" s="2">
-        <v>4</v>
-      </c>
-      <c r="H95" s="2">
-        <v>0</v>
-      </c>
-      <c r="I95" s="23">
-        <f>G95-H95</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="69"/>
-      <c r="B96" s="72"/>
-      <c r="C96" s="34"/>
-      <c r="D96" s="2" t="s">
+      <c r="G96" s="53">
+        <f>SUM(G97:G100)</f>
+        <v>21</v>
+      </c>
+      <c r="H96" s="53">
+        <f>SUM(H97:H100)</f>
+        <v>0</v>
+      </c>
+      <c r="I96" s="21">
+        <f>SUM(I97:I100)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="61"/>
+      <c r="B97" s="84"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E96" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G96" s="4">
-        <v>12</v>
-      </c>
-      <c r="H96" s="2">
-        <v>0</v>
-      </c>
-      <c r="I96" s="23">
-        <f>G96-H96</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="69"/>
-      <c r="B97" s="72"/>
-      <c r="C97" s="34"/>
-      <c r="D97" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E97" s="14" t="s">
-        <v>62</v>
+      <c r="E97" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G97" s="4">
-        <v>8</v>
+      <c r="G97" s="2">
+        <v>6</v>
       </c>
       <c r="H97" s="2">
         <v>0</v>
       </c>
       <c r="I97" s="23">
         <f>G97-H97</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="69"/>
-      <c r="B98" s="72"/>
-      <c r="C98" s="34"/>
+      <c r="A98" s="61"/>
+      <c r="B98" s="84"/>
+      <c r="C98" s="22"/>
       <c r="D98" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G98" s="2">
+        <v>5</v>
+      </c>
+      <c r="H98" s="2">
+        <v>0</v>
+      </c>
+      <c r="I98" s="23">
+        <f t="shared" ref="I98:I100" si="27">G98-H98</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="61"/>
+      <c r="B99" s="84"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G99" s="2">
+        <v>5</v>
+      </c>
+      <c r="H99" s="2">
+        <v>0</v>
+      </c>
+      <c r="I99" s="23">
+        <f>G99-H99</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="61"/>
+      <c r="B100" s="84"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G100" s="2">
+        <v>5</v>
+      </c>
+      <c r="H100" s="2">
+        <v>0</v>
+      </c>
+      <c r="I100" s="23">
+        <f t="shared" si="27"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="61"/>
+      <c r="B101" s="84"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="23"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="61"/>
+      <c r="B102" s="84"/>
+      <c r="C102" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="E98" s="14" t="s">
+      <c r="D102" s="87"/>
+      <c r="E102" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="F102" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" s="53">
+        <f>SUM(G103:G107)</f>
+        <v>36</v>
+      </c>
+      <c r="H102" s="53">
+        <f t="shared" ref="H102:I102" si="28">SUM(H103:H107)</f>
+        <v>0</v>
+      </c>
+      <c r="I102" s="21">
+        <f t="shared" si="28"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="61"/>
+      <c r="B103" s="84"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G103" s="2">
+        <v>8</v>
+      </c>
+      <c r="H103" s="2">
+        <v>0</v>
+      </c>
+      <c r="I103" s="23">
+        <f>G103-H103</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="61"/>
+      <c r="B104" s="84"/>
+      <c r="C104" s="22"/>
+      <c r="D104" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G104" s="2">
+        <v>4</v>
+      </c>
+      <c r="H104" s="2">
+        <v>0</v>
+      </c>
+      <c r="I104" s="23">
+        <f>G104-H104</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="61"/>
+      <c r="B105" s="84"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G105" s="2">
+        <v>12</v>
+      </c>
+      <c r="H105" s="2">
+        <v>0</v>
+      </c>
+      <c r="I105" s="23">
+        <f>G105-H105</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="61"/>
+      <c r="B106" s="84"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106" s="2">
+        <v>8</v>
+      </c>
+      <c r="H106" s="2">
+        <v>0</v>
+      </c>
+      <c r="I106" s="23">
+        <f>G106-H106</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="62"/>
+      <c r="B107" s="85"/>
+      <c r="C107" s="25"/>
+      <c r="D107" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E107" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F98" s="4" t="s">
+      <c r="F107" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G98" s="4">
-        <v>4</v>
-      </c>
-      <c r="H98" s="4">
-        <v>0</v>
-      </c>
-      <c r="I98" s="23">
-        <f t="shared" ref="I98" si="26">G98-H98</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="70"/>
-      <c r="B99" s="73"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="54"/>
-      <c r="E99" s="54"/>
-      <c r="F99" s="54"/>
-      <c r="G99" s="54"/>
-      <c r="H99" s="54"/>
-      <c r="I99" s="55"/>
-    </row>
-    <row r="100" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B100" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="25"/>
-      <c r="D100" s="54"/>
-      <c r="E100" s="54"/>
-      <c r="F100" s="54"/>
-      <c r="G100" s="54"/>
-      <c r="H100" s="54"/>
-      <c r="I100" s="55"/>
+      <c r="G107" s="7">
+        <v>4</v>
+      </c>
+      <c r="H107" s="7">
+        <v>0</v>
+      </c>
+      <c r="I107" s="26">
+        <f t="shared" ref="I107" si="29">G107-H107</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="48">
+    <mergeCell ref="A86:A93"/>
+    <mergeCell ref="B86:B93"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="B95:B107"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A74:A85"/>
+    <mergeCell ref="B74:B85"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A56:A73"/>
+    <mergeCell ref="B56:B73"/>
+    <mergeCell ref="A43:A55"/>
+    <mergeCell ref="B43:B55"/>
+    <mergeCell ref="C102:D102"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A21:A42"/>
     <mergeCell ref="B21:B42"/>
@@ -4233,38 +4495,9 @@
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A86:A99"/>
-    <mergeCell ref="B86:B99"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A74:A85"/>
-    <mergeCell ref="B74:B85"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A56:A73"/>
-    <mergeCell ref="B56:B73"/>
-    <mergeCell ref="A43:A55"/>
-    <mergeCell ref="B43:B55"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F91 F93:F98">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F107">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Close Sprint7 + Update Sprint8
</commit_message>
<xml_diff>
--- a/SelfEducationPlan.xlsx
+++ b/SelfEducationPlan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="192">
   <si>
     <t>11.09.18</t>
   </si>
@@ -556,9 +556,6 @@
     <t>Update product`s amount after create order</t>
   </si>
   <si>
-    <t>TA64</t>
-  </si>
-  <si>
     <t>New function for UI for successful order. Clear state`s parameters after create order.</t>
   </si>
   <si>
@@ -574,9 +571,6 @@
     <t xml:space="preserve">Amend UI "Order is sucsessful" </t>
   </si>
   <si>
-    <t xml:space="preserve">Amend validation "items is sucsessful" </t>
-  </si>
-  <si>
     <t>Amend functionality of browse pictures to products</t>
   </si>
   <si>
@@ -602,6 +596,15 @@
   </si>
   <si>
     <t>[NN] Add enter field for product`s amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amend check on "items are sucsessful" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">set custom size for div </t>
+  </si>
+  <si>
+    <t>add virtual directory</t>
   </si>
 </sst>
 </file>
@@ -1420,119 +1423,119 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1816,11 +1819,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U107"/>
+  <dimension ref="A1:U105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J99" sqref="J99"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,12 +1841,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="40" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="66" t="s">
+      <c r="A1" s="85"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="68"/>
+      <c r="D1" s="87"/>
       <c r="E1" s="41" t="s">
         <v>17</v>
       </c>
@@ -1861,14 +1864,14 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
       <c r="E2" s="11" t="s">
         <v>163</v>
       </c>
@@ -1881,12 +1884,12 @@
       <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="64"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="89"/>
       <c r="E3" s="17" t="s">
         <v>19</v>
       </c>
@@ -1907,7 +1910,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="64"/>
       <c r="C4" s="31"/>
       <c r="D4" s="2" t="s">
@@ -1934,7 +1937,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="64"/>
       <c r="C5" s="31"/>
       <c r="D5" s="2" t="s">
@@ -1961,7 +1964,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="64"/>
       <c r="C6" s="32"/>
       <c r="D6" s="4" t="s">
@@ -1988,7 +1991,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="64"/>
       <c r="C7" s="37"/>
       <c r="D7" s="4" t="s">
@@ -2015,8 +2018,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="25"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
@@ -2039,14 +2042,14 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="61" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="93"/>
       <c r="E9" s="13" t="s">
         <v>164</v>
       </c>
@@ -2061,12 +2064,12 @@
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="64"/>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="70"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="17" t="s">
         <v>19</v>
       </c>
@@ -2087,7 +2090,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="64"/>
       <c r="C11" s="22"/>
       <c r="D11" s="2" t="s">
@@ -2111,7 +2114,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="64"/>
       <c r="C12" s="22"/>
       <c r="D12" s="2" t="s">
@@ -2135,7 +2138,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="64"/>
       <c r="C13" s="33"/>
       <c r="D13" s="4" t="s">
@@ -2159,12 +2162,12 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="64"/>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="74"/>
       <c r="E14" s="20" t="s">
         <v>50</v>
       </c>
@@ -2185,7 +2188,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="64"/>
       <c r="C15" s="22"/>
       <c r="D15" s="2" t="s">
@@ -2209,7 +2212,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="64"/>
       <c r="C16" s="22"/>
       <c r="D16" s="2" t="s">
@@ -2233,12 +2236,12 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="64"/>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="78"/>
+      <c r="D17" s="95"/>
       <c r="E17" s="18" t="s">
         <v>51</v>
       </c>
@@ -2259,7 +2262,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="64"/>
       <c r="C18" s="22"/>
       <c r="D18" s="2" t="s">
@@ -2283,7 +2286,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="64"/>
       <c r="C19" s="31"/>
       <c r="D19" s="2" t="s">
@@ -2310,7 +2313,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="61"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="64"/>
       <c r="C20" s="34"/>
       <c r="D20" s="7" t="s">
@@ -2333,14 +2336,14 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="59"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="83"/>
       <c r="E21" s="13" t="s">
         <v>165</v>
       </c>
@@ -2353,12 +2356,12 @@
       <c r="I21" s="29"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="64"/>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="82"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="18" t="s">
         <v>74</v>
       </c>
@@ -2379,7 +2382,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="64"/>
       <c r="C23" s="22"/>
       <c r="D23" s="2" t="s">
@@ -2403,7 +2406,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="64"/>
       <c r="C24" s="22"/>
       <c r="D24" s="2" t="s">
@@ -2427,7 +2430,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="64"/>
       <c r="C25" s="22"/>
       <c r="D25" s="2" t="s">
@@ -2451,7 +2454,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="64"/>
       <c r="C26" s="22"/>
       <c r="D26" s="2" t="s">
@@ -2475,12 +2478,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="64"/>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="82"/>
+      <c r="D27" s="76"/>
       <c r="E27" s="18" t="s">
         <v>85</v>
       </c>
@@ -2501,7 +2504,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="64"/>
       <c r="C28" s="22"/>
       <c r="D28" s="2" t="s">
@@ -2525,7 +2528,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="64"/>
       <c r="C29" s="22"/>
       <c r="D29" s="2" t="s">
@@ -2548,7 +2551,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="64"/>
       <c r="C30" s="22"/>
       <c r="D30" s="2" t="s">
@@ -2575,7 +2578,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="64"/>
       <c r="C31" s="22"/>
       <c r="D31" s="2" t="s">
@@ -2602,7 +2605,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="64"/>
       <c r="C32" s="31"/>
       <c r="D32" s="2" t="s">
@@ -2626,7 +2629,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="64"/>
       <c r="C33" s="31"/>
       <c r="D33" s="2" t="s">
@@ -2650,7 +2653,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="64"/>
       <c r="C34" s="31"/>
       <c r="D34" s="2" t="s">
@@ -2674,7 +2677,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="64"/>
       <c r="C35" s="32"/>
       <c r="D35" s="4" t="s">
@@ -2698,12 +2701,12 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="61"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="64"/>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="87"/>
+      <c r="D36" s="66"/>
       <c r="E36" s="20" t="s">
         <v>90</v>
       </c>
@@ -2724,7 +2727,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="64"/>
       <c r="C37" s="22"/>
       <c r="D37" s="2" t="s">
@@ -2748,7 +2751,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="64"/>
       <c r="C38" s="33"/>
       <c r="D38" s="4" t="s">
@@ -2772,12 +2775,12 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="61"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="64"/>
-      <c r="C39" s="86" t="s">
+      <c r="C39" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="87"/>
+      <c r="D39" s="66"/>
       <c r="E39" s="20" t="s">
         <v>67</v>
       </c>
@@ -2798,7 +2801,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="61"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="64"/>
       <c r="C40" s="31"/>
       <c r="D40" s="2" t="s">
@@ -2822,7 +2825,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="61"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="64"/>
       <c r="C41" s="31"/>
       <c r="D41" s="2" t="s">
@@ -2846,8 +2849,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="62"/>
-      <c r="B42" s="65"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="84"/>
       <c r="C42" s="34"/>
       <c r="D42" s="7" t="s">
         <v>88</v>
@@ -2869,14 +2872,14 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="80"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="72"/>
       <c r="E43" s="13" t="s">
         <v>166</v>
       </c>
@@ -2892,12 +2895,12 @@
       <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="61"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="86" t="s">
+      <c r="A44" s="62"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="87"/>
+      <c r="D44" s="66"/>
       <c r="E44" s="27" t="s">
         <v>97</v>
       </c>
@@ -2918,8 +2921,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="61"/>
-      <c r="B45" s="92"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="81"/>
       <c r="C45" s="31"/>
       <c r="D45" s="2" t="s">
         <v>100</v>
@@ -2942,12 +2945,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="61"/>
-      <c r="B46" s="92"/>
-      <c r="C46" s="86" t="s">
+      <c r="A46" s="62"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="87"/>
+      <c r="D46" s="66"/>
       <c r="E46" s="27" t="s">
         <v>106</v>
       </c>
@@ -2968,8 +2971,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="61"/>
-      <c r="B47" s="92"/>
+      <c r="A47" s="62"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="22"/>
       <c r="D47" s="2" t="s">
         <v>101</v>
@@ -2992,8 +2995,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="61"/>
-      <c r="B48" s="92"/>
+      <c r="A48" s="62"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="22"/>
       <c r="D48" s="2" t="s">
         <v>102</v>
@@ -3016,8 +3019,8 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="61"/>
-      <c r="B49" s="92"/>
+      <c r="A49" s="62"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="33"/>
       <c r="D49" s="2" t="s">
         <v>103</v>
@@ -3040,8 +3043,8 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="61"/>
-      <c r="B50" s="92"/>
+      <c r="A50" s="62"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="37"/>
       <c r="D50" s="2" t="s">
         <v>104</v>
@@ -3065,8 +3068,8 @@
       <c r="J50" s="43"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="61"/>
-      <c r="B51" s="92"/>
+      <c r="A51" s="62"/>
+      <c r="B51" s="81"/>
       <c r="C51" s="44"/>
       <c r="D51" s="2" t="s">
         <v>109</v>
@@ -3089,8 +3092,8 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="61"/>
-      <c r="B52" s="92"/>
+      <c r="A52" s="62"/>
+      <c r="B52" s="81"/>
       <c r="C52" s="44"/>
       <c r="D52" s="2" t="s">
         <v>110</v>
@@ -3113,10 +3116,10 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="61"/>
-      <c r="B53" s="92"/>
-      <c r="C53" s="71"/>
-      <c r="D53" s="72"/>
+      <c r="A53" s="62"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="74"/>
       <c r="E53" s="27" t="s">
         <v>114</v>
       </c>
@@ -3137,8 +3140,8 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="61"/>
-      <c r="B54" s="92"/>
+      <c r="A54" s="62"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="22"/>
       <c r="D54" s="2" t="s">
         <v>115</v>
@@ -3161,8 +3164,8 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="61"/>
-      <c r="B55" s="92"/>
+      <c r="A55" s="62"/>
+      <c r="B55" s="81"/>
       <c r="C55" s="25"/>
       <c r="D55" s="7" t="s">
         <v>116</v>
@@ -3185,14 +3188,14 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="88" t="s">
+      <c r="A56" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="79"/>
-      <c r="D56" s="80"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="72"/>
       <c r="E56" s="13" t="s">
         <v>167</v>
       </c>
@@ -3208,12 +3211,12 @@
       <c r="I56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="61"/>
-      <c r="B57" s="89"/>
-      <c r="C57" s="86" t="s">
+      <c r="A57" s="62"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="D57" s="87"/>
+      <c r="D57" s="66"/>
       <c r="E57" s="27" t="s">
         <v>97</v>
       </c>
@@ -3234,8 +3237,8 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="61"/>
-      <c r="B58" s="89"/>
+      <c r="A58" s="62"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="31"/>
       <c r="D58" s="2" t="s">
         <v>111</v>
@@ -3258,8 +3261,8 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="61"/>
-      <c r="B59" s="89"/>
+      <c r="A59" s="62"/>
+      <c r="B59" s="78"/>
       <c r="C59" s="31"/>
       <c r="D59" s="2" t="s">
         <v>113</v>
@@ -3282,8 +3285,8 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="61"/>
-      <c r="B60" s="89"/>
+      <c r="A60" s="62"/>
+      <c r="B60" s="78"/>
       <c r="C60" s="31"/>
       <c r="D60" s="2" t="s">
         <v>119</v>
@@ -3306,8 +3309,8 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="61"/>
-      <c r="B61" s="89"/>
+      <c r="A61" s="62"/>
+      <c r="B61" s="78"/>
       <c r="C61" s="31"/>
       <c r="D61" s="2" t="s">
         <v>120</v>
@@ -3330,8 +3333,8 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="61"/>
-      <c r="B62" s="89"/>
+      <c r="A62" s="62"/>
+      <c r="B62" s="78"/>
       <c r="C62" s="31"/>
       <c r="D62" s="2" t="s">
         <v>125</v>
@@ -3354,8 +3357,8 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="61"/>
-      <c r="B63" s="89"/>
+      <c r="A63" s="62"/>
+      <c r="B63" s="78"/>
       <c r="C63" s="22" t="s">
         <v>132</v>
       </c>
@@ -3380,12 +3383,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="61"/>
-      <c r="B64" s="89"/>
-      <c r="C64" s="86" t="s">
+      <c r="A64" s="62"/>
+      <c r="B64" s="78"/>
+      <c r="C64" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="87"/>
+      <c r="D64" s="66"/>
       <c r="E64" s="27" t="s">
         <v>106</v>
       </c>
@@ -3406,8 +3409,8 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="61"/>
-      <c r="B65" s="89"/>
+      <c r="A65" s="62"/>
+      <c r="B65" s="78"/>
       <c r="C65" s="22"/>
       <c r="D65" s="2" t="s">
         <v>129</v>
@@ -3430,8 +3433,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="61"/>
-      <c r="B66" s="89"/>
+      <c r="A66" s="62"/>
+      <c r="B66" s="78"/>
       <c r="C66" s="22"/>
       <c r="D66" s="2" t="s">
         <v>130</v>
@@ -3454,10 +3457,10 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="61"/>
-      <c r="B67" s="89"/>
-      <c r="C67" s="71"/>
-      <c r="D67" s="72"/>
+      <c r="A67" s="62"/>
+      <c r="B67" s="78"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="74"/>
       <c r="E67" s="27" t="s">
         <v>114</v>
       </c>
@@ -3478,8 +3481,8 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="61"/>
-      <c r="B68" s="89"/>
+      <c r="A68" s="62"/>
+      <c r="B68" s="78"/>
       <c r="C68" s="22"/>
       <c r="D68" s="2" t="s">
         <v>115</v>
@@ -3502,8 +3505,8 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="61"/>
-      <c r="B69" s="89"/>
+      <c r="A69" s="62"/>
+      <c r="B69" s="78"/>
       <c r="C69" s="31"/>
       <c r="D69" s="2" t="s">
         <v>116</v>
@@ -3525,12 +3528,12 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="61"/>
-      <c r="B70" s="89"/>
-      <c r="C70" s="71" t="s">
+      <c r="A70" s="62"/>
+      <c r="B70" s="78"/>
+      <c r="C70" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="72"/>
+      <c r="D70" s="74"/>
       <c r="E70" s="27" t="s">
         <v>136</v>
       </c>
@@ -3551,8 +3554,8 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="61"/>
-      <c r="B71" s="89"/>
+      <c r="A71" s="62"/>
+      <c r="B71" s="78"/>
       <c r="C71" s="22"/>
       <c r="D71" s="2" t="s">
         <v>134</v>
@@ -3574,8 +3577,8 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="61"/>
-      <c r="B72" s="89"/>
+      <c r="A72" s="62"/>
+      <c r="B72" s="78"/>
       <c r="C72" s="22"/>
       <c r="D72" s="9" t="s">
         <v>138</v>
@@ -3597,8 +3600,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="62"/>
-      <c r="B73" s="90"/>
+      <c r="A73" s="67"/>
+      <c r="B73" s="79"/>
       <c r="C73" s="25"/>
       <c r="D73" s="39" t="s">
         <v>140</v>
@@ -3620,14 +3623,14 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="60" t="s">
+      <c r="A74" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="83" t="s">
+      <c r="B74" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="C74" s="79"/>
-      <c r="D74" s="80"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="72"/>
       <c r="E74" s="13" t="s">
         <v>168</v>
       </c>
@@ -3643,12 +3646,12 @@
       <c r="I74" s="16"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="61"/>
-      <c r="B75" s="84"/>
-      <c r="C75" s="86" t="s">
+      <c r="A75" s="62"/>
+      <c r="B75" s="69"/>
+      <c r="C75" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="D75" s="87"/>
+      <c r="D75" s="66"/>
       <c r="E75" s="47" t="s">
         <v>97</v>
       </c>
@@ -3669,8 +3672,8 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="61"/>
-      <c r="B76" s="84"/>
+      <c r="A76" s="62"/>
+      <c r="B76" s="69"/>
       <c r="C76" s="22"/>
       <c r="D76" s="2" t="s">
         <v>143</v>
@@ -3693,8 +3696,8 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="61"/>
-      <c r="B77" s="84"/>
+      <c r="A77" s="62"/>
+      <c r="B77" s="69"/>
       <c r="C77" s="22"/>
       <c r="D77" s="2" t="s">
         <v>144</v>
@@ -3717,8 +3720,8 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="61"/>
-      <c r="B78" s="84"/>
+      <c r="A78" s="62"/>
+      <c r="B78" s="69"/>
       <c r="C78" s="31"/>
       <c r="D78" s="2" t="s">
         <v>145</v>
@@ -3741,8 +3744,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="61"/>
-      <c r="B79" s="84"/>
+      <c r="A79" s="62"/>
+      <c r="B79" s="69"/>
       <c r="C79" s="22"/>
       <c r="D79" s="2" t="s">
         <v>146</v>
@@ -3765,8 +3768,8 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="61"/>
-      <c r="B80" s="84"/>
+      <c r="A80" s="62"/>
+      <c r="B80" s="69"/>
       <c r="C80" s="22"/>
       <c r="D80" s="2" t="s">
         <v>147</v>
@@ -3789,10 +3792,10 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="61"/>
-      <c r="B81" s="84"/>
-      <c r="C81" s="71"/>
-      <c r="D81" s="72"/>
+      <c r="A81" s="62"/>
+      <c r="B81" s="69"/>
+      <c r="C81" s="73"/>
+      <c r="D81" s="74"/>
       <c r="E81" s="47" t="s">
         <v>114</v>
       </c>
@@ -3813,8 +3816,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="61"/>
-      <c r="B82" s="84"/>
+      <c r="A82" s="62"/>
+      <c r="B82" s="69"/>
       <c r="C82" s="31"/>
       <c r="D82" s="4" t="s">
         <v>115</v>
@@ -3840,8 +3843,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="61"/>
-      <c r="B83" s="84"/>
+      <c r="A83" s="62"/>
+      <c r="B83" s="69"/>
       <c r="C83" s="49"/>
       <c r="D83" s="2" t="s">
         <v>116</v>
@@ -3864,12 +3867,12 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="61"/>
-      <c r="B84" s="84"/>
-      <c r="C84" s="71" t="s">
+      <c r="A84" s="62"/>
+      <c r="B84" s="69"/>
+      <c r="C84" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="D84" s="72"/>
+      <c r="D84" s="74"/>
       <c r="E84" s="47" t="s">
         <v>150</v>
       </c>
@@ -3890,8 +3893,8 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="62"/>
-      <c r="B85" s="85"/>
+      <c r="A85" s="67"/>
+      <c r="B85" s="70"/>
       <c r="C85" s="25"/>
       <c r="D85" s="7" t="s">
         <v>149</v>
@@ -3914,33 +3917,33 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="60" t="s">
+      <c r="A86" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B86" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="79"/>
-      <c r="D86" s="80"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="72"/>
       <c r="E86" s="57" t="s">
         <v>169</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="11">
-        <f>SUM(G87,G89,G102)</f>
+        <f>SUM(G87,G89,G100)</f>
         <v>56</v>
       </c>
       <c r="H86" s="11">
-        <f>SUM(H87,H89,H102)</f>
+        <f>SUM(H87,H89,H100)</f>
         <v>27.5</v>
       </c>
       <c r="I86" s="16"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="61"/>
+      <c r="A87" s="62"/>
       <c r="B87" s="64"/>
-      <c r="C87" s="71"/>
-      <c r="D87" s="72"/>
+      <c r="C87" s="73"/>
+      <c r="D87" s="74"/>
       <c r="E87" s="50" t="s">
         <v>114</v>
       </c>
@@ -3961,7 +3964,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="61"/>
+      <c r="A88" s="62"/>
       <c r="B88" s="64"/>
       <c r="C88" s="22"/>
       <c r="D88" s="4" t="s">
@@ -3988,12 +3991,12 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="61"/>
+      <c r="A89" s="62"/>
       <c r="B89" s="64"/>
-      <c r="C89" s="71" t="s">
+      <c r="C89" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="D89" s="72"/>
+      <c r="D89" s="74"/>
       <c r="E89" s="50" t="s">
         <v>150</v>
       </c>
@@ -4014,7 +4017,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="61"/>
+      <c r="A90" s="62"/>
       <c r="B90" s="64"/>
       <c r="C90" s="22"/>
       <c r="D90" s="2" t="s">
@@ -4037,13 +4040,13 @@
         <v>1.5</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="61"/>
+      <c r="A91" s="62"/>
       <c r="B91" s="64"/>
-      <c r="C91" s="95"/>
+      <c r="C91" s="60"/>
       <c r="D91" s="2" t="s">
         <v>155</v>
       </c>
@@ -4064,11 +4067,11 @@
         <v>-3</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="61"/>
+      <c r="A92" s="62"/>
       <c r="B92" s="64"/>
       <c r="C92" s="52"/>
       <c r="D92" s="2" t="s">
@@ -4091,20 +4094,20 @@
         <v>1</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="61"/>
+      <c r="A93" s="62"/>
       <c r="B93" s="64"/>
-      <c r="C93" s="93" t="s">
+      <c r="C93" s="58" t="s">
         <v>173</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>158</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F93" s="4" t="s">
         <v>31</v>
@@ -4123,12 +4126,12 @@
     <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="55"/>
       <c r="B94" s="56"/>
-      <c r="C94" s="94"/>
+      <c r="C94" s="59"/>
       <c r="D94" s="7" t="s">
         <v>159</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>33</v>
@@ -4144,342 +4147,280 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="60" t="s">
+      <c r="A95" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B95" s="83" t="s">
+      <c r="B95" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="79"/>
-      <c r="D95" s="80"/>
+      <c r="C95" s="71"/>
+      <c r="D95" s="72"/>
       <c r="E95" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F95" s="54"/>
       <c r="G95" s="11">
-        <f>SUM(G96,G98,G110)</f>
-        <v>26</v>
+        <f>SUM(G96,G100)</f>
+        <v>52</v>
       </c>
       <c r="H95" s="11">
-        <f>SUM(H96,H98,H110)</f>
-        <v>0</v>
+        <f>SUM(H96,H100,H108)</f>
+        <v>16</v>
       </c>
       <c r="I95" s="16"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="61"/>
-      <c r="B96" s="84"/>
-      <c r="C96" s="86" t="s">
+      <c r="A96" s="62"/>
+      <c r="B96" s="69"/>
+      <c r="C96" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="D96" s="87"/>
+      <c r="D96" s="66"/>
       <c r="E96" s="53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F96" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G96" s="53">
-        <f>SUM(G97:G100)</f>
-        <v>21</v>
+        <f>SUM(G97:G99)</f>
+        <v>16</v>
       </c>
       <c r="H96" s="53">
-        <f>SUM(H97:H100)</f>
-        <v>0</v>
+        <f>SUM(H97:H99)</f>
+        <v>16</v>
       </c>
       <c r="I96" s="21">
-        <f>SUM(I97:I100)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="61"/>
-      <c r="B97" s="84"/>
+        <f>SUM(I97:I99)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="62"/>
+      <c r="B97" s="69"/>
       <c r="C97" s="22"/>
       <c r="D97" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G97" s="2">
         <v>6</v>
       </c>
       <c r="H97" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I97" s="23">
         <f>G97-H97</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="61"/>
-      <c r="B98" s="84"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="62"/>
+      <c r="B98" s="69"/>
       <c r="C98" s="22"/>
       <c r="D98" s="2" t="s">
         <v>161</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G98" s="2">
         <v>5</v>
       </c>
       <c r="H98" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I98" s="23">
-        <f t="shared" ref="I98:I100" si="27">G98-H98</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="61"/>
-      <c r="B99" s="84"/>
+        <f t="shared" ref="I98" si="27">G98-H98</f>
+        <v>0</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="62"/>
+      <c r="B99" s="69"/>
       <c r="C99" s="22"/>
       <c r="D99" s="2" t="s">
         <v>172</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G99" s="2">
         <v>5</v>
       </c>
       <c r="H99" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I99" s="23">
         <f>G99-H99</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="61"/>
-      <c r="B100" s="84"/>
-      <c r="C100" s="22"/>
-      <c r="D100" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="62"/>
+      <c r="B100" s="69"/>
+      <c r="C100" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" s="66"/>
+      <c r="E100" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="F100" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G100" s="2">
-        <v>5</v>
-      </c>
-      <c r="H100" s="2">
-        <v>0</v>
-      </c>
-      <c r="I100" s="23">
-        <f t="shared" si="27"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="61"/>
-      <c r="B101" s="84"/>
-      <c r="C101" s="22"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="23"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="61"/>
-      <c r="B102" s="84"/>
-      <c r="C102" s="86" t="s">
-        <v>162</v>
-      </c>
-      <c r="D102" s="87"/>
-      <c r="E102" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="F102" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="G102" s="53">
-        <f>SUM(G103:G107)</f>
+      <c r="G100" s="53">
+        <f>SUM(G101:G105)</f>
         <v>36</v>
       </c>
-      <c r="H102" s="53">
-        <f t="shared" ref="H102:I102" si="28">SUM(H103:H107)</f>
-        <v>0</v>
-      </c>
-      <c r="I102" s="21">
+      <c r="H100" s="53">
+        <f t="shared" ref="H100:I100" si="28">SUM(H101:H105)</f>
+        <v>0</v>
+      </c>
+      <c r="I100" s="21">
         <f t="shared" si="28"/>
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="61"/>
-      <c r="B103" s="84"/>
+    <row r="101" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="62"/>
+      <c r="B101" s="69"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G101" s="2">
+        <v>8</v>
+      </c>
+      <c r="H101" s="2">
+        <v>0</v>
+      </c>
+      <c r="I101" s="23">
+        <f>G101-H101</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="62"/>
+      <c r="B102" s="69"/>
+      <c r="C102" s="22"/>
+      <c r="D102" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" s="2">
+        <v>4</v>
+      </c>
+      <c r="H102" s="2">
+        <v>0</v>
+      </c>
+      <c r="I102" s="23">
+        <f>G102-H102</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="62"/>
+      <c r="B103" s="69"/>
       <c r="C103" s="22"/>
       <c r="D103" s="2" t="s">
         <v>185</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G103" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H103" s="2">
         <v>0</v>
       </c>
       <c r="I103" s="23">
         <f>G103-H103</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="61"/>
-      <c r="B104" s="84"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="62"/>
+      <c r="B104" s="69"/>
       <c r="C104" s="22"/>
       <c r="D104" s="2" t="s">
         <v>186</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G104" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H104" s="2">
         <v>0</v>
       </c>
       <c r="I104" s="23">
         <f>G104-H104</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="61"/>
-      <c r="B105" s="84"/>
-      <c r="C105" s="22"/>
-      <c r="D105" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="67"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E105" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F105" s="2" t="s">
+      <c r="E105" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F105" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G105" s="2">
-        <v>12</v>
-      </c>
-      <c r="H105" s="2">
-        <v>0</v>
-      </c>
-      <c r="I105" s="23">
-        <f>G105-H105</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="61"/>
-      <c r="B106" s="84"/>
-      <c r="C106" s="22"/>
-      <c r="D106" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G106" s="2">
-        <v>8</v>
-      </c>
-      <c r="H106" s="2">
-        <v>0</v>
-      </c>
-      <c r="I106" s="23">
-        <f>G106-H106</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="62"/>
-      <c r="B107" s="85"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="E107" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G107" s="7">
-        <v>4</v>
-      </c>
-      <c r="H107" s="7">
-        <v>0</v>
-      </c>
-      <c r="I107" s="26">
-        <f t="shared" ref="I107" si="29">G107-H107</f>
+      <c r="G105" s="7">
+        <v>4</v>
+      </c>
+      <c r="H105" s="7">
+        <v>0</v>
+      </c>
+      <c r="I105" s="26">
+        <f t="shared" ref="I105" si="29">G105-H105</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A86:A93"/>
-    <mergeCell ref="B86:B93"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="B95:B107"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A74:A85"/>
-    <mergeCell ref="B74:B85"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A56:A73"/>
-    <mergeCell ref="B56:B73"/>
-    <mergeCell ref="A43:A55"/>
-    <mergeCell ref="B43:B55"/>
-    <mergeCell ref="C102:D102"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A21:A42"/>
     <mergeCell ref="B21:B42"/>
@@ -4495,9 +4436,42 @@
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A74:A85"/>
+    <mergeCell ref="B74:B85"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A56:A73"/>
+    <mergeCell ref="B56:B73"/>
+    <mergeCell ref="A43:A55"/>
+    <mergeCell ref="B43:B55"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A86:A93"/>
+    <mergeCell ref="B86:B93"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A95:A105"/>
+    <mergeCell ref="B95:B105"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C100:D100"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F107">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F105">
       <formula1>Schedule_state</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>